<commit_message>
Fix missing first new_cases & new_deaths
</commit_message>
<xml_diff>
--- a/public/data/latest/owid-covid-latest.xlsx
+++ b/public/data/latest/owid-covid-latest.xlsx
@@ -1225,7 +1225,9 @@
       <c r="AG6" t="inlineStr"/>
       <c r="AH6" t="inlineStr"/>
       <c r="AI6" t="inlineStr"/>
-      <c r="AJ6" t="inlineStr"/>
+      <c r="AJ6" t="n">
+        <v>65.73999999999999</v>
+      </c>
       <c r="AK6" t="n">
         <v>32866268</v>
       </c>

</xml_diff>

<commit_message>
Hospital & ICU update
</commit_message>
<xml_diff>
--- a/public/data/latest/owid-covid-latest.xlsx
+++ b/public/data/latest/owid-covid-latest.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -54,18 +54,86 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -1760,16 +1828,16 @@
       </c>
       <c r="P11" t="inlineStr"/>
       <c r="Q11" t="n">
-        <v>475</v>
+        <v>414</v>
       </c>
       <c r="R11" t="n">
-        <v>52.74</v>
+        <v>45.967</v>
       </c>
       <c r="S11" t="n">
-        <v>2412</v>
+        <v>2043</v>
       </c>
       <c r="T11" t="n">
-        <v>267.81</v>
+        <v>226.839</v>
       </c>
       <c r="U11" t="inlineStr"/>
       <c r="V11" t="inlineStr"/>
@@ -2659,28 +2727,28 @@
       </c>
       <c r="P18" t="inlineStr"/>
       <c r="Q18" t="n">
-        <v>543</v>
+        <v>492</v>
       </c>
       <c r="R18" t="n">
-        <v>46.852</v>
+        <v>42.452</v>
       </c>
       <c r="S18" t="n">
-        <v>2538</v>
+        <v>2361</v>
       </c>
       <c r="T18" t="n">
-        <v>218.989</v>
+        <v>203.717</v>
       </c>
       <c r="U18" t="n">
-        <v>4019.507</v>
+        <v>3647.2</v>
       </c>
       <c r="V18" t="n">
-        <v>346.82</v>
+        <v>314.695</v>
       </c>
       <c r="W18" t="n">
-        <v>1270.703</v>
+        <v>1135.134</v>
       </c>
       <c r="X18" t="n">
-        <v>109.641</v>
+        <v>97.944</v>
       </c>
       <c r="Y18" t="n">
         <v>28360</v>
@@ -3767,18 +3835,10 @@
         <v>11.04</v>
       </c>
       <c r="P27" t="inlineStr"/>
-      <c r="Q27" t="n">
-        <v>536</v>
-      </c>
-      <c r="R27" t="n">
-        <v>77.14</v>
-      </c>
-      <c r="S27" t="n">
-        <v>6624</v>
-      </c>
-      <c r="T27" t="n">
-        <v>953.307</v>
-      </c>
+      <c r="Q27" t="inlineStr"/>
+      <c r="R27" t="inlineStr"/>
+      <c r="S27" t="inlineStr"/>
+      <c r="T27" t="inlineStr"/>
       <c r="U27" t="inlineStr"/>
       <c r="V27" t="inlineStr"/>
       <c r="W27" t="inlineStr"/>
@@ -4381,16 +4441,16 @@
       </c>
       <c r="P32" t="inlineStr"/>
       <c r="Q32" t="n">
-        <v>710</v>
+        <v>774</v>
       </c>
       <c r="R32" t="n">
-        <v>18.812</v>
+        <v>20.508</v>
       </c>
       <c r="S32" t="n">
-        <v>3725</v>
+        <v>4180</v>
       </c>
       <c r="T32" t="n">
-        <v>98.696</v>
+        <v>110.751</v>
       </c>
       <c r="U32" t="inlineStr"/>
       <c r="V32" t="inlineStr"/>
@@ -5792,18 +5852,18 @@
       <c r="Q43" t="inlineStr"/>
       <c r="R43" t="inlineStr"/>
       <c r="S43" t="n">
-        <v>2976</v>
+        <v>2664</v>
       </c>
       <c r="T43" t="n">
-        <v>724.922</v>
+        <v>648.922</v>
       </c>
       <c r="U43" t="inlineStr"/>
       <c r="V43" t="inlineStr"/>
       <c r="W43" t="n">
-        <v>2182.429</v>
+        <v>1496.58</v>
       </c>
       <c r="X43" t="n">
-        <v>531.617</v>
+        <v>364.551</v>
       </c>
       <c r="Y43" t="n">
         <v>7411</v>
@@ -6082,16 +6142,16 @@
       <c r="S45" t="inlineStr"/>
       <c r="T45" t="inlineStr"/>
       <c r="U45" t="n">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="V45" t="n">
-        <v>3.425</v>
+        <v>15.984</v>
       </c>
       <c r="W45" t="n">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="X45" t="n">
-        <v>94.76000000000001</v>
+        <v>81.06</v>
       </c>
       <c r="Y45" t="n">
         <v>18070</v>
@@ -6223,28 +6283,28 @@
       </c>
       <c r="P46" t="inlineStr"/>
       <c r="Q46" t="n">
-        <v>612</v>
+        <v>741</v>
       </c>
       <c r="R46" t="n">
-        <v>57.148</v>
+        <v>69.194</v>
       </c>
       <c r="S46" t="n">
-        <v>4594</v>
+        <v>4973</v>
       </c>
       <c r="T46" t="n">
-        <v>428.986</v>
+        <v>464.377</v>
       </c>
       <c r="U46" t="n">
-        <v>1257.952</v>
+        <v>1382.641</v>
       </c>
       <c r="V46" t="n">
-        <v>117.467</v>
+        <v>129.11</v>
       </c>
       <c r="W46" t="n">
-        <v>7628.156</v>
+        <v>8195.290000000001</v>
       </c>
       <c r="X46" t="n">
-        <v>712.314</v>
+        <v>765.273</v>
       </c>
       <c r="Y46" t="n">
         <v>33642</v>
@@ -6507,21 +6567,25 @@
       </c>
       <c r="P48" t="inlineStr"/>
       <c r="Q48" t="n">
-        <v>87</v>
+        <v>102</v>
       </c>
       <c r="R48" t="n">
-        <v>15.02</v>
+        <v>17.61</v>
       </c>
       <c r="S48" t="n">
-        <v>661</v>
+        <v>817</v>
       </c>
       <c r="T48" t="n">
-        <v>114.119</v>
+        <v>141.052</v>
       </c>
       <c r="U48" t="inlineStr"/>
       <c r="V48" t="inlineStr"/>
-      <c r="W48" t="inlineStr"/>
-      <c r="X48" t="inlineStr"/>
+      <c r="W48" t="n">
+        <v>1049.485</v>
+      </c>
+      <c r="X48" t="n">
+        <v>181.189</v>
+      </c>
       <c r="Y48" t="n">
         <v>38383</v>
       </c>
@@ -7636,28 +7700,28 @@
       </c>
       <c r="P57" t="inlineStr"/>
       <c r="Q57" t="n">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="R57" t="n">
-        <v>23.369</v>
+        <v>30.154</v>
       </c>
       <c r="S57" t="n">
-        <v>381</v>
+        <v>435</v>
       </c>
       <c r="T57" t="n">
-        <v>287.214</v>
+        <v>327.921</v>
       </c>
       <c r="U57" t="n">
-        <v>20.026</v>
+        <v>29.038</v>
       </c>
       <c r="V57" t="n">
-        <v>15.096</v>
+        <v>21.89</v>
       </c>
       <c r="W57" t="n">
-        <v>243.315</v>
+        <v>274.356</v>
       </c>
       <c r="X57" t="n">
-        <v>183.421</v>
+        <v>206.821</v>
       </c>
       <c r="Y57" t="n">
         <v>6648</v>
@@ -8335,28 +8399,28 @@
       </c>
       <c r="P62" t="inlineStr"/>
       <c r="Q62" t="n">
-        <v>2745</v>
+        <v>2650</v>
       </c>
       <c r="R62" t="n">
-        <v>42.054</v>
+        <v>40.598</v>
       </c>
       <c r="S62" t="n">
-        <v>24961</v>
+        <v>24620</v>
       </c>
       <c r="T62" t="n">
-        <v>382.406</v>
+        <v>377.182</v>
       </c>
       <c r="U62" t="n">
-        <v>1125.995</v>
+        <v>1088.981</v>
       </c>
       <c r="V62" t="n">
-        <v>17.25</v>
+        <v>16.683</v>
       </c>
       <c r="W62" t="n">
-        <v>8446.912</v>
+        <v>7514.751</v>
       </c>
       <c r="X62" t="n">
-        <v>129.408</v>
+        <v>115.127</v>
       </c>
       <c r="Y62" t="n">
         <v>213156</v>
@@ -8837,10 +8901,10 @@
       </c>
       <c r="P66" t="inlineStr"/>
       <c r="Q66" t="n">
-        <v>5029</v>
+        <v>5546</v>
       </c>
       <c r="R66" t="n">
-        <v>60.023</v>
+        <v>66.194</v>
       </c>
       <c r="S66" t="inlineStr"/>
       <c r="T66" t="inlineStr"/>
@@ -9127,10 +9191,10 @@
       <c r="S68" t="inlineStr"/>
       <c r="T68" t="inlineStr"/>
       <c r="U68" t="n">
-        <v>190.489</v>
+        <v>168.136</v>
       </c>
       <c r="V68" t="n">
-        <v>18.276</v>
+        <v>16.131</v>
       </c>
       <c r="W68" t="inlineStr"/>
       <c r="X68" t="inlineStr"/>
@@ -10093,10 +10157,10 @@
       <c r="Q76" t="inlineStr"/>
       <c r="R76" t="inlineStr"/>
       <c r="S76" t="n">
-        <v>7022</v>
+        <v>6072</v>
       </c>
       <c r="T76" t="n">
-        <v>726.889</v>
+        <v>628.549</v>
       </c>
       <c r="U76" t="inlineStr"/>
       <c r="V76" t="inlineStr"/>
@@ -10238,16 +10302,16 @@
       </c>
       <c r="P77" t="inlineStr"/>
       <c r="Q77" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R77" t="n">
-        <v>8.791</v>
+        <v>2.93</v>
       </c>
       <c r="S77" t="n">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="T77" t="n">
-        <v>84.982</v>
+        <v>73.26000000000001</v>
       </c>
       <c r="U77" t="inlineStr"/>
       <c r="V77" t="inlineStr"/>
@@ -11012,28 +11076,28 @@
       </c>
       <c r="P83" t="inlineStr"/>
       <c r="Q83" t="n">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="R83" t="n">
-        <v>5.873</v>
+        <v>5.468</v>
       </c>
       <c r="S83" t="n">
-        <v>220</v>
+        <v>321</v>
       </c>
       <c r="T83" t="n">
-        <v>44.554</v>
+        <v>65.009</v>
       </c>
       <c r="U83" t="n">
-        <v>18.123</v>
+        <v>16.109</v>
       </c>
       <c r="V83" t="n">
-        <v>3.67</v>
+        <v>3.262</v>
       </c>
       <c r="W83" t="n">
-        <v>83.568</v>
+        <v>121.828</v>
       </c>
       <c r="X83" t="n">
-        <v>16.924</v>
+        <v>24.673</v>
       </c>
       <c r="Y83" t="n">
         <v>13802</v>
@@ -11310,24 +11374,24 @@
       </c>
       <c r="P85" t="inlineStr"/>
       <c r="Q85" t="n">
-        <v>2743</v>
+        <v>2580</v>
       </c>
       <c r="R85" t="n">
-        <v>45.367</v>
+        <v>42.672</v>
       </c>
       <c r="S85" t="n">
-        <v>27901</v>
+        <v>26151</v>
       </c>
       <c r="T85" t="n">
-        <v>461.465</v>
+        <v>432.521</v>
       </c>
       <c r="U85" t="inlineStr"/>
       <c r="V85" t="inlineStr"/>
       <c r="W85" t="n">
-        <v>4230.156</v>
+        <v>3630.141</v>
       </c>
       <c r="X85" t="n">
-        <v>69.964</v>
+        <v>60.04</v>
       </c>
       <c r="Y85" t="n">
         <v>128740</v>
@@ -12622,10 +12686,10 @@
       <c r="Q95" t="inlineStr"/>
       <c r="R95" t="inlineStr"/>
       <c r="S95" t="n">
-        <v>903</v>
+        <v>1010</v>
       </c>
       <c r="T95" t="n">
-        <v>478.74</v>
+        <v>535.468</v>
       </c>
       <c r="U95" t="n">
         <v>90.38200000000001</v>
@@ -12634,10 +12698,10 @@
         <v>47.917</v>
       </c>
       <c r="W95" t="n">
-        <v>739.7569999999999</v>
+        <v>1487.374</v>
       </c>
       <c r="X95" t="n">
-        <v>392.194</v>
+        <v>788.5549999999999</v>
       </c>
       <c r="Y95" t="n">
         <v>11207</v>
@@ -13354,22 +13418,22 @@
       <c r="Q101" t="inlineStr"/>
       <c r="R101" t="inlineStr"/>
       <c r="S101" t="n">
-        <v>2478</v>
+        <v>2510</v>
       </c>
       <c r="T101" t="n">
-        <v>910.263</v>
+        <v>922.018</v>
       </c>
       <c r="U101" t="n">
-        <v>108.144</v>
+        <v>120.81</v>
       </c>
       <c r="V101" t="n">
-        <v>39.725</v>
+        <v>44.378</v>
       </c>
       <c r="W101" t="n">
-        <v>699.526</v>
+        <v>597.228</v>
       </c>
       <c r="X101" t="n">
-        <v>256.962</v>
+        <v>219.384</v>
       </c>
       <c r="Y101" t="n">
         <v>10344</v>
@@ -13507,16 +13571,16 @@
       </c>
       <c r="P102" t="inlineStr"/>
       <c r="Q102" t="n">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="R102" t="n">
-        <v>60.705</v>
+        <v>51.12</v>
       </c>
       <c r="S102" t="n">
-        <v>207</v>
+        <v>150</v>
       </c>
       <c r="T102" t="n">
-        <v>330.684</v>
+        <v>239.626</v>
       </c>
       <c r="U102" t="inlineStr"/>
       <c r="V102" t="inlineStr"/>
@@ -14325,10 +14389,10 @@
       <c r="U108" t="inlineStr"/>
       <c r="V108" t="inlineStr"/>
       <c r="W108" t="n">
-        <v>22.365</v>
+        <v>21.47</v>
       </c>
       <c r="X108" t="n">
-        <v>50.653</v>
+        <v>48.626</v>
       </c>
       <c r="Y108" t="inlineStr"/>
       <c r="Z108" t="inlineStr"/>
@@ -16079,28 +16143,28 @@
       </c>
       <c r="P122" t="inlineStr"/>
       <c r="Q122" t="n">
-        <v>580</v>
+        <v>631</v>
       </c>
       <c r="R122" t="n">
-        <v>33.849</v>
+        <v>36.825</v>
       </c>
       <c r="S122" t="n">
-        <v>1533</v>
+        <v>1797</v>
       </c>
       <c r="T122" t="n">
-        <v>89.467</v>
+        <v>104.874</v>
       </c>
       <c r="U122" t="n">
-        <v>277.614</v>
+        <v>276.622</v>
       </c>
       <c r="V122" t="n">
-        <v>16.202</v>
+        <v>16.144</v>
       </c>
       <c r="W122" t="n">
-        <v>1516.96</v>
+        <v>1779.702</v>
       </c>
       <c r="X122" t="n">
-        <v>88.53100000000001</v>
+        <v>103.864</v>
       </c>
       <c r="Y122" t="inlineStr"/>
       <c r="Z122" t="n">
@@ -16869,22 +16933,22 @@
       <c r="Q128" t="inlineStr"/>
       <c r="R128" t="inlineStr"/>
       <c r="S128" t="n">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="T128" t="n">
-        <v>25.455</v>
+        <v>23.795</v>
       </c>
       <c r="U128" t="n">
-        <v>16.279</v>
+        <v>17.297</v>
       </c>
       <c r="V128" t="n">
-        <v>3.003</v>
+        <v>3.191</v>
       </c>
       <c r="W128" t="n">
-        <v>92.589</v>
+        <v>81.39700000000001</v>
       </c>
       <c r="X128" t="n">
-        <v>17.079</v>
+        <v>15.014</v>
       </c>
       <c r="Y128" t="n">
         <v>8962</v>
@@ -18080,10 +18144,10 @@
       <c r="Q137" t="inlineStr"/>
       <c r="R137" t="inlineStr"/>
       <c r="S137" t="n">
-        <v>18180</v>
+        <v>16686</v>
       </c>
       <c r="T137" t="n">
-        <v>480.36</v>
+        <v>440.885</v>
       </c>
       <c r="U137" t="inlineStr"/>
       <c r="V137" t="inlineStr"/>
@@ -18223,24 +18287,24 @@
       </c>
       <c r="P138" t="inlineStr"/>
       <c r="Q138" t="n">
-        <v>483</v>
+        <v>504</v>
       </c>
       <c r="R138" t="n">
-        <v>47.368</v>
+        <v>49.428</v>
       </c>
       <c r="S138" t="n">
-        <v>3027</v>
+        <v>2870</v>
       </c>
       <c r="T138" t="n">
-        <v>296.861</v>
+        <v>281.463</v>
       </c>
       <c r="U138" t="inlineStr"/>
       <c r="V138" t="inlineStr"/>
       <c r="W138" t="n">
-        <v>302.628</v>
+        <v>263.932</v>
       </c>
       <c r="X138" t="n">
-        <v>29.679</v>
+        <v>25.884</v>
       </c>
       <c r="Y138" t="n">
         <v>37990</v>
@@ -18515,20 +18579,20 @@
       </c>
       <c r="P140" t="inlineStr"/>
       <c r="Q140" t="n">
-        <v>1267</v>
+        <v>1210</v>
       </c>
       <c r="R140" t="n">
-        <v>65.86</v>
+        <v>62.897</v>
       </c>
       <c r="S140" t="inlineStr"/>
       <c r="T140" t="inlineStr"/>
       <c r="U140" t="inlineStr"/>
       <c r="V140" t="inlineStr"/>
       <c r="W140" t="n">
-        <v>7143.359</v>
+        <v>6618.185</v>
       </c>
       <c r="X140" t="n">
-        <v>371.321</v>
+        <v>344.022</v>
       </c>
       <c r="Y140" t="n">
         <v>25840</v>
@@ -20356,10 +20420,10 @@
       <c r="Q155" t="inlineStr"/>
       <c r="R155" t="inlineStr"/>
       <c r="S155" t="n">
-        <v>2210</v>
+        <v>2426</v>
       </c>
       <c r="T155" t="n">
-        <v>404.788</v>
+        <v>444.351</v>
       </c>
       <c r="U155" t="inlineStr"/>
       <c r="V155" t="inlineStr"/>
@@ -20497,28 +20561,28 @@
       </c>
       <c r="P156" t="inlineStr"/>
       <c r="Q156" t="n">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="R156" t="n">
-        <v>97.16500000000001</v>
+        <v>99.089</v>
       </c>
       <c r="S156" t="n">
-        <v>1214</v>
+        <v>1179</v>
       </c>
       <c r="T156" t="n">
-        <v>583.954</v>
+        <v>567.1180000000001</v>
       </c>
       <c r="U156" t="n">
-        <v>115.89</v>
+        <v>113.892</v>
       </c>
       <c r="V156" t="n">
-        <v>55.745</v>
+        <v>54.784</v>
       </c>
       <c r="W156" t="n">
-        <v>727.309</v>
+        <v>688.346</v>
       </c>
       <c r="X156" t="n">
-        <v>349.847</v>
+        <v>331.105</v>
       </c>
       <c r="Y156" t="n">
         <v>10750</v>
@@ -21279,28 +21343,28 @@
       </c>
       <c r="P162" t="inlineStr"/>
       <c r="Q162" t="n">
-        <v>1955</v>
+        <v>1907</v>
       </c>
       <c r="R162" t="n">
-        <v>41.814</v>
+        <v>40.787</v>
       </c>
       <c r="S162" t="n">
-        <v>11336</v>
+        <v>10744</v>
       </c>
       <c r="T162" t="n">
-        <v>242.456</v>
+        <v>229.795</v>
       </c>
       <c r="U162" t="n">
-        <v>49.806</v>
+        <v>39.845</v>
       </c>
       <c r="V162" t="n">
-        <v>1.065</v>
+        <v>0.852</v>
       </c>
       <c r="W162" t="n">
-        <v>1162.468</v>
+        <v>990.14</v>
       </c>
       <c r="X162" t="n">
-        <v>24.863</v>
+        <v>21.177</v>
       </c>
       <c r="Y162" t="inlineStr"/>
       <c r="Z162" t="n">
@@ -21799,18 +21863,18 @@
       </c>
       <c r="P166" t="inlineStr"/>
       <c r="Q166" t="n">
-        <v>288</v>
+        <v>323</v>
       </c>
       <c r="R166" t="n">
-        <v>28.517</v>
+        <v>31.983</v>
       </c>
       <c r="S166" t="inlineStr"/>
       <c r="T166" t="inlineStr"/>
       <c r="U166" t="n">
-        <v>165.85</v>
+        <v>175.722</v>
       </c>
       <c r="V166" t="n">
-        <v>16.422</v>
+        <v>17.399</v>
       </c>
       <c r="W166" t="inlineStr"/>
       <c r="X166" t="inlineStr"/>
@@ -23748,24 +23812,24 @@
       </c>
       <c r="P181" t="inlineStr"/>
       <c r="Q181" t="n">
-        <v>1364</v>
+        <v>1751</v>
       </c>
       <c r="R181" t="n">
-        <v>20.093</v>
+        <v>25.793</v>
       </c>
       <c r="S181" t="n">
-        <v>18943</v>
+        <v>22520</v>
       </c>
       <c r="T181" t="n">
-        <v>279.041</v>
+        <v>331.733</v>
       </c>
       <c r="U181" t="inlineStr"/>
       <c r="V181" t="inlineStr"/>
       <c r="W181" t="n">
-        <v>10064.676</v>
+        <v>13757.061</v>
       </c>
       <c r="X181" t="n">
-        <v>148.258</v>
+        <v>202.649</v>
       </c>
       <c r="Y181" t="n">
         <v>357238</v>
@@ -23903,28 +23967,28 @@
       </c>
       <c r="P182" t="inlineStr"/>
       <c r="Q182" t="n">
-        <v>22489</v>
+        <v>23069</v>
       </c>
       <c r="R182" t="n">
-        <v>67.94199999999999</v>
+        <v>69.694</v>
       </c>
       <c r="S182" t="n">
-        <v>119463</v>
+        <v>125220</v>
       </c>
       <c r="T182" t="n">
-        <v>360.913</v>
+        <v>378.305</v>
       </c>
       <c r="U182" t="n">
-        <v>1536</v>
+        <v>1134</v>
       </c>
       <c r="V182" t="n">
-        <v>4.64</v>
+        <v>3.426</v>
       </c>
       <c r="W182" t="n">
-        <v>28859</v>
+        <v>23403</v>
       </c>
       <c r="X182" t="n">
-        <v>87.187</v>
+        <v>70.703</v>
       </c>
       <c r="Y182" t="n">
         <v>243910</v>
@@ -25221,6 +25285,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Interim hospital & ICU update for US & Canada
</commit_message>
<xml_diff>
--- a/public/data/latest/owid-covid-latest.xlsx
+++ b/public/data/latest/owid-covid-latest.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="446">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="446">
   <si>
     <t>iso_code</t>
   </si>
@@ -3087,22 +3087,22 @@
         <v>0.08400000000000001</v>
       </c>
       <c r="Y14">
-        <v>12273</v>
+        <v>11085</v>
       </c>
       <c r="Z14">
-        <v>2405722</v>
+        <v>2416807</v>
       </c>
       <c r="AA14">
-        <v>1413.814</v>
+        <v>1420.329</v>
       </c>
       <c r="AB14">
-        <v>7.213</v>
+        <v>6.515</v>
       </c>
       <c r="AC14">
-        <v>10036</v>
+        <v>10212</v>
       </c>
       <c r="AD14">
-        <v>5.898</v>
+        <v>6.001</v>
       </c>
       <c r="AE14">
         <v>0.026</v>
@@ -4424,22 +4424,22 @@
         <v>10.218</v>
       </c>
       <c r="Y27">
-        <v>10762</v>
+        <v>11436</v>
       </c>
       <c r="Z27">
-        <v>1173704</v>
+        <v>1185140</v>
       </c>
       <c r="AA27">
-        <v>168.916</v>
+        <v>170.562</v>
       </c>
       <c r="AB27">
-        <v>1.549</v>
+        <v>1.646</v>
       </c>
       <c r="AC27">
-        <v>5815</v>
+        <v>6295</v>
       </c>
       <c r="AD27">
-        <v>0.837</v>
+        <v>0.906</v>
       </c>
       <c r="AE27">
         <v>0.145</v>
@@ -4908,16 +4908,16 @@
         <v>3.278</v>
       </c>
       <c r="Q32">
-        <v>774</v>
+        <v>850</v>
       </c>
       <c r="R32">
-        <v>20.508</v>
+        <v>22.521</v>
       </c>
       <c r="S32">
-        <v>4180</v>
+        <v>4651</v>
       </c>
       <c r="T32">
-        <v>110.751</v>
+        <v>123.231</v>
       </c>
       <c r="Y32">
         <v>59157</v>
@@ -6088,22 +6088,22 @@
         <v>364.551</v>
       </c>
       <c r="Y43">
-        <v>6602</v>
+        <v>9919</v>
       </c>
       <c r="Z43">
-        <v>1041678</v>
+        <v>1051597</v>
       </c>
       <c r="AA43">
-        <v>253.742</v>
+        <v>256.158</v>
       </c>
       <c r="AB43">
-        <v>1.608</v>
+        <v>2.416</v>
       </c>
       <c r="AC43">
-        <v>5333</v>
+        <v>5847</v>
       </c>
       <c r="AD43">
-        <v>1.299</v>
+        <v>1.424</v>
       </c>
       <c r="AE43">
         <v>0.209</v>
@@ -7339,27 +7339,6 @@
       <c r="O54">
         <v>1.321</v>
       </c>
-      <c r="Z54">
-        <v>609398</v>
-      </c>
-      <c r="AA54">
-        <v>93.953</v>
-      </c>
-      <c r="AC54">
-        <v>2484</v>
-      </c>
-      <c r="AD54">
-        <v>0.383</v>
-      </c>
-      <c r="AE54">
-        <v>0.079</v>
-      </c>
-      <c r="AF54">
-        <v>12.6</v>
-      </c>
-      <c r="AG54" t="s">
-        <v>443</v>
-      </c>
       <c r="AL54">
         <v>47.22</v>
       </c>
@@ -8907,22 +8886,22 @@
         <v>16.131</v>
       </c>
       <c r="Y68">
-        <v>11817</v>
+        <v>13881</v>
       </c>
       <c r="Z68">
-        <v>2840278</v>
+        <v>2854159</v>
       </c>
       <c r="AA68">
-        <v>272.5</v>
+        <v>273.831</v>
       </c>
       <c r="AB68">
-        <v>1.134</v>
+        <v>1.332</v>
       </c>
       <c r="AC68">
-        <v>9322</v>
+        <v>9244</v>
       </c>
       <c r="AD68">
-        <v>0.894</v>
+        <v>0.887</v>
       </c>
       <c r="AE68">
         <v>0.06900000000000001</v>
@@ -9988,22 +9967,22 @@
         <v>0.173</v>
       </c>
       <c r="Y79">
-        <v>896236</v>
+        <v>931408</v>
       </c>
       <c r="Z79">
-        <v>176531997</v>
+        <v>177463405</v>
       </c>
       <c r="AA79">
-        <v>127.921</v>
+        <v>128.596</v>
       </c>
       <c r="AB79">
-        <v>0.649</v>
+        <v>0.675</v>
       </c>
       <c r="AC79">
-        <v>961464</v>
+        <v>934482</v>
       </c>
       <c r="AD79">
-        <v>0.697</v>
+        <v>0.677</v>
       </c>
       <c r="AE79">
         <v>0.019</v>
@@ -10107,22 +10086,22 @@
         <v>0.734</v>
       </c>
       <c r="Y80">
-        <v>38309</v>
+        <v>44734</v>
       </c>
       <c r="Z80">
-        <v>5061283</v>
+        <v>5106017</v>
       </c>
       <c r="AA80">
-        <v>18.504</v>
+        <v>18.668</v>
       </c>
       <c r="AB80">
-        <v>0.14</v>
+        <v>0.164</v>
       </c>
       <c r="AC80">
-        <v>39000</v>
+        <v>32934</v>
       </c>
       <c r="AD80">
-        <v>0.143</v>
+        <v>0.12</v>
       </c>
       <c r="AE80">
         <v>0.192</v>
@@ -10252,22 +10231,22 @@
         <v>1.364</v>
       </c>
       <c r="Y82">
-        <v>49601</v>
+        <v>54217</v>
       </c>
       <c r="Z82">
-        <v>7885416</v>
+        <v>7939633</v>
       </c>
       <c r="AA82">
-        <v>93.88200000000001</v>
+        <v>94.527</v>
       </c>
       <c r="AB82">
-        <v>0.591</v>
+        <v>0.645</v>
       </c>
       <c r="AC82">
-        <v>53126</v>
+        <v>53241</v>
       </c>
       <c r="AD82">
-        <v>0.633</v>
+        <v>0.634</v>
       </c>
       <c r="AE82">
         <v>0.116</v>
@@ -10918,17 +10897,11 @@
       <c r="O87">
         <v>0.338</v>
       </c>
-      <c r="Y87">
-        <v>1113</v>
-      </c>
       <c r="Z87">
         <v>141170</v>
       </c>
       <c r="AA87">
         <v>47.674</v>
-      </c>
-      <c r="AB87">
-        <v>0.376</v>
       </c>
       <c r="AC87">
         <v>532</v>
@@ -12806,16 +12779,16 @@
         <v>0.082</v>
       </c>
       <c r="Z105">
-        <v>87749</v>
+        <v>88638</v>
       </c>
       <c r="AA105">
-        <v>4.587</v>
+        <v>4.633</v>
       </c>
       <c r="AC105">
-        <v>568</v>
+        <v>612</v>
       </c>
       <c r="AD105">
-        <v>0.03</v>
+        <v>0.032</v>
       </c>
       <c r="AE105">
         <v>0.182</v>
@@ -15597,22 +15570,22 @@
         <v>0.268</v>
       </c>
       <c r="Y131">
-        <v>35073</v>
+        <v>38917</v>
       </c>
       <c r="Z131">
-        <v>6884940</v>
+        <v>6923857</v>
       </c>
       <c r="AA131">
-        <v>31.169</v>
+        <v>31.345</v>
       </c>
       <c r="AB131">
-        <v>0.159</v>
+        <v>0.176</v>
       </c>
       <c r="AC131">
-        <v>37851</v>
+        <v>38212</v>
       </c>
       <c r="AD131">
-        <v>0.171</v>
+        <v>0.173</v>
       </c>
       <c r="AE131">
         <v>0.058</v>
@@ -16793,22 +16766,22 @@
         <v>344.022</v>
       </c>
       <c r="Y141">
-        <v>31022</v>
+        <v>34343</v>
       </c>
       <c r="Z141">
-        <v>4868383</v>
+        <v>4902726</v>
       </c>
       <c r="AA141">
-        <v>253.065</v>
+        <v>254.85</v>
       </c>
       <c r="AB141">
-        <v>1.613</v>
+        <v>1.785</v>
       </c>
       <c r="AC141">
-        <v>16761</v>
+        <v>18115</v>
       </c>
       <c r="AD141">
-        <v>0.871</v>
+        <v>0.9419999999999999</v>
       </c>
       <c r="AE141">
         <v>0.215</v>
@@ -17055,22 +17028,22 @@
         <v>0.342</v>
       </c>
       <c r="Y143">
-        <v>3409</v>
+        <v>4216</v>
       </c>
       <c r="Z143">
-        <v>741036</v>
+        <v>745252</v>
       </c>
       <c r="AA143">
-        <v>57.213</v>
+        <v>57.539</v>
       </c>
       <c r="AB143">
-        <v>0.263</v>
+        <v>0.326</v>
       </c>
       <c r="AC143">
-        <v>3079</v>
+        <v>3265</v>
       </c>
       <c r="AD143">
-        <v>0.238</v>
+        <v>0.252</v>
       </c>
       <c r="AE143">
         <v>0.038</v>
@@ -18795,22 +18768,22 @@
         <v>0.412</v>
       </c>
       <c r="Y161">
-        <v>59734</v>
+        <v>67176</v>
       </c>
       <c r="Z161">
-        <v>4245610</v>
+        <v>4312786</v>
       </c>
       <c r="AA161">
-        <v>82.81</v>
+        <v>84.12</v>
       </c>
       <c r="AB161">
-        <v>1.165</v>
+        <v>1.31</v>
       </c>
       <c r="AC161">
-        <v>45484</v>
+        <v>46434</v>
       </c>
       <c r="AD161">
-        <v>0.887</v>
+        <v>0.906</v>
       </c>
       <c r="AE161">
         <v>0.019</v>
@@ -20822,22 +20795,22 @@
         <v>3.685</v>
       </c>
       <c r="Y180">
-        <v>74436</v>
+        <v>34938</v>
       </c>
       <c r="Z180">
-        <v>5645178</v>
+        <v>5680116</v>
       </c>
       <c r="AA180">
-        <v>129.081</v>
+        <v>129.879</v>
       </c>
       <c r="AB180">
-        <v>1.702</v>
+        <v>0.799</v>
       </c>
       <c r="AC180">
-        <v>19143</v>
+        <v>13500</v>
       </c>
       <c r="AD180">
-        <v>0.438</v>
+        <v>0.309</v>
       </c>
       <c r="AE180">
         <v>0.364</v>
@@ -21212,28 +21185,28 @@
         <v>8.066000000000001</v>
       </c>
       <c r="Q183">
-        <v>23069</v>
+        <v>23707</v>
       </c>
       <c r="R183">
-        <v>69.694</v>
+        <v>71.622</v>
       </c>
       <c r="S183">
-        <v>125220</v>
+        <v>132476</v>
       </c>
       <c r="T183">
-        <v>378.305</v>
+        <v>400.226</v>
       </c>
       <c r="U183">
-        <v>1134</v>
+        <v>1269</v>
       </c>
       <c r="V183">
-        <v>3.426</v>
+        <v>3.834</v>
       </c>
       <c r="W183">
-        <v>23403</v>
+        <v>28673</v>
       </c>
       <c r="X183">
-        <v>70.703</v>
+        <v>86.625</v>
       </c>
       <c r="Y183">
         <v>871502</v>

</xml_diff>

<commit_message>
Revert "Interim hospital & ICU update for US & Canada"
This reverts commit a9a2c27e4a9ce8b284a330692358f7baeca10c69.
</commit_message>
<xml_diff>
--- a/public/data/latest/owid-covid-latest.xlsx
+++ b/public/data/latest/owid-covid-latest.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="446">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="446">
   <si>
     <t>iso_code</t>
   </si>
@@ -3087,22 +3087,22 @@
         <v>0.08400000000000001</v>
       </c>
       <c r="Y14">
-        <v>11085</v>
+        <v>12273</v>
       </c>
       <c r="Z14">
-        <v>2416807</v>
+        <v>2405722</v>
       </c>
       <c r="AA14">
-        <v>1420.329</v>
+        <v>1413.814</v>
       </c>
       <c r="AB14">
-        <v>6.515</v>
+        <v>7.213</v>
       </c>
       <c r="AC14">
-        <v>10212</v>
+        <v>10036</v>
       </c>
       <c r="AD14">
-        <v>6.001</v>
+        <v>5.898</v>
       </c>
       <c r="AE14">
         <v>0.026</v>
@@ -4424,22 +4424,22 @@
         <v>10.218</v>
       </c>
       <c r="Y27">
-        <v>11436</v>
+        <v>10762</v>
       </c>
       <c r="Z27">
-        <v>1185140</v>
+        <v>1173704</v>
       </c>
       <c r="AA27">
-        <v>170.562</v>
+        <v>168.916</v>
       </c>
       <c r="AB27">
-        <v>1.646</v>
+        <v>1.549</v>
       </c>
       <c r="AC27">
-        <v>6295</v>
+        <v>5815</v>
       </c>
       <c r="AD27">
-        <v>0.906</v>
+        <v>0.837</v>
       </c>
       <c r="AE27">
         <v>0.145</v>
@@ -4908,16 +4908,16 @@
         <v>3.278</v>
       </c>
       <c r="Q32">
-        <v>850</v>
+        <v>774</v>
       </c>
       <c r="R32">
-        <v>22.521</v>
+        <v>20.508</v>
       </c>
       <c r="S32">
-        <v>4651</v>
+        <v>4180</v>
       </c>
       <c r="T32">
-        <v>123.231</v>
+        <v>110.751</v>
       </c>
       <c r="Y32">
         <v>59157</v>
@@ -6088,22 +6088,22 @@
         <v>364.551</v>
       </c>
       <c r="Y43">
-        <v>9919</v>
+        <v>6602</v>
       </c>
       <c r="Z43">
-        <v>1051597</v>
+        <v>1041678</v>
       </c>
       <c r="AA43">
-        <v>256.158</v>
+        <v>253.742</v>
       </c>
       <c r="AB43">
-        <v>2.416</v>
+        <v>1.608</v>
       </c>
       <c r="AC43">
-        <v>5847</v>
+        <v>5333</v>
       </c>
       <c r="AD43">
-        <v>1.424</v>
+        <v>1.299</v>
       </c>
       <c r="AE43">
         <v>0.209</v>
@@ -7339,6 +7339,27 @@
       <c r="O54">
         <v>1.321</v>
       </c>
+      <c r="Z54">
+        <v>609398</v>
+      </c>
+      <c r="AA54">
+        <v>93.953</v>
+      </c>
+      <c r="AC54">
+        <v>2484</v>
+      </c>
+      <c r="AD54">
+        <v>0.383</v>
+      </c>
+      <c r="AE54">
+        <v>0.079</v>
+      </c>
+      <c r="AF54">
+        <v>12.6</v>
+      </c>
+      <c r="AG54" t="s">
+        <v>443</v>
+      </c>
       <c r="AL54">
         <v>47.22</v>
       </c>
@@ -8886,22 +8907,22 @@
         <v>16.131</v>
       </c>
       <c r="Y68">
-        <v>13881</v>
+        <v>11817</v>
       </c>
       <c r="Z68">
-        <v>2854159</v>
+        <v>2840278</v>
       </c>
       <c r="AA68">
-        <v>273.831</v>
+        <v>272.5</v>
       </c>
       <c r="AB68">
-        <v>1.332</v>
+        <v>1.134</v>
       </c>
       <c r="AC68">
-        <v>9244</v>
+        <v>9322</v>
       </c>
       <c r="AD68">
-        <v>0.887</v>
+        <v>0.894</v>
       </c>
       <c r="AE68">
         <v>0.06900000000000001</v>
@@ -9967,22 +9988,22 @@
         <v>0.173</v>
       </c>
       <c r="Y79">
-        <v>931408</v>
+        <v>896236</v>
       </c>
       <c r="Z79">
-        <v>177463405</v>
+        <v>176531997</v>
       </c>
       <c r="AA79">
-        <v>128.596</v>
+        <v>127.921</v>
       </c>
       <c r="AB79">
-        <v>0.675</v>
+        <v>0.649</v>
       </c>
       <c r="AC79">
-        <v>934482</v>
+        <v>961464</v>
       </c>
       <c r="AD79">
-        <v>0.677</v>
+        <v>0.697</v>
       </c>
       <c r="AE79">
         <v>0.019</v>
@@ -10086,22 +10107,22 @@
         <v>0.734</v>
       </c>
       <c r="Y80">
-        <v>44734</v>
+        <v>38309</v>
       </c>
       <c r="Z80">
-        <v>5106017</v>
+        <v>5061283</v>
       </c>
       <c r="AA80">
-        <v>18.668</v>
+        <v>18.504</v>
       </c>
       <c r="AB80">
-        <v>0.164</v>
+        <v>0.14</v>
       </c>
       <c r="AC80">
-        <v>32934</v>
+        <v>39000</v>
       </c>
       <c r="AD80">
-        <v>0.12</v>
+        <v>0.143</v>
       </c>
       <c r="AE80">
         <v>0.192</v>
@@ -10231,22 +10252,22 @@
         <v>1.364</v>
       </c>
       <c r="Y82">
-        <v>54217</v>
+        <v>49601</v>
       </c>
       <c r="Z82">
-        <v>7939633</v>
+        <v>7885416</v>
       </c>
       <c r="AA82">
-        <v>94.527</v>
+        <v>93.88200000000001</v>
       </c>
       <c r="AB82">
-        <v>0.645</v>
+        <v>0.591</v>
       </c>
       <c r="AC82">
-        <v>53241</v>
+        <v>53126</v>
       </c>
       <c r="AD82">
-        <v>0.634</v>
+        <v>0.633</v>
       </c>
       <c r="AE82">
         <v>0.116</v>
@@ -10897,11 +10918,17 @@
       <c r="O87">
         <v>0.338</v>
       </c>
+      <c r="Y87">
+        <v>1113</v>
+      </c>
       <c r="Z87">
         <v>141170</v>
       </c>
       <c r="AA87">
         <v>47.674</v>
+      </c>
+      <c r="AB87">
+        <v>0.376</v>
       </c>
       <c r="AC87">
         <v>532</v>
@@ -12779,16 +12806,16 @@
         <v>0.082</v>
       </c>
       <c r="Z105">
-        <v>88638</v>
+        <v>87749</v>
       </c>
       <c r="AA105">
-        <v>4.633</v>
+        <v>4.587</v>
       </c>
       <c r="AC105">
-        <v>612</v>
+        <v>568</v>
       </c>
       <c r="AD105">
-        <v>0.032</v>
+        <v>0.03</v>
       </c>
       <c r="AE105">
         <v>0.182</v>
@@ -15570,22 +15597,22 @@
         <v>0.268</v>
       </c>
       <c r="Y131">
-        <v>38917</v>
+        <v>35073</v>
       </c>
       <c r="Z131">
-        <v>6923857</v>
+        <v>6884940</v>
       </c>
       <c r="AA131">
-        <v>31.345</v>
+        <v>31.169</v>
       </c>
       <c r="AB131">
-        <v>0.176</v>
+        <v>0.159</v>
       </c>
       <c r="AC131">
-        <v>38212</v>
+        <v>37851</v>
       </c>
       <c r="AD131">
-        <v>0.173</v>
+        <v>0.171</v>
       </c>
       <c r="AE131">
         <v>0.058</v>
@@ -16766,22 +16793,22 @@
         <v>344.022</v>
       </c>
       <c r="Y141">
-        <v>34343</v>
+        <v>31022</v>
       </c>
       <c r="Z141">
-        <v>4902726</v>
+        <v>4868383</v>
       </c>
       <c r="AA141">
-        <v>254.85</v>
+        <v>253.065</v>
       </c>
       <c r="AB141">
-        <v>1.785</v>
+        <v>1.613</v>
       </c>
       <c r="AC141">
-        <v>18115</v>
+        <v>16761</v>
       </c>
       <c r="AD141">
-        <v>0.9419999999999999</v>
+        <v>0.871</v>
       </c>
       <c r="AE141">
         <v>0.215</v>
@@ -17028,22 +17055,22 @@
         <v>0.342</v>
       </c>
       <c r="Y143">
-        <v>4216</v>
+        <v>3409</v>
       </c>
       <c r="Z143">
-        <v>745252</v>
+        <v>741036</v>
       </c>
       <c r="AA143">
-        <v>57.539</v>
+        <v>57.213</v>
       </c>
       <c r="AB143">
-        <v>0.326</v>
+        <v>0.263</v>
       </c>
       <c r="AC143">
-        <v>3265</v>
+        <v>3079</v>
       </c>
       <c r="AD143">
-        <v>0.252</v>
+        <v>0.238</v>
       </c>
       <c r="AE143">
         <v>0.038</v>
@@ -18768,22 +18795,22 @@
         <v>0.412</v>
       </c>
       <c r="Y161">
-        <v>67176</v>
+        <v>59734</v>
       </c>
       <c r="Z161">
-        <v>4312786</v>
+        <v>4245610</v>
       </c>
       <c r="AA161">
-        <v>84.12</v>
+        <v>82.81</v>
       </c>
       <c r="AB161">
-        <v>1.31</v>
+        <v>1.165</v>
       </c>
       <c r="AC161">
-        <v>46434</v>
+        <v>45484</v>
       </c>
       <c r="AD161">
-        <v>0.906</v>
+        <v>0.887</v>
       </c>
       <c r="AE161">
         <v>0.019</v>
@@ -20795,22 +20822,22 @@
         <v>3.685</v>
       </c>
       <c r="Y180">
-        <v>34938</v>
+        <v>74436</v>
       </c>
       <c r="Z180">
-        <v>5680116</v>
+        <v>5645178</v>
       </c>
       <c r="AA180">
-        <v>129.879</v>
+        <v>129.081</v>
       </c>
       <c r="AB180">
-        <v>0.799</v>
+        <v>1.702</v>
       </c>
       <c r="AC180">
-        <v>13500</v>
+        <v>19143</v>
       </c>
       <c r="AD180">
-        <v>0.309</v>
+        <v>0.438</v>
       </c>
       <c r="AE180">
         <v>0.364</v>
@@ -21185,28 +21212,28 @@
         <v>8.066000000000001</v>
       </c>
       <c r="Q183">
-        <v>23707</v>
+        <v>23069</v>
       </c>
       <c r="R183">
-        <v>71.622</v>
+        <v>69.694</v>
       </c>
       <c r="S183">
-        <v>132476</v>
+        <v>125220</v>
       </c>
       <c r="T183">
-        <v>400.226</v>
+        <v>378.305</v>
       </c>
       <c r="U183">
-        <v>1269</v>
+        <v>1134</v>
       </c>
       <c r="V183">
-        <v>3.834</v>
+        <v>3.426</v>
       </c>
       <c r="W183">
-        <v>28673</v>
+        <v>23403</v>
       </c>
       <c r="X183">
-        <v>86.625</v>
+        <v>70.703</v>
       </c>
       <c r="Y183">
         <v>871502</v>

</xml_diff>

<commit_message>
Replace ECDC's hospital & ICU data for the UK with official government data
</commit_message>
<xml_diff>
--- a/public/data/latest/owid-covid-latest.xlsx
+++ b/public/data/latest/owid-covid-latest.xlsx
@@ -2772,16 +2772,16 @@
         <v>5.964</v>
       </c>
       <c r="Q11">
-        <v>414</v>
+        <v>396</v>
       </c>
       <c r="R11">
-        <v>45.967</v>
+        <v>43.969</v>
       </c>
       <c r="S11">
-        <v>2043</v>
+        <v>1946</v>
       </c>
       <c r="T11">
-        <v>226.839</v>
+        <v>216.069</v>
       </c>
       <c r="Y11">
         <v>20462</v>
@@ -3515,28 +3515,28 @@
         <v>5.448</v>
       </c>
       <c r="Q18">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="R18">
-        <v>42.452</v>
+        <v>42.538</v>
       </c>
       <c r="S18">
-        <v>2361</v>
+        <v>2188</v>
       </c>
       <c r="T18">
-        <v>203.717</v>
+        <v>188.79</v>
       </c>
       <c r="U18">
-        <v>3647.2</v>
+        <v>3645.176</v>
       </c>
       <c r="V18">
-        <v>314.695</v>
+        <v>314.521</v>
       </c>
       <c r="W18">
-        <v>1135.134</v>
+        <v>1136.146</v>
       </c>
       <c r="X18">
-        <v>97.944</v>
+        <v>98.03100000000001</v>
       </c>
       <c r="Y18">
         <v>39313</v>
@@ -4423,6 +4423,18 @@
       <c r="O27">
         <v>9.17</v>
       </c>
+      <c r="Q27">
+        <v>464</v>
+      </c>
+      <c r="R27">
+        <v>66.77800000000001</v>
+      </c>
+      <c r="S27">
+        <v>4756</v>
+      </c>
+      <c r="T27">
+        <v>684.47</v>
+      </c>
       <c r="Y27">
         <v>11436</v>
       </c>
@@ -6076,16 +6088,16 @@
         <v>12.632</v>
       </c>
       <c r="S43">
-        <v>2664</v>
+        <v>2524</v>
       </c>
       <c r="T43">
-        <v>648.922</v>
+        <v>614.8200000000001</v>
       </c>
       <c r="W43">
-        <v>1496.58</v>
+        <v>1696.997</v>
       </c>
       <c r="X43">
-        <v>364.551</v>
+        <v>413.371</v>
       </c>
       <c r="Y43">
         <v>9919</v>
@@ -6469,28 +6481,28 @@
         <v>13.433</v>
       </c>
       <c r="Q46">
-        <v>741</v>
+        <v>877</v>
       </c>
       <c r="R46">
-        <v>69.194</v>
+        <v>81.89400000000001</v>
       </c>
       <c r="S46">
-        <v>4973</v>
+        <v>6126</v>
       </c>
       <c r="T46">
-        <v>464.377</v>
+        <v>572.043</v>
       </c>
       <c r="U46">
-        <v>1382.641</v>
+        <v>1387.669</v>
       </c>
       <c r="V46">
-        <v>129.11</v>
+        <v>129.58</v>
       </c>
       <c r="W46">
-        <v>8195.290000000001</v>
+        <v>8275.735000000001</v>
       </c>
       <c r="X46">
-        <v>765.273</v>
+        <v>772.784</v>
       </c>
       <c r="Y46">
         <v>68223</v>
@@ -6715,23 +6727,11 @@
       <c r="O48">
         <v>4.809</v>
       </c>
-      <c r="Q48">
-        <v>102</v>
-      </c>
-      <c r="R48">
-        <v>17.61</v>
-      </c>
-      <c r="S48">
-        <v>817</v>
-      </c>
-      <c r="T48">
-        <v>141.052</v>
-      </c>
       <c r="W48">
-        <v>1049.485</v>
+        <v>1050.483</v>
       </c>
       <c r="X48">
-        <v>181.189</v>
+        <v>181.362</v>
       </c>
       <c r="Y48">
         <v>27874</v>
@@ -6771,6 +6771,9 @@
       </c>
       <c r="AK48">
         <v>1145.85</v>
+      </c>
+      <c r="AL48">
+        <v>51.85</v>
       </c>
       <c r="AM48">
         <v>5792203</v>
@@ -7607,16 +7610,16 @@
         <v>3.769</v>
       </c>
       <c r="Q57">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="R57">
-        <v>30.154</v>
+        <v>32.415</v>
       </c>
       <c r="S57">
-        <v>435</v>
+        <v>388</v>
       </c>
       <c r="T57">
-        <v>327.921</v>
+        <v>292.49</v>
       </c>
       <c r="U57">
         <v>29.038</v>
@@ -8220,28 +8223,28 @@
         <v>4.795</v>
       </c>
       <c r="Q62">
-        <v>2650</v>
+        <v>2625</v>
       </c>
       <c r="R62">
-        <v>40.598</v>
+        <v>40.215</v>
       </c>
       <c r="S62">
-        <v>24620</v>
+        <v>24407</v>
       </c>
       <c r="T62">
-        <v>377.182</v>
+        <v>373.919</v>
       </c>
       <c r="U62">
-        <v>1088.981</v>
+        <v>1061.708</v>
       </c>
       <c r="V62">
-        <v>16.683</v>
+        <v>16.266</v>
       </c>
       <c r="W62">
-        <v>7514.751</v>
+        <v>7153.381</v>
       </c>
       <c r="X62">
-        <v>115.127</v>
+        <v>109.591</v>
       </c>
       <c r="Y62">
         <v>226467</v>
@@ -8360,7 +8363,7 @@
         <v>0.128</v>
       </c>
       <c r="AL63">
-        <v>63.89</v>
+        <v>72.22</v>
       </c>
       <c r="AM63">
         <v>2225728</v>
@@ -8633,10 +8636,10 @@
         <v>7.852</v>
       </c>
       <c r="Q66">
-        <v>5546</v>
+        <v>5623</v>
       </c>
       <c r="R66">
-        <v>66.194</v>
+        <v>67.113</v>
       </c>
       <c r="Z66">
         <v>34801593</v>
@@ -8670,6 +8673,9 @@
       </c>
       <c r="AK66">
         <v>483.67</v>
+      </c>
+      <c r="AL66">
+        <v>85.19</v>
       </c>
       <c r="AM66">
         <v>83783945</v>
@@ -8880,10 +8886,10 @@
         <v>4.263</v>
       </c>
       <c r="U68">
-        <v>168.136</v>
+        <v>171.051</v>
       </c>
       <c r="V68">
-        <v>16.131</v>
+        <v>16.411</v>
       </c>
       <c r="Y68">
         <v>13881</v>
@@ -9693,10 +9699,10 @@
         <v>11.372</v>
       </c>
       <c r="S77">
-        <v>6072</v>
+        <v>5856</v>
       </c>
       <c r="T77">
-        <v>628.549</v>
+        <v>606.189</v>
       </c>
       <c r="Y77">
         <v>27265</v>
@@ -9830,16 +9836,16 @@
         <v>0</v>
       </c>
       <c r="Q78">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R78">
-        <v>2.93</v>
+        <v>0</v>
       </c>
       <c r="S78">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="T78">
-        <v>73.26000000000001</v>
+        <v>67.399</v>
       </c>
       <c r="Y78">
         <v>954</v>
@@ -10463,16 +10469,16 @@
         <v>2.112</v>
       </c>
       <c r="Q84">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="R84">
-        <v>5.468</v>
+        <v>8.506</v>
       </c>
       <c r="S84">
-        <v>321</v>
+        <v>491</v>
       </c>
       <c r="T84">
-        <v>65.009</v>
+        <v>99.437</v>
       </c>
       <c r="U84">
         <v>16.109</v>
@@ -10657,7 +10663,7 @@
         <v>13863.95</v>
       </c>
       <c r="AL85">
-        <v>73.15000000000001</v>
+        <v>76.84999999999999</v>
       </c>
       <c r="AM85">
         <v>8655541</v>
@@ -10749,22 +10755,22 @@
         <v>7.733</v>
       </c>
       <c r="Q86">
-        <v>2580</v>
+        <v>2555</v>
       </c>
       <c r="R86">
-        <v>42.672</v>
+        <v>42.258</v>
       </c>
       <c r="S86">
-        <v>26151</v>
+        <v>25706</v>
       </c>
       <c r="T86">
-        <v>432.521</v>
+        <v>425.161</v>
       </c>
       <c r="W86">
-        <v>3630.141</v>
+        <v>6692.321</v>
       </c>
       <c r="X86">
-        <v>60.04</v>
+        <v>110.687</v>
       </c>
       <c r="Y86">
         <v>135106</v>
@@ -11813,10 +11819,10 @@
         <v>9.694000000000001</v>
       </c>
       <c r="S96">
-        <v>1010</v>
+        <v>999</v>
       </c>
       <c r="T96">
-        <v>535.468</v>
+        <v>529.636</v>
       </c>
       <c r="U96">
         <v>90.38200000000001</v>
@@ -11825,10 +11831,10 @@
         <v>47.917</v>
       </c>
       <c r="W96">
-        <v>1487.374</v>
+        <v>786.913</v>
       </c>
       <c r="X96">
-        <v>788.5549999999999</v>
+        <v>417.194</v>
       </c>
       <c r="Y96">
         <v>12352</v>
@@ -12389,10 +12395,10 @@
         <v>32.221</v>
       </c>
       <c r="S102">
-        <v>2510</v>
+        <v>2480</v>
       </c>
       <c r="T102">
-        <v>922.018</v>
+        <v>910.997</v>
       </c>
       <c r="U102">
         <v>120.81</v>
@@ -12532,16 +12538,16 @@
         <v>5.021</v>
       </c>
       <c r="Q103">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="R103">
-        <v>51.12</v>
+        <v>52.718</v>
       </c>
       <c r="S103">
-        <v>150</v>
+        <v>136</v>
       </c>
       <c r="T103">
-        <v>239.626</v>
+        <v>217.261</v>
       </c>
       <c r="Y103">
         <v>9318</v>
@@ -13219,10 +13225,10 @@
         <v>3.559</v>
       </c>
       <c r="W109">
-        <v>21.47</v>
+        <v>23.26</v>
       </c>
       <c r="X109">
-        <v>48.626</v>
+        <v>52.679</v>
       </c>
       <c r="Y109">
         <v>2600</v>
@@ -14669,28 +14675,28 @@
         <v>5.661</v>
       </c>
       <c r="Q123">
-        <v>631</v>
+        <v>724</v>
       </c>
       <c r="R123">
-        <v>36.825</v>
+        <v>42.253</v>
       </c>
       <c r="S123">
-        <v>1797</v>
+        <v>2104</v>
       </c>
       <c r="T123">
-        <v>104.874</v>
+        <v>122.791</v>
       </c>
       <c r="U123">
-        <v>276.622</v>
+        <v>278.605</v>
       </c>
       <c r="V123">
-        <v>16.144</v>
+        <v>16.26</v>
       </c>
       <c r="W123">
-        <v>1779.702</v>
+        <v>1823.327</v>
       </c>
       <c r="X123">
-        <v>103.864</v>
+        <v>106.41</v>
       </c>
       <c r="Z123">
         <v>5323887</v>
@@ -14712,6 +14718,9 @@
       </c>
       <c r="AG123" t="s">
         <v>442</v>
+      </c>
+      <c r="AL123">
+        <v>84.26000000000001</v>
       </c>
       <c r="AM123">
         <v>17134873</v>
@@ -15317,10 +15326,10 @@
         <v>0.764</v>
       </c>
       <c r="S129">
-        <v>129</v>
+        <v>140</v>
       </c>
       <c r="T129">
-        <v>23.795</v>
+        <v>25.824</v>
       </c>
       <c r="U129">
         <v>17.297</v>
@@ -15374,7 +15383,7 @@
         <v>62.53</v>
       </c>
       <c r="AL129">
-        <v>52.78</v>
+        <v>64.81</v>
       </c>
       <c r="AM129">
         <v>5421242</v>
@@ -16358,10 +16367,10 @@
         <v>7.685</v>
       </c>
       <c r="S138">
-        <v>16686</v>
+        <v>16970</v>
       </c>
       <c r="T138">
-        <v>440.885</v>
+        <v>448.389</v>
       </c>
       <c r="Y138">
         <v>48466</v>
@@ -16492,22 +16501,22 @@
         <v>7.664</v>
       </c>
       <c r="Q139">
-        <v>504</v>
+        <v>482</v>
       </c>
       <c r="R139">
-        <v>49.428</v>
+        <v>47.27</v>
       </c>
       <c r="S139">
-        <v>2870</v>
+        <v>2840</v>
       </c>
       <c r="T139">
-        <v>281.463</v>
+        <v>278.521</v>
       </c>
       <c r="W139">
-        <v>263.932</v>
+        <v>317.512</v>
       </c>
       <c r="X139">
-        <v>25.884</v>
+        <v>31.139</v>
       </c>
       <c r="Y139">
         <v>20695</v>
@@ -16754,10 +16763,10 @@
         <v>5.22</v>
       </c>
       <c r="Q141">
-        <v>1210</v>
+        <v>1130</v>
       </c>
       <c r="R141">
-        <v>62.897</v>
+        <v>58.739</v>
       </c>
       <c r="W141">
         <v>6618.185</v>
@@ -18215,10 +18224,10 @@
         <v>15.49</v>
       </c>
       <c r="S156">
-        <v>2426</v>
+        <v>2650</v>
       </c>
       <c r="T156">
-        <v>444.351</v>
+        <v>485.38</v>
       </c>
       <c r="Y156">
         <v>12396</v>
@@ -18346,16 +18355,16 @@
         <v>16.08</v>
       </c>
       <c r="Q157">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="R157">
-        <v>99.089</v>
+        <v>93.798</v>
       </c>
       <c r="S157">
-        <v>1179</v>
+        <v>1174</v>
       </c>
       <c r="T157">
-        <v>567.1180000000001</v>
+        <v>564.713</v>
       </c>
       <c r="U157">
         <v>113.892</v>
@@ -18991,28 +19000,28 @@
         <v>2.264</v>
       </c>
       <c r="Q163">
-        <v>1907</v>
+        <v>2022</v>
       </c>
       <c r="R163">
-        <v>40.787</v>
+        <v>43.247</v>
       </c>
       <c r="S163">
-        <v>10744</v>
+        <v>12172</v>
       </c>
       <c r="T163">
-        <v>229.795</v>
+        <v>260.337</v>
       </c>
       <c r="U163">
-        <v>39.845</v>
+        <v>174.32</v>
       </c>
       <c r="V163">
-        <v>0.852</v>
+        <v>3.728</v>
       </c>
       <c r="W163">
-        <v>990.14</v>
+        <v>2461.404</v>
       </c>
       <c r="X163">
-        <v>21.177</v>
+        <v>52.645</v>
       </c>
       <c r="Z163">
         <v>22660315</v>
@@ -19437,16 +19446,16 @@
         <v>3.649</v>
       </c>
       <c r="Q167">
-        <v>323</v>
+        <v>336</v>
       </c>
       <c r="R167">
-        <v>31.983</v>
+        <v>33.27</v>
       </c>
       <c r="U167">
-        <v>175.722</v>
+        <v>187.569</v>
       </c>
       <c r="V167">
-        <v>17.399</v>
+        <v>18.572</v>
       </c>
       <c r="Y167">
         <v>34116</v>
@@ -20702,6 +20711,9 @@
       <c r="AG179" t="s">
         <v>445</v>
       </c>
+      <c r="AL179">
+        <v>47.22</v>
+      </c>
       <c r="AM179">
         <v>45741000</v>
       </c>
@@ -21036,22 +21048,22 @@
         <v>10.128</v>
       </c>
       <c r="Q182">
-        <v>1751</v>
+        <v>2645</v>
       </c>
       <c r="R182">
-        <v>25.793</v>
+        <v>38.962</v>
       </c>
       <c r="S182">
-        <v>22520</v>
+        <v>30451</v>
       </c>
       <c r="T182">
-        <v>331.733</v>
+        <v>448.561</v>
       </c>
       <c r="W182">
-        <v>13757.061</v>
+        <v>6276</v>
       </c>
       <c r="X182">
-        <v>202.649</v>
+        <v>92.449</v>
       </c>
       <c r="Y182">
         <v>464611</v>

</xml_diff>

<commit_message>
Hospital & ICU weekly update
</commit_message>
<xml_diff>
--- a/public/data/latest/owid-covid-latest.xlsx
+++ b/public/data/latest/owid-covid-latest.xlsx
@@ -2823,16 +2823,16 @@
         <v>5.599</v>
       </c>
       <c r="R11">
-        <v>363</v>
+        <v>372</v>
       </c>
       <c r="S11">
-        <v>40.305</v>
+        <v>41.304</v>
       </c>
       <c r="T11">
-        <v>1864</v>
+        <v>1874</v>
       </c>
       <c r="U11">
-        <v>206.964</v>
+        <v>208.074</v>
       </c>
       <c r="Z11">
         <v>14089</v>
@@ -3602,28 +3602,28 @@
         <v>4.413</v>
       </c>
       <c r="R18">
-        <v>468</v>
+        <v>371</v>
       </c>
       <c r="S18">
-        <v>40.381</v>
+        <v>32.011</v>
       </c>
       <c r="T18">
-        <v>2185</v>
+        <v>1955</v>
       </c>
       <c r="U18">
-        <v>188.531</v>
+        <v>168.685</v>
       </c>
       <c r="V18">
-        <v>3475.21</v>
+        <v>2838.847</v>
       </c>
       <c r="W18">
-        <v>299.855</v>
+        <v>244.947</v>
       </c>
       <c r="X18">
-        <v>1030.928</v>
+        <v>909.524</v>
       </c>
       <c r="Y18">
-        <v>88.953</v>
+        <v>78.477</v>
       </c>
       <c r="Z18">
         <v>42414</v>
@@ -4538,16 +4538,16 @@
         <v>7.792</v>
       </c>
       <c r="R27">
-        <v>453</v>
+        <v>380</v>
       </c>
       <c r="S27">
-        <v>65.194</v>
+        <v>54.688</v>
       </c>
       <c r="T27">
-        <v>4689</v>
+        <v>4205</v>
       </c>
       <c r="U27">
-        <v>674.827</v>
+        <v>605.171</v>
       </c>
       <c r="Z27">
         <v>9642</v>
@@ -5052,16 +5052,16 @@
         <v>3.649</v>
       </c>
       <c r="R32">
-        <v>844</v>
+        <v>899</v>
       </c>
       <c r="S32">
-        <v>22.362</v>
+        <v>23.82</v>
       </c>
       <c r="T32">
-        <v>4592</v>
+        <v>4848</v>
       </c>
       <c r="U32">
-        <v>121.668</v>
+        <v>128.451</v>
       </c>
       <c r="Z32">
         <v>67878</v>
@@ -6265,16 +6265,16 @@
         <v>8.734</v>
       </c>
       <c r="T43">
-        <v>2453</v>
+        <v>2131</v>
       </c>
       <c r="U43">
-        <v>597.525</v>
+        <v>519.0890000000001</v>
       </c>
       <c r="X43">
-        <v>1530.822</v>
+        <v>1211.565</v>
       </c>
       <c r="Y43">
-        <v>372.892</v>
+        <v>295.124</v>
       </c>
       <c r="Z43">
         <v>7713</v>
@@ -6533,28 +6533,28 @@
         <v>3.751</v>
       </c>
       <c r="R45">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="S45">
-        <v>31.967</v>
+        <v>35.392</v>
       </c>
       <c r="T45">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="U45">
-        <v>207.787</v>
+        <v>213.495</v>
       </c>
       <c r="V45">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="W45">
-        <v>25.117</v>
+        <v>17.125</v>
       </c>
       <c r="X45">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="Y45">
-        <v>133.577</v>
+        <v>137.002</v>
       </c>
       <c r="Z45">
         <v>13231</v>
@@ -6688,28 +6688,28 @@
         <v>16.475</v>
       </c>
       <c r="R46">
-        <v>933</v>
+        <v>1098</v>
       </c>
       <c r="S46">
-        <v>87.123</v>
+        <v>102.531</v>
       </c>
       <c r="T46">
-        <v>6288</v>
+        <v>6830</v>
       </c>
       <c r="U46">
-        <v>587.171</v>
+        <v>637.782</v>
       </c>
       <c r="V46">
-        <v>1476.158</v>
+        <v>1923.631</v>
       </c>
       <c r="W46">
-        <v>137.843</v>
+        <v>179.628</v>
       </c>
       <c r="X46">
-        <v>8835.83</v>
+        <v>12029.48</v>
       </c>
       <c r="Y46">
-        <v>825.086</v>
+        <v>1123.307</v>
       </c>
       <c r="Z46">
         <v>59222</v>
@@ -6946,11 +6946,23 @@
       <c r="P48">
         <v>4.267</v>
       </c>
+      <c r="R48">
+        <v>138</v>
+      </c>
+      <c r="S48">
+        <v>23.825</v>
+      </c>
+      <c r="T48">
+        <v>875</v>
+      </c>
+      <c r="U48">
+        <v>151.065</v>
+      </c>
       <c r="X48">
-        <v>1002.598</v>
+        <v>861.9349999999999</v>
       </c>
       <c r="Y48">
-        <v>173.094</v>
+        <v>148.809</v>
       </c>
       <c r="Z48">
         <v>25827</v>
@@ -7865,28 +7877,28 @@
         <v>4.954</v>
       </c>
       <c r="R57">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="S57">
-        <v>35.431</v>
+        <v>32.415</v>
       </c>
       <c r="T57">
-        <v>431</v>
+        <v>418</v>
       </c>
       <c r="U57">
-        <v>324.906</v>
+        <v>315.106</v>
       </c>
       <c r="V57">
-        <v>33.043</v>
+        <v>31.04</v>
       </c>
       <c r="W57">
-        <v>24.909</v>
+        <v>23.399</v>
       </c>
       <c r="X57">
-        <v>283.367</v>
+        <v>277.359</v>
       </c>
       <c r="Y57">
-        <v>213.614</v>
+        <v>209.085</v>
       </c>
       <c r="Z57">
         <v>6793</v>
@@ -8367,6 +8379,18 @@
       <c r="P61">
         <v>0.825</v>
       </c>
+      <c r="R61">
+        <v>29</v>
+      </c>
+      <c r="S61">
+        <v>5.234</v>
+      </c>
+      <c r="T61">
+        <v>176</v>
+      </c>
+      <c r="U61">
+        <v>31.765</v>
+      </c>
       <c r="Z61">
         <v>4326</v>
       </c>
@@ -8502,28 +8526,28 @@
         <v>6.023</v>
       </c>
       <c r="R62">
-        <v>2665</v>
+        <v>2620</v>
       </c>
       <c r="S62">
-        <v>40.828</v>
+        <v>40.139</v>
       </c>
       <c r="T62">
-        <v>24780</v>
+        <v>24526</v>
       </c>
       <c r="U62">
-        <v>379.633</v>
+        <v>375.742</v>
       </c>
       <c r="V62">
-        <v>1085.085</v>
+        <v>1325.674</v>
       </c>
       <c r="W62">
-        <v>16.624</v>
+        <v>20.31</v>
       </c>
       <c r="X62">
-        <v>7086.172</v>
+        <v>8387.495000000001</v>
       </c>
       <c r="Y62">
-        <v>108.561</v>
+        <v>128.498</v>
       </c>
       <c r="Z62">
         <v>186188</v>
@@ -8936,10 +8960,16 @@
         <v>10.606</v>
       </c>
       <c r="R66">
-        <v>5745</v>
+        <v>5300</v>
       </c>
       <c r="S66">
-        <v>68.569</v>
+        <v>63.258</v>
+      </c>
+      <c r="X66">
+        <v>2324.214</v>
+      </c>
+      <c r="Y66">
+        <v>27.741</v>
       </c>
       <c r="AA66">
         <v>35118592</v>
@@ -9195,10 +9225,10 @@
         <v>3.303</v>
       </c>
       <c r="V68">
-        <v>120.513</v>
+        <v>103.991</v>
       </c>
       <c r="W68">
-        <v>11.562</v>
+        <v>9.977</v>
       </c>
       <c r="Z68">
         <v>12556</v>
@@ -10050,10 +10080,10 @@
         <v>10.958</v>
       </c>
       <c r="T77">
-        <v>5619</v>
+        <v>4980</v>
       </c>
       <c r="U77">
-        <v>581.6559999999999</v>
+        <v>515.509</v>
       </c>
       <c r="Z77">
         <v>18550</v>
@@ -10192,6 +10222,18 @@
       <c r="P78">
         <v>0</v>
       </c>
+      <c r="R78">
+        <v>0</v>
+      </c>
+      <c r="S78">
+        <v>0</v>
+      </c>
+      <c r="T78">
+        <v>20</v>
+      </c>
+      <c r="U78">
+        <v>58.608</v>
+      </c>
       <c r="Z78">
         <v>914</v>
       </c>
@@ -10826,28 +10868,28 @@
         <v>5.237</v>
       </c>
       <c r="R84">
-        <v>65</v>
+        <v>128</v>
       </c>
       <c r="S84">
-        <v>13.164</v>
+        <v>25.922</v>
       </c>
       <c r="T84">
-        <v>673</v>
+        <v>1426</v>
       </c>
       <c r="U84">
-        <v>136.296</v>
+        <v>288.793</v>
       </c>
       <c r="V84">
-        <v>15.103</v>
+        <v>29.198</v>
       </c>
       <c r="W84">
-        <v>3.059</v>
+        <v>5.913</v>
       </c>
       <c r="X84">
-        <v>382.6</v>
+        <v>695.728</v>
       </c>
       <c r="Y84">
-        <v>77.48399999999999</v>
+        <v>140.898</v>
       </c>
       <c r="Z84">
         <v>17765</v>
@@ -11121,22 +11163,22 @@
         <v>8.404</v>
       </c>
       <c r="R86">
-        <v>2583</v>
+        <v>2615</v>
       </c>
       <c r="S86">
-        <v>42.721</v>
+        <v>43.25</v>
       </c>
       <c r="T86">
-        <v>25658</v>
+        <v>26042</v>
       </c>
       <c r="U86">
-        <v>424.367</v>
+        <v>430.718</v>
       </c>
       <c r="X86">
-        <v>3253.504</v>
+        <v>3948.68</v>
       </c>
       <c r="Y86">
-        <v>53.811</v>
+        <v>65.309</v>
       </c>
       <c r="Z86">
         <v>141641</v>
@@ -12238,17 +12280,23 @@
       <c r="P96">
         <v>9.846</v>
       </c>
+      <c r="T96">
+        <v>1147</v>
+      </c>
+      <c r="U96">
+        <v>608.1</v>
+      </c>
       <c r="V96">
-        <v>109.048</v>
+        <v>116.907</v>
       </c>
       <c r="W96">
-        <v>57.813</v>
+        <v>61.98</v>
       </c>
       <c r="X96">
-        <v>827.192</v>
+        <v>921.504</v>
       </c>
       <c r="Y96">
-        <v>438.549</v>
+        <v>488.55</v>
       </c>
       <c r="Z96">
         <v>12293</v>
@@ -12836,22 +12884,22 @@
         <v>14.169</v>
       </c>
       <c r="T102">
-        <v>2571</v>
+        <v>2212</v>
       </c>
       <c r="U102">
-        <v>944.425</v>
+        <v>812.551</v>
       </c>
       <c r="V102">
-        <v>128.604</v>
+        <v>109.118</v>
       </c>
       <c r="W102">
-        <v>47.241</v>
+        <v>40.083</v>
       </c>
       <c r="X102">
-        <v>709.269</v>
+        <v>649.838</v>
       </c>
       <c r="Y102">
-        <v>260.541</v>
+        <v>238.71</v>
       </c>
       <c r="Z102">
         <v>11369</v>
@@ -12991,16 +13039,16 @@
         <v>5.477</v>
       </c>
       <c r="R103">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="S103">
-        <v>54.315</v>
+        <v>36.743</v>
       </c>
       <c r="T103">
-        <v>125</v>
+        <v>92</v>
       </c>
       <c r="U103">
-        <v>199.688</v>
+        <v>146.97</v>
       </c>
       <c r="Z103">
         <v>10406</v>
@@ -13705,10 +13753,10 @@
         <v>2.265</v>
       </c>
       <c r="X109">
-        <v>25.943</v>
+        <v>34.889</v>
       </c>
       <c r="Y109">
-        <v>58.757</v>
+        <v>79.018</v>
       </c>
       <c r="Z109">
         <v>2600</v>
@@ -15239,28 +15287,28 @@
         <v>5.778</v>
       </c>
       <c r="R123">
-        <v>704</v>
+        <v>711</v>
       </c>
       <c r="S123">
-        <v>41.086</v>
+        <v>41.494</v>
       </c>
       <c r="T123">
-        <v>2006</v>
+        <v>1850</v>
       </c>
       <c r="U123">
-        <v>117.071</v>
+        <v>107.967</v>
       </c>
       <c r="V123">
-        <v>318.264</v>
+        <v>278.605</v>
       </c>
       <c r="W123">
-        <v>18.574</v>
+        <v>16.26</v>
       </c>
       <c r="X123">
-        <v>1694.435</v>
+        <v>1552.654</v>
       </c>
       <c r="Y123">
-        <v>98.88800000000001</v>
+        <v>90.614</v>
       </c>
       <c r="AA123">
         <v>5323887</v>
@@ -15929,22 +15977,22 @@
         <v>1.159</v>
       </c>
       <c r="T129">
-        <v>128</v>
+        <v>143</v>
       </c>
       <c r="U129">
-        <v>23.611</v>
+        <v>26.378</v>
       </c>
       <c r="V129">
-        <v>10.175</v>
+        <v>19.332</v>
       </c>
       <c r="W129">
-        <v>1.877</v>
+        <v>3.566</v>
       </c>
       <c r="X129">
-        <v>95.64100000000001</v>
+        <v>106.833</v>
       </c>
       <c r="Y129">
-        <v>17.642</v>
+        <v>19.706</v>
       </c>
       <c r="Z129">
         <v>27920</v>
@@ -17003,10 +17051,10 @@
         <v>8.361000000000001</v>
       </c>
       <c r="T138">
-        <v>16786</v>
+        <v>16727</v>
       </c>
       <c r="U138">
-        <v>443.527</v>
+        <v>441.968</v>
       </c>
       <c r="Z138">
         <v>58371</v>
@@ -17143,22 +17191,22 @@
         <v>12.777</v>
       </c>
       <c r="R139">
-        <v>500</v>
+        <v>558</v>
       </c>
       <c r="S139">
-        <v>49.035</v>
+        <v>54.724</v>
       </c>
       <c r="T139">
-        <v>3044</v>
+        <v>3770</v>
       </c>
       <c r="U139">
-        <v>298.528</v>
+        <v>369.727</v>
       </c>
       <c r="X139">
-        <v>267.901</v>
+        <v>455.431</v>
       </c>
       <c r="Y139">
-        <v>26.273</v>
+        <v>44.665</v>
       </c>
       <c r="Z139">
         <v>23440</v>
@@ -17414,10 +17462,10 @@
         <v>4.641</v>
       </c>
       <c r="R141">
-        <v>1119</v>
+        <v>1065</v>
       </c>
       <c r="S141">
-        <v>58.167</v>
+        <v>55.36</v>
       </c>
       <c r="X141">
         <v>5310.204</v>
@@ -18974,10 +19022,10 @@
         <v>14.208</v>
       </c>
       <c r="T156">
-        <v>2771</v>
+        <v>2980</v>
       </c>
       <c r="U156">
-        <v>507.542</v>
+        <v>545.823</v>
       </c>
       <c r="Z156">
         <v>15440</v>
@@ -19117,28 +19165,28 @@
         <v>11.751</v>
       </c>
       <c r="R157">
-        <v>190</v>
+        <v>202</v>
       </c>
       <c r="S157">
-        <v>91.393</v>
+        <v>97.16500000000001</v>
       </c>
       <c r="T157">
-        <v>1173</v>
+        <v>1192</v>
       </c>
       <c r="U157">
-        <v>564.232</v>
+        <v>573.371</v>
       </c>
       <c r="V157">
-        <v>112.893</v>
+        <v>113.892</v>
       </c>
       <c r="W157">
-        <v>54.303</v>
+        <v>54.784</v>
       </c>
       <c r="X157">
-        <v>747.29</v>
+        <v>743.294</v>
       </c>
       <c r="Y157">
-        <v>359.458</v>
+        <v>357.536</v>
       </c>
       <c r="Z157">
         <v>6193</v>
@@ -19791,17 +19839,29 @@
       <c r="P163">
         <v>4.29</v>
       </c>
+      <c r="R163">
+        <v>2318</v>
+      </c>
+      <c r="S163">
+        <v>49.578</v>
+      </c>
+      <c r="T163">
+        <v>14951</v>
+      </c>
+      <c r="U163">
+        <v>319.775</v>
+      </c>
       <c r="V163">
-        <v>47.814</v>
+        <v>94.631</v>
       </c>
       <c r="W163">
-        <v>1.023</v>
+        <v>2.024</v>
       </c>
       <c r="X163">
-        <v>1264.072</v>
+        <v>1832.854</v>
       </c>
       <c r="Y163">
-        <v>27.036</v>
+        <v>39.201</v>
       </c>
       <c r="AI163">
         <v>676186</v>
@@ -20220,16 +20280,22 @@
         <v>13.056</v>
       </c>
       <c r="R167">
-        <v>359</v>
+        <v>372</v>
       </c>
       <c r="S167">
-        <v>35.547</v>
+        <v>36.834</v>
+      </c>
+      <c r="T167">
+        <v>2844</v>
+      </c>
+      <c r="U167">
+        <v>281.605</v>
       </c>
       <c r="V167">
-        <v>205.338</v>
+        <v>172.761</v>
       </c>
       <c r="W167">
-        <v>20.332</v>
+        <v>17.106</v>
       </c>
       <c r="Z167">
         <v>29552</v>
@@ -21915,22 +21981,22 @@
         <v>15.848</v>
       </c>
       <c r="R182">
-        <v>2821</v>
+        <v>3626</v>
       </c>
       <c r="S182">
-        <v>41.555</v>
+        <v>53.413</v>
       </c>
       <c r="T182">
-        <v>30370</v>
+        <v>36797</v>
       </c>
       <c r="U182">
-        <v>447.368</v>
+        <v>542.0410000000001</v>
       </c>
       <c r="X182">
-        <v>22608</v>
+        <v>16617</v>
       </c>
       <c r="Y182">
-        <v>333.029</v>
+        <v>244.778</v>
       </c>
       <c r="Z182">
         <v>536947</v>
@@ -22070,28 +22136,28 @@
         <v>10.017</v>
       </c>
       <c r="R183">
-        <v>23821</v>
+        <v>23891</v>
       </c>
       <c r="S183">
-        <v>71.96599999999999</v>
+        <v>72.178</v>
       </c>
       <c r="T183">
-        <v>132370</v>
+        <v>128947</v>
       </c>
       <c r="U183">
-        <v>399.906</v>
+        <v>389.565</v>
       </c>
       <c r="V183">
-        <v>1269</v>
+        <v>1273</v>
       </c>
       <c r="W183">
-        <v>3.834</v>
+        <v>3.846</v>
       </c>
       <c r="X183">
-        <v>28673</v>
+        <v>33902</v>
       </c>
       <c r="Y183">
-        <v>86.625</v>
+        <v>102.422</v>
       </c>
       <c r="Z183">
         <v>875195</v>

</xml_diff>

<commit_message>
Add Israel to hospital & ICU data
</commit_message>
<xml_diff>
--- a/public/data/latest/owid-covid-latest.xlsx
+++ b/public/data/latest/owid-covid-latest.xlsx
@@ -5097,16 +5097,16 @@
         <v>3.369</v>
       </c>
       <c r="R32">
-        <v>859</v>
+        <v>851</v>
       </c>
       <c r="S32">
-        <v>22.76</v>
+        <v>22.548</v>
       </c>
       <c r="T32">
-        <v>4490</v>
+        <v>4395</v>
       </c>
       <c r="U32">
-        <v>118.965</v>
+        <v>116.448</v>
       </c>
       <c r="Z32">
         <v>16895320</v>
@@ -11118,6 +11118,30 @@
       <c r="P85">
         <v>5.876</v>
       </c>
+      <c r="R85">
+        <v>399</v>
+      </c>
+      <c r="S85">
+        <v>46.098</v>
+      </c>
+      <c r="T85">
+        <v>1822</v>
+      </c>
+      <c r="U85">
+        <v>210.501</v>
+      </c>
+      <c r="V85">
+        <v>1195</v>
+      </c>
+      <c r="W85">
+        <v>138.062</v>
+      </c>
+      <c r="X85">
+        <v>1949</v>
+      </c>
+      <c r="Y85">
+        <v>225.174</v>
+      </c>
       <c r="Z85">
         <v>10001084</v>
       </c>
@@ -22136,22 +22160,22 @@
         <v>18.346</v>
       </c>
       <c r="R183">
-        <v>3953</v>
+        <v>3960</v>
       </c>
       <c r="S183">
-        <v>58.23</v>
+        <v>58.333</v>
       </c>
       <c r="T183">
-        <v>38676</v>
+        <v>38562</v>
       </c>
       <c r="U183">
-        <v>569.72</v>
+        <v>568.0410000000001</v>
       </c>
       <c r="X183">
-        <v>28362</v>
+        <v>28394</v>
       </c>
       <c r="Y183">
-        <v>417.789</v>
+        <v>418.26</v>
       </c>
       <c r="Z183">
         <v>63623219</v>
@@ -22291,16 +22315,16 @@
         <v>9.281000000000001</v>
       </c>
       <c r="R184">
-        <v>22304</v>
+        <v>22008</v>
       </c>
       <c r="S184">
-        <v>67.383</v>
+        <v>66.489</v>
       </c>
       <c r="T184">
-        <v>119927</v>
+        <v>116264</v>
       </c>
       <c r="U184">
-        <v>362.314</v>
+        <v>351.248</v>
       </c>
       <c r="V184">
         <v>1158</v>

</xml_diff>

<commit_message>
Replace Swedish data in JHU with official time series
</commit_message>
<xml_diff>
--- a/public/data/latest/owid-covid-latest.xlsx
+++ b/public/data/latest/owid-covid-latest.xlsx
@@ -21497,40 +21497,40 @@
         <v>450</v>
       </c>
       <c r="E168">
-        <v>556289</v>
+        <v>560472</v>
       </c>
       <c r="F168">
-        <v>9123</v>
+        <v>4174</v>
       </c>
       <c r="G168">
-        <v>3289.143</v>
+        <v>3211.429</v>
       </c>
       <c r="H168">
-        <v>11247</v>
+        <v>11391</v>
       </c>
       <c r="I168">
-        <v>242</v>
+        <v>0</v>
       </c>
       <c r="J168">
-        <v>132</v>
+        <v>18.571</v>
       </c>
       <c r="K168">
-        <v>55082.1</v>
+        <v>55496.288</v>
       </c>
       <c r="L168">
-        <v>903.333</v>
+        <v>413.297</v>
       </c>
       <c r="M168">
-        <v>325.681</v>
+        <v>317.986</v>
       </c>
       <c r="N168">
-        <v>1113.645</v>
+        <v>1127.903</v>
       </c>
       <c r="O168">
-        <v>23.962</v>
+        <v>0</v>
       </c>
       <c r="P168">
-        <v>13.07</v>
+        <v>1.839</v>
       </c>
       <c r="Q168">
         <v>1.3</v>
@@ -24102,40 +24102,40 @@
         <v>450</v>
       </c>
       <c r="E191">
-        <v>100274664</v>
+        <v>100278847</v>
       </c>
       <c r="F191">
-        <v>550396</v>
+        <v>545447</v>
       </c>
       <c r="G191">
-        <v>583090.286</v>
+        <v>583012.571</v>
       </c>
       <c r="H191">
-        <v>2157446</v>
+        <v>2157590</v>
       </c>
       <c r="I191">
-        <v>17361</v>
+        <v>17119</v>
       </c>
       <c r="J191">
-        <v>14357</v>
+        <v>14243.571</v>
       </c>
       <c r="K191">
-        <v>12864.304</v>
+        <v>12864.841</v>
       </c>
       <c r="L191">
-        <v>70.611</v>
+        <v>69.976</v>
       </c>
       <c r="M191">
-        <v>74.80500000000001</v>
+        <v>74.795</v>
       </c>
       <c r="N191">
-        <v>276.78</v>
+        <v>276.799</v>
       </c>
       <c r="O191">
-        <v>2.227</v>
+        <v>2.196</v>
       </c>
       <c r="P191">
-        <v>1.842</v>
+        <v>1.827</v>
       </c>
       <c r="Q191">
         <v>1.06</v>

</xml_diff>

<commit_message>
Hospital & ICU data update
</commit_message>
<xml_diff>
--- a/public/data/latest/owid-covid-latest.xlsx
+++ b/public/data/latest/owid-covid-latest.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="934" uniqueCount="457">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="934" uniqueCount="458">
   <si>
     <t>iso_code</t>
   </si>
@@ -1370,6 +1370,9 @@
   </si>
   <si>
     <t>2021-01-19</t>
+  </si>
+  <si>
+    <t>2021-01-29</t>
   </si>
   <si>
     <t>2021-01-27</t>
@@ -2289,7 +2292,7 @@
         <v>7.3</v>
       </c>
       <c r="AH5" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="AR5">
         <v>52.78</v>
@@ -2571,7 +2574,7 @@
         <v>3.8</v>
       </c>
       <c r="AH8" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="AI8">
         <v>327999</v>
@@ -2821,7 +2824,7 @@
         <v>6287</v>
       </c>
       <c r="AH10" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="AR10">
         <v>52.31</v>
@@ -2922,16 +2925,16 @@
         <v>1.03</v>
       </c>
       <c r="R11">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="S11">
-        <v>36.419</v>
+        <v>35.863</v>
       </c>
       <c r="T11">
-        <v>1635</v>
+        <v>1518</v>
       </c>
       <c r="U11">
-        <v>181.538</v>
+        <v>168.547</v>
       </c>
       <c r="Z11">
         <v>8488882</v>
@@ -2952,7 +2955,7 @@
         <v>23.78</v>
       </c>
       <c r="AH11" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="AI11">
         <v>169439</v>
@@ -3294,7 +3297,7 @@
         <v>30.6</v>
       </c>
       <c r="AH14" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="AI14">
         <v>144130</v>
@@ -3437,7 +3440,7 @@
         <v>25.6</v>
       </c>
       <c r="AH15" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="AR15">
         <v>80.09</v>
@@ -3657,7 +3660,7 @@
         <v>10</v>
       </c>
       <c r="AH17" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="AR17">
         <v>27.78</v>
@@ -3755,28 +3758,28 @@
         <v>1.09</v>
       </c>
       <c r="R18">
-        <v>367</v>
+        <v>322</v>
       </c>
       <c r="S18">
-        <v>31.666</v>
+        <v>27.783</v>
       </c>
       <c r="T18">
-        <v>1892</v>
+        <v>1923</v>
       </c>
       <c r="U18">
-        <v>163.25</v>
+        <v>165.924</v>
       </c>
       <c r="V18">
-        <v>2533.312</v>
+        <v>2420</v>
       </c>
       <c r="W18">
-        <v>218.585</v>
+        <v>208.808</v>
       </c>
       <c r="X18">
-        <v>814.423</v>
+        <v>967.191</v>
       </c>
       <c r="Y18">
-        <v>70.27200000000001</v>
+        <v>83.453</v>
       </c>
       <c r="Z18">
         <v>7971536</v>
@@ -3803,7 +3806,7 @@
         <v>17.9</v>
       </c>
       <c r="AH18" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="AI18">
         <v>246870</v>
@@ -4148,7 +4151,7 @@
         <v>3804.9</v>
       </c>
       <c r="AH21" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="AR21">
         <v>81.94</v>
@@ -4270,7 +4273,7 @@
         <v>2.5</v>
       </c>
       <c r="AH22" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="AR22">
         <v>30.56</v>
@@ -4772,16 +4775,16 @@
         <v>0.78</v>
       </c>
       <c r="R27">
-        <v>340</v>
+        <v>281</v>
       </c>
       <c r="S27">
-        <v>48.932</v>
+        <v>40.441</v>
       </c>
       <c r="T27">
-        <v>3485</v>
+        <v>2857</v>
       </c>
       <c r="U27">
-        <v>501.551</v>
+        <v>411.171</v>
       </c>
       <c r="Z27">
         <v>1345912</v>
@@ -4808,7 +4811,7 @@
         <v>15.1</v>
       </c>
       <c r="AH27" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="AI27">
         <v>32917</v>
@@ -5313,16 +5316,16 @@
         <v>1.02</v>
       </c>
       <c r="R32">
-        <v>851</v>
+        <v>834</v>
       </c>
       <c r="S32">
-        <v>22.548</v>
+        <v>22.097</v>
       </c>
       <c r="T32">
-        <v>4395</v>
+        <v>3975</v>
       </c>
       <c r="U32">
-        <v>116.448</v>
+        <v>105.32</v>
       </c>
       <c r="Z32">
         <v>17120912</v>
@@ -5349,7 +5352,7 @@
         <v>11.1</v>
       </c>
       <c r="AH32" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="AI32">
         <v>903664</v>
@@ -5483,7 +5486,7 @@
         <v>1.407</v>
       </c>
       <c r="AH33" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="AR33">
         <v>64.81</v>
@@ -5789,7 +5792,7 @@
         <v>12.2</v>
       </c>
       <c r="AH36" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="AI36">
         <v>67096</v>
@@ -6051,7 +6054,7 @@
         <v>4</v>
       </c>
       <c r="AH38" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="AR38">
         <v>81.02</v>
@@ -6500,7 +6503,7 @@
         <v>11</v>
       </c>
       <c r="AH42" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="AR42">
         <v>17.59</v>
@@ -6595,16 +6598,16 @@
         <v>0.82</v>
       </c>
       <c r="T43">
-        <v>1761</v>
+        <v>1474</v>
       </c>
       <c r="U43">
-        <v>428.961</v>
+        <v>359.051</v>
       </c>
       <c r="X43">
-        <v>978.92</v>
+        <v>825.838</v>
       </c>
       <c r="Y43">
-        <v>238.455</v>
+        <v>201.165</v>
       </c>
       <c r="Z43">
         <v>1169837</v>
@@ -6631,7 +6634,7 @@
         <v>9.199999999999999</v>
       </c>
       <c r="AH43" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="AI43">
         <v>69984</v>
@@ -6783,7 +6786,7 @@
         <v>28.1</v>
       </c>
       <c r="AH44" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="AR44">
         <v>83.33</v>
@@ -6881,28 +6884,28 @@
         <v>0.89</v>
       </c>
       <c r="R45">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="S45">
-        <v>44.526</v>
+        <v>39.959</v>
       </c>
       <c r="T45">
-        <v>208</v>
+        <v>173</v>
       </c>
       <c r="U45">
-        <v>237.47</v>
+        <v>197.511</v>
       </c>
       <c r="V45">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="W45">
-        <v>19.409</v>
+        <v>17.125</v>
       </c>
       <c r="X45">
-        <v>112</v>
+        <v>86</v>
       </c>
       <c r="Y45">
-        <v>127.869</v>
+        <v>98.185</v>
       </c>
       <c r="Z45">
         <v>1311720</v>
@@ -6929,7 +6932,7 @@
         <v>73.5</v>
       </c>
       <c r="AH45" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="AI45">
         <v>17379</v>
@@ -7051,28 +7054,28 @@
         <v>0.99</v>
       </c>
       <c r="R46">
-        <v>1119</v>
+        <v>1047</v>
       </c>
       <c r="S46">
-        <v>104.492</v>
+        <v>97.768</v>
       </c>
       <c r="T46">
-        <v>6449</v>
+        <v>5798</v>
       </c>
       <c r="U46">
-        <v>602.205</v>
+        <v>541.415</v>
       </c>
       <c r="V46">
-        <v>1985.975</v>
+        <v>1845.197</v>
       </c>
       <c r="W46">
-        <v>185.449</v>
+        <v>172.304</v>
       </c>
       <c r="X46">
-        <v>11397.99</v>
+        <v>10376.344</v>
       </c>
       <c r="Y46">
-        <v>1064.339</v>
+        <v>968.938</v>
       </c>
       <c r="AA46">
         <v>49859</v>
@@ -7093,7 +7096,7 @@
         <v>6.6</v>
       </c>
       <c r="AH46" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="AI46">
         <v>236697</v>
@@ -7236,7 +7239,7 @@
         <v>3.7</v>
       </c>
       <c r="AH47" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="AR47">
         <v>21.3</v>
@@ -7331,22 +7334,22 @@
         <v>0.84</v>
       </c>
       <c r="R48">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="S48">
-        <v>22.617</v>
+        <v>21.408</v>
       </c>
       <c r="T48">
-        <v>799</v>
+        <v>725</v>
       </c>
       <c r="U48">
-        <v>137.944</v>
+        <v>125.168</v>
       </c>
       <c r="X48">
-        <v>667.401</v>
+        <v>607.544</v>
       </c>
       <c r="Y48">
-        <v>115.224</v>
+        <v>104.89</v>
       </c>
       <c r="Z48">
         <v>12745107</v>
@@ -7373,7 +7376,7 @@
         <v>123.4</v>
       </c>
       <c r="AH48" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="AI48">
         <v>221067</v>
@@ -7688,7 +7691,7 @@
         <v>4.4</v>
       </c>
       <c r="AH51" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="AR51">
         <v>70.37</v>
@@ -7810,7 +7813,7 @@
         <v>0.27</v>
       </c>
       <c r="AH52" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="AI52">
         <v>2982</v>
@@ -8036,7 +8039,7 @@
         <v>105.205</v>
       </c>
       <c r="AH54" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="AR54">
         <v>47.22</v>
@@ -8330,22 +8333,22 @@
         <v>33.923</v>
       </c>
       <c r="T57">
-        <v>433</v>
+        <v>425</v>
       </c>
       <c r="U57">
-        <v>326.413</v>
+        <v>320.383</v>
       </c>
       <c r="V57">
-        <v>29.038</v>
+        <v>32.042</v>
       </c>
       <c r="W57">
-        <v>21.89</v>
+        <v>24.154</v>
       </c>
       <c r="X57">
-        <v>298.387</v>
+        <v>295.383</v>
       </c>
       <c r="Y57">
-        <v>224.936</v>
+        <v>222.672</v>
       </c>
       <c r="Z57">
         <v>754948</v>
@@ -8372,7 +8375,7 @@
         <v>9.800000000000001</v>
       </c>
       <c r="AH57" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="AI57">
         <v>31629</v>
@@ -8622,7 +8625,7 @@
         <v>12.3</v>
       </c>
       <c r="AH59" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="AR59">
         <v>40.74</v>
@@ -8747,7 +8750,7 @@
         <v>528</v>
       </c>
       <c r="AH60" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="AR60">
         <v>41.67</v>
@@ -8848,16 +8851,16 @@
         <v>0.99</v>
       </c>
       <c r="R61">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="S61">
-        <v>5.053</v>
+        <v>4.332</v>
       </c>
       <c r="T61">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="U61">
-        <v>26.17</v>
+        <v>24.546</v>
       </c>
       <c r="Z61">
         <v>2773595</v>
@@ -8884,7 +8887,7 @@
         <v>40.9</v>
       </c>
       <c r="AH61" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="AI61">
         <v>138323</v>
@@ -9009,28 +9012,28 @@
         <v>1.17</v>
       </c>
       <c r="R62">
-        <v>2766</v>
+        <v>2955</v>
       </c>
       <c r="S62">
-        <v>42.376</v>
+        <v>45.271</v>
       </c>
       <c r="T62">
-        <v>25235</v>
+        <v>26357</v>
       </c>
       <c r="U62">
-        <v>386.604</v>
+        <v>403.793</v>
       </c>
       <c r="V62">
-        <v>1354.896</v>
+        <v>1656.849</v>
       </c>
       <c r="W62">
-        <v>20.757</v>
+        <v>25.383</v>
       </c>
       <c r="X62">
-        <v>9104.391</v>
+        <v>10483.638</v>
       </c>
       <c r="Y62">
-        <v>139.481</v>
+        <v>160.611</v>
       </c>
       <c r="AA62">
         <v>199211</v>
@@ -9051,7 +9054,7 @@
         <v>14.1</v>
       </c>
       <c r="AH62" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="AI62">
         <v>1136906</v>
@@ -9467,16 +9470,16 @@
         <v>0.96</v>
       </c>
       <c r="R66">
-        <v>4950</v>
+        <v>4607</v>
       </c>
       <c r="S66">
-        <v>59.081</v>
+        <v>54.987</v>
       </c>
       <c r="X66">
-        <v>2333.297</v>
+        <v>2510.918</v>
       </c>
       <c r="Y66">
-        <v>27.849</v>
+        <v>29.969</v>
       </c>
       <c r="Z66">
         <v>37387669</v>
@@ -9497,7 +9500,7 @@
         <v>9.5</v>
       </c>
       <c r="AH66" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="AI66">
         <v>2104317</v>
@@ -9646,7 +9649,7 @@
         <v>12.7</v>
       </c>
       <c r="AH67" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="AR67">
         <v>38.89</v>
@@ -9750,10 +9753,10 @@
         <v>0.92</v>
       </c>
       <c r="V68">
-        <v>102.048</v>
+        <v>87.46899999999999</v>
       </c>
       <c r="W68">
-        <v>9.791</v>
+        <v>8.391999999999999</v>
       </c>
       <c r="Z68">
         <v>4019134</v>
@@ -9780,7 +9783,7 @@
         <v>48</v>
       </c>
       <c r="AH68" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="AI68">
         <v>232070</v>
@@ -10018,7 +10021,7 @@
         <v>7.7</v>
       </c>
       <c r="AH70" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="AR70">
         <v>59.72</v>
@@ -10564,7 +10567,7 @@
         <v>4.834</v>
       </c>
       <c r="AH76" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="AR76">
         <v>71.3</v>
@@ -10650,10 +10653,10 @@
         <v>0.88</v>
       </c>
       <c r="T77">
-        <v>4345</v>
+        <v>3793</v>
       </c>
       <c r="U77">
-        <v>449.777</v>
+        <v>392.636</v>
       </c>
       <c r="Z77">
         <v>2633880</v>
@@ -10680,7 +10683,7 @@
         <v>13</v>
       </c>
       <c r="AH77" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="AI77">
         <v>187508</v>
@@ -10807,11 +10810,23 @@
       <c r="Q78">
         <v>1.1</v>
       </c>
+      <c r="R78">
+        <v>0</v>
+      </c>
+      <c r="S78">
+        <v>0</v>
+      </c>
+      <c r="T78">
+        <v>17</v>
+      </c>
+      <c r="U78">
+        <v>49.817</v>
+      </c>
       <c r="X78">
-        <v>0.956</v>
+        <v>3.824</v>
       </c>
       <c r="Y78">
-        <v>2.801</v>
+        <v>11.205</v>
       </c>
       <c r="Z78">
         <v>259951</v>
@@ -10838,7 +10853,7 @@
         <v>242.8</v>
       </c>
       <c r="AH78" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="AI78">
         <v>15522</v>
@@ -10987,7 +11002,7 @@
         <v>55.2</v>
       </c>
       <c r="AH79" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="AI79">
         <v>2355979</v>
@@ -11130,7 +11145,7 @@
         <v>3.5</v>
       </c>
       <c r="AH80" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="AI80">
         <v>373786</v>
@@ -11311,7 +11326,7 @@
         <v>8.699999999999999</v>
       </c>
       <c r="AH82" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="AR82">
         <v>72.69</v>
@@ -11436,7 +11451,7 @@
         <v>40.2</v>
       </c>
       <c r="AH83" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="AR83">
         <v>53.7</v>
@@ -11534,28 +11549,28 @@
         <v>1.25</v>
       </c>
       <c r="R84">
-        <v>196</v>
+        <v>221</v>
       </c>
       <c r="S84">
-        <v>39.694</v>
+        <v>44.757</v>
       </c>
       <c r="T84">
-        <v>1923</v>
+        <v>1914</v>
       </c>
       <c r="U84">
-        <v>389.445</v>
+        <v>387.622</v>
       </c>
       <c r="V84">
-        <v>59.404</v>
+        <v>66.452</v>
       </c>
       <c r="W84">
-        <v>12.03</v>
+        <v>13.458</v>
       </c>
       <c r="X84">
-        <v>900.117</v>
+        <v>840.713</v>
       </c>
       <c r="Y84">
-        <v>182.291</v>
+        <v>170.261</v>
       </c>
       <c r="Z84">
         <v>2973658</v>
@@ -11582,7 +11597,7 @@
         <v>11.1</v>
       </c>
       <c r="AH84" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="AI84">
         <v>161500</v>
@@ -11665,7 +11680,7 @@
         <v>340</v>
       </c>
       <c r="D85" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="E85">
         <v>628895</v>
@@ -11707,28 +11722,28 @@
         <v>1.2</v>
       </c>
       <c r="R85">
-        <v>399</v>
+        <v>420</v>
       </c>
       <c r="S85">
-        <v>46.098</v>
+        <v>48.524</v>
       </c>
       <c r="T85">
-        <v>1822</v>
+        <v>1772</v>
       </c>
       <c r="U85">
-        <v>210.501</v>
+        <v>204.724</v>
       </c>
       <c r="V85">
-        <v>1195</v>
+        <v>1115</v>
       </c>
       <c r="W85">
-        <v>138.062</v>
+        <v>128.819</v>
       </c>
       <c r="X85">
-        <v>1949</v>
+        <v>1817</v>
       </c>
       <c r="Y85">
-        <v>225.174</v>
+        <v>209.923</v>
       </c>
       <c r="Z85">
         <v>10857373</v>
@@ -11755,7 +11770,7 @@
         <v>10.1</v>
       </c>
       <c r="AH85" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="AI85">
         <v>4347206</v>
@@ -11883,22 +11898,22 @@
         <v>1</v>
       </c>
       <c r="R86">
-        <v>2503</v>
+        <v>2400</v>
       </c>
       <c r="S86">
-        <v>41.398</v>
+        <v>39.694</v>
       </c>
       <c r="T86">
-        <v>25260</v>
+        <v>23709</v>
       </c>
       <c r="U86">
-        <v>417.784</v>
+        <v>392.132</v>
       </c>
       <c r="X86">
-        <v>3871.549</v>
+        <v>3663.197</v>
       </c>
       <c r="Y86">
-        <v>64.033</v>
+        <v>60.587</v>
       </c>
       <c r="Z86">
         <v>31317253</v>
@@ -11925,7 +11940,7 @@
         <v>19.9</v>
       </c>
       <c r="AH86" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="AI86">
         <v>1653027</v>
@@ -12077,7 +12092,7 @@
         <v>9.4</v>
       </c>
       <c r="AH87" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="AR87">
         <v>71.3</v>
@@ -12202,7 +12217,7 @@
         <v>15.1</v>
       </c>
       <c r="AH88" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="AR88">
         <v>53.24</v>
@@ -12324,7 +12339,7 @@
         <v>24.5</v>
       </c>
       <c r="AH89" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="AR89">
         <v>81.48</v>
@@ -12538,7 +12553,7 @@
         <v>39.1</v>
       </c>
       <c r="AH91" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="AR91">
         <v>59.26</v>
@@ -12734,7 +12749,7 @@
         <v>18.6</v>
       </c>
       <c r="AH93" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="AR93">
         <v>62.96</v>
@@ -13019,22 +13034,22 @@
         <v>1.12</v>
       </c>
       <c r="T96">
-        <v>1136</v>
+        <v>1109</v>
       </c>
       <c r="U96">
-        <v>602.268</v>
+        <v>587.954</v>
       </c>
       <c r="V96">
-        <v>148.344</v>
+        <v>158.169</v>
       </c>
       <c r="W96">
-        <v>78.64700000000001</v>
+        <v>83.85599999999999</v>
       </c>
       <c r="X96">
-        <v>794.772</v>
+        <v>734.845</v>
       </c>
       <c r="Y96">
-        <v>421.361</v>
+        <v>389.59</v>
       </c>
       <c r="Z96">
         <v>1136011</v>
@@ -13061,7 +13076,7 @@
         <v>13.4</v>
       </c>
       <c r="AH96" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="AI96">
         <v>21355</v>
@@ -13477,7 +13492,7 @@
         <v>0.51</v>
       </c>
       <c r="AH100" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="AR100">
         <v>76.84999999999999</v>
@@ -13640,22 +13655,22 @@
         <v>0.83</v>
       </c>
       <c r="T102">
-        <v>1910</v>
+        <v>1432</v>
       </c>
       <c r="U102">
-        <v>701.615</v>
+        <v>526.028</v>
       </c>
       <c r="V102">
-        <v>95.479</v>
+        <v>104.247</v>
       </c>
       <c r="W102">
-        <v>35.073</v>
+        <v>38.294</v>
       </c>
       <c r="X102">
-        <v>514.415</v>
+        <v>510.518</v>
       </c>
       <c r="Y102">
-        <v>188.964</v>
+        <v>187.532</v>
       </c>
       <c r="Z102">
         <v>1890518</v>
@@ -13682,7 +13697,7 @@
         <v>6.5</v>
       </c>
       <c r="AH102" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="AI102">
         <v>76387</v>
@@ -13810,16 +13825,16 @@
         <v>0.87</v>
       </c>
       <c r="R103">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="S103">
-        <v>31.95</v>
+        <v>22.365</v>
       </c>
       <c r="T103">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="U103">
-        <v>140.58</v>
+        <v>113.423</v>
       </c>
       <c r="Z103">
         <v>1853881</v>
@@ -13846,7 +13861,7 @@
         <v>55.2</v>
       </c>
       <c r="AH103" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="AI103">
         <v>10449</v>
@@ -13992,7 +14007,7 @@
         <v>9.9</v>
       </c>
       <c r="AH104" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="AR104">
         <v>37.04</v>
@@ -14108,7 +14123,7 @@
         <v>2.9</v>
       </c>
       <c r="AH105" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="AR105">
         <v>51.85</v>
@@ -14236,7 +14251,7 @@
         <v>17</v>
       </c>
       <c r="AH106" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="AR106">
         <v>77.31</v>
@@ -14361,7 +14376,7 @@
         <v>37.3</v>
       </c>
       <c r="AH107" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="AS107">
         <v>540542</v>
@@ -14554,10 +14569,10 @@
         <v>1.16</v>
       </c>
       <c r="X109">
-        <v>42.941</v>
+        <v>18.787</v>
       </c>
       <c r="Y109">
-        <v>97.253</v>
+        <v>42.548</v>
       </c>
       <c r="Z109">
         <v>577450</v>
@@ -14584,7 +14599,7 @@
         <v>20.3</v>
       </c>
       <c r="AH109" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="AI109">
         <v>23512</v>
@@ -14795,7 +14810,7 @@
         <v>23.4</v>
       </c>
       <c r="AH111" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="AR111">
         <v>58.33</v>
@@ -15012,7 +15027,7 @@
         <v>2.5</v>
       </c>
       <c r="AH113" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="AI113">
         <v>656044</v>
@@ -15410,7 +15425,7 @@
         <v>897.3</v>
       </c>
       <c r="AH117" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="AR117">
         <v>73.61</v>
@@ -15633,7 +15648,7 @@
         <v>14.8</v>
       </c>
       <c r="AH119" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="AR119">
         <v>76.84999999999999</v>
@@ -15758,7 +15773,7 @@
         <v>3.5</v>
       </c>
       <c r="AH120" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="AR120">
         <v>64.81</v>
@@ -15886,7 +15901,7 @@
         <v>48.9</v>
       </c>
       <c r="AH121" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="AI121">
         <v>3800</v>
@@ -16029,7 +16044,7 @@
         <v>7.1</v>
       </c>
       <c r="AH122" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="AR122">
         <v>46.3</v>
@@ -16154,7 +16169,7 @@
         <v>14.8</v>
       </c>
       <c r="AH123" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="AR123">
         <v>60.19</v>
@@ -16258,28 +16273,28 @@
         <v>0.85</v>
       </c>
       <c r="R124">
-        <v>676</v>
+        <v>680</v>
       </c>
       <c r="S124">
-        <v>39.452</v>
+        <v>39.685</v>
       </c>
       <c r="T124">
-        <v>1708</v>
+        <v>1667</v>
       </c>
       <c r="U124">
-        <v>99.68000000000001</v>
+        <v>97.28700000000001</v>
       </c>
       <c r="V124">
-        <v>236.963</v>
+        <v>233.989</v>
       </c>
       <c r="W124">
-        <v>13.829</v>
+        <v>13.656</v>
       </c>
       <c r="X124">
-        <v>1336.511</v>
+        <v>1253.227</v>
       </c>
       <c r="Y124">
-        <v>77.999</v>
+        <v>73.139</v>
       </c>
       <c r="Z124">
         <v>5921923</v>
@@ -16300,7 +16315,7 @@
         <v>9.6</v>
       </c>
       <c r="AH124" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="AI124">
         <v>203450</v>
@@ -16437,7 +16452,7 @@
         <v>873.3</v>
       </c>
       <c r="AH125" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="AR125">
         <v>22.22</v>
@@ -16752,7 +16767,7 @@
         <v>8.9</v>
       </c>
       <c r="AH128" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="AR128">
         <v>58.33</v>
@@ -16874,7 +16889,7 @@
         <v>7.3</v>
       </c>
       <c r="AH129" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="AS129">
         <v>2083380</v>
@@ -16966,22 +16981,22 @@
         <v>1.01</v>
       </c>
       <c r="T130">
-        <v>158</v>
+        <v>135</v>
       </c>
       <c r="U130">
-        <v>29.145</v>
+        <v>24.902</v>
       </c>
       <c r="V130">
-        <v>14.244</v>
+        <v>10.175</v>
       </c>
       <c r="W130">
-        <v>2.628</v>
+        <v>1.877</v>
       </c>
       <c r="X130">
-        <v>91.571</v>
+        <v>87.502</v>
       </c>
       <c r="Y130">
-        <v>16.891</v>
+        <v>16.14</v>
       </c>
       <c r="Z130">
         <v>3310107</v>
@@ -17008,7 +17023,7 @@
         <v>47.6</v>
       </c>
       <c r="AH130" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="AI130">
         <v>83883</v>
@@ -17285,7 +17300,7 @@
         <v>22.1</v>
       </c>
       <c r="AH132" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="AR132">
         <v>57.87</v>
@@ -17407,7 +17422,7 @@
         <v>8.1</v>
       </c>
       <c r="AH133" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="AR133">
         <v>78.7</v>
@@ -17523,7 +17538,7 @@
         <v>6.5</v>
       </c>
       <c r="AH134" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="AI134">
         <v>6420</v>
@@ -17755,7 +17770,7 @@
         <v>3.2</v>
       </c>
       <c r="AH136" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="AR136">
         <v>55.56</v>
@@ -17978,7 +17993,7 @@
         <v>19</v>
       </c>
       <c r="AH138" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="AR138">
         <v>63.43</v>
@@ -18079,10 +18094,16 @@
         <v>0.97</v>
       </c>
       <c r="T139">
-        <v>15588</v>
+        <v>14377</v>
       </c>
       <c r="U139">
-        <v>411.873</v>
+        <v>379.876</v>
+      </c>
+      <c r="X139">
+        <v>66.777</v>
+      </c>
+      <c r="Y139">
+        <v>1.764</v>
       </c>
       <c r="Z139">
         <v>8140873</v>
@@ -18109,7 +18130,7 @@
         <v>7.1</v>
       </c>
       <c r="AH139" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="AI139">
         <v>1008253</v>
@@ -18234,22 +18255,22 @@
         <v>1.35</v>
       </c>
       <c r="R140">
-        <v>647</v>
+        <v>742</v>
       </c>
       <c r="S140">
-        <v>63.452</v>
+        <v>72.76900000000001</v>
       </c>
       <c r="T140">
-        <v>4889</v>
+        <v>6117</v>
       </c>
       <c r="U140">
-        <v>479.469</v>
+        <v>599.9</v>
       </c>
       <c r="X140">
-        <v>549.692</v>
+        <v>606.249</v>
       </c>
       <c r="Y140">
-        <v>53.909</v>
+        <v>59.455</v>
       </c>
       <c r="Z140">
         <v>6956898</v>
@@ -18276,7 +18297,7 @@
         <v>5.2</v>
       </c>
       <c r="AH140" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="AI140">
         <v>296004</v>
@@ -18428,7 +18449,7 @@
         <v>18.5</v>
       </c>
       <c r="AH141" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="AR141">
         <v>56.48</v>
@@ -18526,16 +18547,16 @@
         <v>0.95</v>
       </c>
       <c r="R142">
-        <v>1076</v>
+        <v>1020</v>
       </c>
       <c r="S142">
-        <v>55.932</v>
+        <v>53.021</v>
       </c>
       <c r="X142">
-        <v>8379.004999999999</v>
+        <v>4713.686</v>
       </c>
       <c r="Y142">
-        <v>435.552</v>
+        <v>245.024</v>
       </c>
       <c r="Z142">
         <v>5354600</v>
@@ -18562,7 +18583,7 @@
         <v>7.7</v>
       </c>
       <c r="AH142" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="AI142">
         <v>609396</v>
@@ -18714,7 +18735,7 @@
         <v>19.1</v>
       </c>
       <c r="AH143" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="AR143">
         <v>50.46</v>
@@ -18839,7 +18860,7 @@
         <v>17.3</v>
       </c>
       <c r="AH144" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="AR144">
         <v>35.19</v>
@@ -19438,7 +19459,7 @@
         <v>206.1</v>
       </c>
       <c r="AH151" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="AI151">
         <v>295530</v>
@@ -19572,7 +19593,7 @@
         <v>8.4</v>
       </c>
       <c r="AH152" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="AR152">
         <v>50.46</v>
@@ -19697,7 +19718,7 @@
         <v>6.2</v>
       </c>
       <c r="AH153" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="AI153">
         <v>361830</v>
@@ -20039,7 +20060,7 @@
         <v>1129.8</v>
       </c>
       <c r="AH156" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="AI156">
         <v>113050</v>
@@ -20161,10 +20182,10 @@
         <v>1.06</v>
       </c>
       <c r="T157">
-        <v>3164</v>
+        <v>3078</v>
       </c>
       <c r="U157">
-        <v>579.525</v>
+        <v>563.773</v>
       </c>
       <c r="Z157">
         <v>1723941</v>
@@ -20191,7 +20212,7 @@
         <v>7.2</v>
       </c>
       <c r="AH157" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="AI157">
         <v>115399</v>
@@ -20319,28 +20340,28 @@
         <v>1.05</v>
       </c>
       <c r="R158">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="S158">
-        <v>91.874</v>
+        <v>91.393</v>
       </c>
       <c r="T158">
-        <v>1220</v>
+        <v>1149</v>
       </c>
       <c r="U158">
-        <v>586.84</v>
+        <v>552.688</v>
       </c>
       <c r="V158">
-        <v>106.898</v>
+        <v>102.902</v>
       </c>
       <c r="W158">
-        <v>51.42</v>
+        <v>49.498</v>
       </c>
       <c r="X158">
-        <v>747.29</v>
+        <v>695.3390000000001</v>
       </c>
       <c r="Y158">
-        <v>359.458</v>
+        <v>334.469</v>
       </c>
       <c r="Z158">
         <v>996753</v>
@@ -20367,7 +20388,7 @@
         <v>10</v>
       </c>
       <c r="AH158" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="AI158">
         <v>64972</v>
@@ -20682,7 +20703,7 @@
         <v>5.4</v>
       </c>
       <c r="AH161" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="AR161">
         <v>56.48</v>
@@ -20810,7 +20831,7 @@
         <v>102.4</v>
       </c>
       <c r="AH162" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="AR162">
         <v>63.89</v>
@@ -20935,7 +20956,7 @@
         <v>26.5</v>
       </c>
       <c r="AH163" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="AR163">
         <v>41.67</v>
@@ -21020,17 +21041,29 @@
       <c r="Q164">
         <v>1.51</v>
       </c>
+      <c r="R164">
+        <v>3583</v>
+      </c>
+      <c r="S164">
+        <v>76.634</v>
+      </c>
+      <c r="T164">
+        <v>25228</v>
+      </c>
+      <c r="U164">
+        <v>539.581</v>
+      </c>
       <c r="V164">
-        <v>136.468</v>
+        <v>115.55</v>
       </c>
       <c r="W164">
-        <v>2.919</v>
+        <v>2.471</v>
       </c>
       <c r="X164">
-        <v>3078.996</v>
+        <v>3480.431</v>
       </c>
       <c r="Y164">
-        <v>65.854</v>
+        <v>74.44</v>
       </c>
       <c r="Z164">
         <v>26433920</v>
@@ -21051,7 +21084,7 @@
         <v>6.5</v>
       </c>
       <c r="AH164" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="AI164">
         <v>1356461</v>
@@ -21203,7 +21236,7 @@
         <v>21.5</v>
       </c>
       <c r="AH165" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="AR165">
         <v>81.94</v>
@@ -21452,7 +21485,7 @@
         <v>423</v>
       </c>
       <c r="D168" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="E168">
         <v>564557</v>
@@ -21494,22 +21527,22 @@
         <v>1.3</v>
       </c>
       <c r="R168">
-        <v>354</v>
+        <v>303</v>
       </c>
       <c r="S168">
-        <v>35.052</v>
+        <v>30.002</v>
       </c>
       <c r="T168">
-        <v>2531</v>
+        <v>2127</v>
       </c>
       <c r="U168">
-        <v>250.612</v>
+        <v>210.609</v>
       </c>
       <c r="V168">
-        <v>139.196</v>
+        <v>110.567</v>
       </c>
       <c r="W168">
-        <v>13.783</v>
+        <v>10.948</v>
       </c>
       <c r="AI168">
         <v>190096</v>
@@ -21658,7 +21691,7 @@
         <v>10.2</v>
       </c>
       <c r="AH169" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="AI169">
         <v>197368</v>
@@ -21872,7 +21905,7 @@
         <v>392</v>
       </c>
       <c r="AH171" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="AR171">
         <v>19.44</v>
@@ -22353,7 +22386,7 @@
         <v>21.6</v>
       </c>
       <c r="AH176" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="AR176">
         <v>37.5</v>
@@ -22481,7 +22514,7 @@
         <v>33.3</v>
       </c>
       <c r="AH177" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="AR177">
         <v>68.52</v>
@@ -22701,7 +22734,7 @@
         <v>26.5</v>
       </c>
       <c r="AH179" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="AI179">
         <v>1697575</v>
@@ -22841,7 +22874,7 @@
         <v>16.5</v>
       </c>
       <c r="AH180" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="AR180">
         <v>51.85</v>
@@ -22969,7 +23002,7 @@
         <v>4.5</v>
       </c>
       <c r="AH181" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="AR181">
         <v>54.63</v>
@@ -23094,7 +23127,7 @@
         <v>46.8</v>
       </c>
       <c r="AH182" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="AI182">
         <v>2868650</v>
@@ -23219,22 +23252,22 @@
         <v>1.04</v>
       </c>
       <c r="R183">
-        <v>3960</v>
+        <v>3937</v>
       </c>
       <c r="S183">
-        <v>58.333</v>
+        <v>57.994</v>
       </c>
       <c r="T183">
-        <v>38562</v>
+        <v>36931</v>
       </c>
       <c r="U183">
-        <v>568.0410000000001</v>
+        <v>544.015</v>
       </c>
       <c r="X183">
-        <v>28394</v>
+        <v>25365</v>
       </c>
       <c r="Y183">
-        <v>418.26</v>
+        <v>373.641</v>
       </c>
       <c r="Z183">
         <v>66422967</v>
@@ -23261,7 +23294,7 @@
         <v>17.2</v>
       </c>
       <c r="AH183" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="AI183">
         <v>7923497</v>
@@ -23389,28 +23422,28 @@
         <v>0.99</v>
       </c>
       <c r="R184">
-        <v>22008</v>
+        <v>20113</v>
       </c>
       <c r="S184">
-        <v>66.489</v>
+        <v>60.764</v>
       </c>
       <c r="T184">
-        <v>116264</v>
+        <v>104303</v>
       </c>
       <c r="U184">
-        <v>351.248</v>
+        <v>315.112</v>
       </c>
       <c r="V184">
-        <v>1158</v>
+        <v>1067</v>
       </c>
       <c r="W184">
-        <v>3.498</v>
+        <v>3.224</v>
       </c>
       <c r="X184">
-        <v>27012</v>
+        <v>28089</v>
       </c>
       <c r="Y184">
-        <v>81.607</v>
+        <v>84.86</v>
       </c>
       <c r="Z184">
         <v>283521441</v>
@@ -23431,7 +23464,7 @@
         <v>4.072</v>
       </c>
       <c r="AH184" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="AI184">
         <v>24652634</v>
@@ -23583,7 +23616,7 @@
         <v>9.4</v>
       </c>
       <c r="AH185" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="AR185">
         <v>64.81</v>
@@ -24340,7 +24373,7 @@
         <v>8.800000000000001</v>
       </c>
       <c r="AH193" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="AR193">
         <v>49.07</v>
@@ -24468,7 +24501,7 @@
         <v>6.5</v>
       </c>
       <c r="AH194" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="AR194">
         <v>87.04000000000001</v>

</xml_diff>

<commit_message>
Weekly hospital & ICU update
</commit_message>
<xml_diff>
--- a/public/data/latest/owid-covid-latest.xlsx
+++ b/public/data/latest/owid-covid-latest.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="945" uniqueCount="454">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="945" uniqueCount="455">
   <si>
     <t>iso_code</t>
   </si>
@@ -1364,6 +1364,9 @@
   </si>
   <si>
     <t>2021-02-04</t>
+  </si>
+  <si>
+    <t>2021-02-05</t>
   </si>
   <si>
     <t>tests performed</t>
@@ -2113,7 +2116,7 @@
         <v>4</v>
       </c>
       <c r="AH4" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AR4">
         <v>60.19</v>
@@ -2348,7 +2351,7 @@
         <v>11.3</v>
       </c>
       <c r="AH6" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="AI6">
         <v>1036</v>
@@ -2648,7 +2651,7 @@
         <v>3.8</v>
       </c>
       <c r="AH9" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="AI9">
         <v>444018</v>
@@ -2924,7 +2927,7 @@
         <v>5588.5</v>
       </c>
       <c r="AH12" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AR12">
         <v>75.45999999999999</v>
@@ -3025,16 +3028,16 @@
         <v>0.96</v>
       </c>
       <c r="R13">
-        <v>323</v>
+        <v>297</v>
       </c>
       <c r="S13">
-        <v>35.863</v>
+        <v>32.977</v>
       </c>
       <c r="T13">
-        <v>1518</v>
+        <v>1387</v>
       </c>
       <c r="U13">
-        <v>168.547</v>
+        <v>154.002</v>
       </c>
       <c r="Z13">
         <v>81397</v>
@@ -3055,7 +3058,7 @@
         <v>10.423</v>
       </c>
       <c r="AH13" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AI13">
         <v>238241</v>
@@ -3400,7 +3403,7 @@
         <v>24.7</v>
       </c>
       <c r="AH16" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="AI16">
         <v>177233</v>
@@ -3543,7 +3546,7 @@
         <v>29.4</v>
       </c>
       <c r="AH17" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AI17">
         <v>567</v>
@@ -3784,7 +3787,7 @@
         <v>9.6</v>
       </c>
       <c r="AH19" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AR19">
         <v>27.78</v>
@@ -3882,28 +3885,22 @@
         <v>1.08</v>
       </c>
       <c r="R20">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="S20">
-        <v>27.783</v>
+        <v>27.18</v>
       </c>
       <c r="T20">
-        <v>1923</v>
+        <v>1788</v>
       </c>
       <c r="U20">
-        <v>165.924</v>
-      </c>
-      <c r="V20">
-        <v>2420</v>
-      </c>
-      <c r="W20">
-        <v>208.808</v>
+        <v>154.276</v>
       </c>
       <c r="X20">
-        <v>967.191</v>
+        <v>812.4</v>
       </c>
       <c r="Y20">
-        <v>83.453</v>
+        <v>70.09699999999999</v>
       </c>
       <c r="Z20">
         <v>43266</v>
@@ -3930,7 +3927,7 @@
         <v>18.2</v>
       </c>
       <c r="AH20" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AI20">
         <v>351513</v>
@@ -4272,7 +4269,7 @@
         <v>13988.3</v>
       </c>
       <c r="AH23" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="AR23">
         <v>69.91</v>
@@ -4394,7 +4391,7 @@
         <v>3.1</v>
       </c>
       <c r="AH24" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AI24">
         <v>3560</v>
@@ -4531,7 +4528,7 @@
         <v>8.300000000000001</v>
       </c>
       <c r="AH25" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AR25">
         <v>42.59</v>
@@ -4944,16 +4941,16 @@
         <v>0.83</v>
       </c>
       <c r="R29">
-        <v>281</v>
+        <v>263</v>
       </c>
       <c r="S29">
-        <v>40.441</v>
+        <v>37.85</v>
       </c>
       <c r="T29">
-        <v>2857</v>
+        <v>2866</v>
       </c>
       <c r="U29">
-        <v>411.171</v>
+        <v>412.466</v>
       </c>
       <c r="Z29">
         <v>11452</v>
@@ -4980,7 +4977,7 @@
         <v>17.6</v>
       </c>
       <c r="AH29" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AI29">
         <v>54025</v>
@@ -5485,16 +5482,16 @@
         <v>0.92</v>
       </c>
       <c r="R34">
-        <v>834</v>
+        <v>737</v>
       </c>
       <c r="S34">
-        <v>22.097</v>
+        <v>19.527</v>
       </c>
       <c r="T34">
-        <v>3975</v>
+        <v>3432</v>
       </c>
       <c r="U34">
-        <v>105.32</v>
+        <v>90.93300000000001</v>
       </c>
       <c r="Z34">
         <v>50138</v>
@@ -5521,7 +5518,7 @@
         <v>14.2</v>
       </c>
       <c r="AH34" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="AI34">
         <v>1015083</v>
@@ -5655,7 +5652,7 @@
         <v>0.849</v>
       </c>
       <c r="AH35" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AR35">
         <v>64.81</v>
@@ -5961,7 +5958,7 @@
         <v>12.7</v>
       </c>
       <c r="AH38" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AI38">
         <v>291937</v>
@@ -6226,7 +6223,7 @@
         <v>6</v>
       </c>
       <c r="AH40" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AR40">
         <v>81.02</v>
@@ -6675,7 +6672,7 @@
         <v>16.3</v>
       </c>
       <c r="AH44" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="AR44">
         <v>23.15</v>
@@ -6770,16 +6767,16 @@
         <v>0.86</v>
       </c>
       <c r="T45">
-        <v>1474</v>
+        <v>1249</v>
       </c>
       <c r="U45">
-        <v>359.051</v>
+        <v>304.243</v>
       </c>
       <c r="X45">
-        <v>825.838</v>
+        <v>627.436</v>
       </c>
       <c r="Y45">
-        <v>201.165</v>
+        <v>152.837</v>
       </c>
       <c r="Z45">
         <v>7023</v>
@@ -6806,7 +6803,7 @@
         <v>10.8</v>
       </c>
       <c r="AH45" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="AI45">
         <v>87929</v>
@@ -6955,7 +6952,7 @@
         <v>19.8</v>
       </c>
       <c r="AH46" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AR46">
         <v>83.33</v>
@@ -7053,28 +7050,28 @@
         <v>0.7</v>
       </c>
       <c r="R47">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="S47">
-        <v>39.959</v>
+        <v>36.534</v>
       </c>
       <c r="T47">
-        <v>173</v>
+        <v>140</v>
       </c>
       <c r="U47">
-        <v>197.511</v>
+        <v>159.836</v>
       </c>
       <c r="V47">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="W47">
-        <v>17.125</v>
+        <v>19.409</v>
       </c>
       <c r="X47">
-        <v>86</v>
+        <v>62</v>
       </c>
       <c r="Y47">
-        <v>98.185</v>
+        <v>70.78400000000001</v>
       </c>
       <c r="Z47">
         <v>27085</v>
@@ -7101,7 +7098,7 @@
         <v>172.1</v>
       </c>
       <c r="AH47" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AI47">
         <v>25168</v>
@@ -7223,28 +7220,28 @@
         <v>0.9</v>
       </c>
       <c r="R48">
-        <v>1047</v>
+        <v>954</v>
       </c>
       <c r="S48">
-        <v>97.768</v>
+        <v>89.084</v>
       </c>
       <c r="T48">
-        <v>5798</v>
+        <v>5482</v>
       </c>
       <c r="U48">
-        <v>541.415</v>
+        <v>511.907</v>
       </c>
       <c r="V48">
-        <v>1845.197</v>
+        <v>1771.792</v>
       </c>
       <c r="W48">
-        <v>172.304</v>
+        <v>165.449</v>
       </c>
       <c r="X48">
-        <v>10376.344</v>
+        <v>9654.353999999999</v>
       </c>
       <c r="Y48">
-        <v>968.938</v>
+        <v>901.519</v>
       </c>
       <c r="Z48">
         <v>56043</v>
@@ -7265,7 +7262,7 @@
         <v>7.2</v>
       </c>
       <c r="AH48" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AI48">
         <v>327759</v>
@@ -7408,7 +7405,7 @@
         <v>5</v>
       </c>
       <c r="AH49" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="AR49">
         <v>32.41</v>
@@ -7503,22 +7500,22 @@
         <v>0.76</v>
       </c>
       <c r="R50">
-        <v>124</v>
+        <v>97</v>
       </c>
       <c r="S50">
-        <v>21.408</v>
+        <v>16.747</v>
       </c>
       <c r="T50">
-        <v>725</v>
+        <v>529</v>
       </c>
       <c r="U50">
-        <v>125.168</v>
+        <v>91.33</v>
       </c>
       <c r="X50">
-        <v>607.544</v>
+        <v>380.089</v>
       </c>
       <c r="Y50">
-        <v>104.89</v>
+        <v>65.621</v>
       </c>
       <c r="Z50">
         <v>15960</v>
@@ -7545,7 +7542,7 @@
         <v>193.3</v>
       </c>
       <c r="AH50" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AI50">
         <v>298112</v>
@@ -7860,7 +7857,7 @@
         <v>4.8</v>
       </c>
       <c r="AH53" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="AR53">
         <v>70.37</v>
@@ -7982,7 +7979,7 @@
         <v>0.283</v>
       </c>
       <c r="AH54" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="AI54">
         <v>6228</v>
@@ -8226,7 +8223,7 @@
         <v>105.205</v>
       </c>
       <c r="AH56" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AR56">
         <v>47.22</v>
@@ -8514,28 +8511,28 @@
         <v>1.01</v>
       </c>
       <c r="R59">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="S59">
-        <v>33.923</v>
+        <v>28.646</v>
       </c>
       <c r="T59">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="U59">
-        <v>320.383</v>
+        <v>319.629</v>
       </c>
       <c r="V59">
-        <v>32.042</v>
+        <v>26.034</v>
       </c>
       <c r="W59">
-        <v>24.154</v>
+        <v>19.625</v>
       </c>
       <c r="X59">
-        <v>295.383</v>
+        <v>298.387</v>
       </c>
       <c r="Y59">
-        <v>222.672</v>
+        <v>224.936</v>
       </c>
       <c r="Z59">
         <v>5920</v>
@@ -8562,7 +8559,7 @@
         <v>9</v>
       </c>
       <c r="AH59" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AI59">
         <v>46194</v>
@@ -8812,7 +8809,7 @@
         <v>11</v>
       </c>
       <c r="AH61" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AR61">
         <v>46.3</v>
@@ -9016,7 +9013,7 @@
         <v>528</v>
       </c>
       <c r="AH64" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AR64">
         <v>41.67</v>
@@ -9117,16 +9114,16 @@
         <v>1.07</v>
       </c>
       <c r="R65">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="S65">
-        <v>4.332</v>
+        <v>3.61</v>
       </c>
       <c r="T65">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="U65">
-        <v>24.546</v>
+        <v>22.741</v>
       </c>
       <c r="Z65">
         <v>6767</v>
@@ -9153,7 +9150,7 @@
         <v>37.3</v>
       </c>
       <c r="AH65" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AI65">
         <v>193917</v>
@@ -9278,28 +9275,28 @@
         <v>1.17</v>
       </c>
       <c r="R66">
-        <v>2955</v>
+        <v>3148</v>
       </c>
       <c r="S66">
-        <v>45.271</v>
+        <v>48.228</v>
       </c>
       <c r="T66">
-        <v>26357</v>
+        <v>27573</v>
       </c>
       <c r="U66">
-        <v>403.793</v>
+        <v>422.422</v>
       </c>
       <c r="V66">
-        <v>1656.849</v>
+        <v>1732.825</v>
       </c>
       <c r="W66">
-        <v>25.383</v>
+        <v>26.547</v>
       </c>
       <c r="X66">
-        <v>10483.638</v>
+        <v>10425.195</v>
       </c>
       <c r="Y66">
-        <v>160.611</v>
+        <v>159.716</v>
       </c>
       <c r="Z66">
         <v>214907</v>
@@ -9320,7 +9317,7 @@
         <v>14.9</v>
       </c>
       <c r="AH66" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="AI66">
         <v>1825982</v>
@@ -9736,16 +9733,16 @@
         <v>0.92</v>
       </c>
       <c r="R70">
-        <v>4607</v>
+        <v>4337</v>
       </c>
       <c r="S70">
-        <v>54.987</v>
+        <v>51.764</v>
       </c>
       <c r="X70">
-        <v>2510.918</v>
+        <v>2044.663</v>
       </c>
       <c r="Y70">
-        <v>29.969</v>
+        <v>24.404</v>
       </c>
       <c r="AA70">
         <v>38471483</v>
@@ -9766,7 +9763,7 @@
         <v>10</v>
       </c>
       <c r="AH70" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AI70">
         <v>2987398</v>
@@ -9915,7 +9912,7 @@
         <v>6.4</v>
       </c>
       <c r="AH71" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="AR71">
         <v>38.89</v>
@@ -10019,10 +10016,10 @@
         <v>0.89</v>
       </c>
       <c r="V72">
-        <v>87.46899999999999</v>
+        <v>65.116</v>
       </c>
       <c r="W72">
-        <v>8.391999999999999</v>
+        <v>6.247</v>
       </c>
       <c r="Z72">
         <v>37591</v>
@@ -10049,7 +10046,7 @@
         <v>38.5</v>
       </c>
       <c r="AH72" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="AI72">
         <v>359723</v>
@@ -10287,7 +10284,7 @@
         <v>9.5</v>
       </c>
       <c r="AH74" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="AR74">
         <v>51.39</v>
@@ -10860,10 +10857,10 @@
         <v>0.82</v>
       </c>
       <c r="T80">
-        <v>3793</v>
+        <v>3562</v>
       </c>
       <c r="U80">
-        <v>392.636</v>
+        <v>368.724</v>
       </c>
       <c r="Z80">
         <v>15434</v>
@@ -10890,7 +10887,7 @@
         <v>13</v>
       </c>
       <c r="AH80" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AI80">
         <v>357303</v>
@@ -11018,16 +11015,16 @@
         <v>0.67</v>
       </c>
       <c r="T81">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="U81">
-        <v>49.817</v>
+        <v>46.886</v>
       </c>
       <c r="X81">
-        <v>3.824</v>
+        <v>0.956</v>
       </c>
       <c r="Y81">
-        <v>11.205</v>
+        <v>2.801</v>
       </c>
       <c r="Z81">
         <v>716</v>
@@ -11054,7 +11051,7 @@
         <v>285.2</v>
       </c>
       <c r="AH81" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AI81">
         <v>16951</v>
@@ -11203,7 +11200,7 @@
         <v>53.4</v>
       </c>
       <c r="AH82" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="AI82">
         <v>4959445</v>
@@ -11346,7 +11343,7 @@
         <v>3.5</v>
       </c>
       <c r="AH83" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="AI83">
         <v>796819</v>
@@ -11527,7 +11524,7 @@
         <v>8.300000000000001</v>
       </c>
       <c r="AH85" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AR85">
         <v>72.69</v>
@@ -11652,7 +11649,7 @@
         <v>46.9</v>
       </c>
       <c r="AH86" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="AR86">
         <v>44.44</v>
@@ -11750,28 +11747,28 @@
         <v>0.83</v>
       </c>
       <c r="R87">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="S87">
-        <v>44.757</v>
+        <v>42.732</v>
       </c>
       <c r="T87">
-        <v>1914</v>
+        <v>1515</v>
       </c>
       <c r="U87">
-        <v>387.622</v>
+        <v>306.817</v>
       </c>
       <c r="V87">
-        <v>66.452</v>
+        <v>67.458</v>
       </c>
       <c r="W87">
-        <v>13.458</v>
+        <v>13.662</v>
       </c>
       <c r="X87">
-        <v>840.713</v>
+        <v>618.201</v>
       </c>
       <c r="Y87">
-        <v>170.261</v>
+        <v>125.198</v>
       </c>
       <c r="Z87">
         <v>18190</v>
@@ -11798,7 +11795,7 @@
         <v>15.9</v>
       </c>
       <c r="AH87" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AI87">
         <v>219200</v>
@@ -11881,7 +11878,7 @@
         <v>339</v>
       </c>
       <c r="D88" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="E88">
         <v>675618</v>
@@ -11923,28 +11920,28 @@
         <v>1.04</v>
       </c>
       <c r="R88">
-        <v>420</v>
+        <v>395</v>
       </c>
       <c r="S88">
-        <v>48.524</v>
+        <v>45.636</v>
       </c>
       <c r="T88">
-        <v>1772</v>
+        <v>1668</v>
       </c>
       <c r="U88">
-        <v>204.724</v>
+        <v>192.709</v>
       </c>
       <c r="V88">
-        <v>1115</v>
+        <v>1004</v>
       </c>
       <c r="W88">
-        <v>128.819</v>
+        <v>115.995</v>
       </c>
       <c r="X88">
-        <v>1817</v>
+        <v>1594</v>
       </c>
       <c r="Y88">
-        <v>209.923</v>
+        <v>184.159</v>
       </c>
       <c r="Z88">
         <v>54737</v>
@@ -11971,7 +11968,7 @@
         <v>10.8</v>
       </c>
       <c r="AH88" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AI88">
         <v>5336910</v>
@@ -12099,22 +12096,22 @@
         <v>0.91</v>
       </c>
       <c r="R89">
-        <v>2400</v>
+        <v>2215</v>
       </c>
       <c r="S89">
-        <v>39.694</v>
+        <v>36.635</v>
       </c>
       <c r="T89">
-        <v>23709</v>
+        <v>22311</v>
       </c>
       <c r="U89">
-        <v>392.132</v>
+        <v>369.01</v>
       </c>
       <c r="X89">
-        <v>3663.197</v>
+        <v>3208.428</v>
       </c>
       <c r="Y89">
-        <v>60.587</v>
+        <v>53.065</v>
       </c>
       <c r="Z89">
         <v>244429</v>
@@ -12141,7 +12138,7 @@
         <v>20.5</v>
       </c>
       <c r="AH89" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AI89">
         <v>2335997</v>
@@ -12293,7 +12290,7 @@
         <v>8.6</v>
       </c>
       <c r="AH90" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="AR90">
         <v>71.3</v>
@@ -12418,7 +12415,7 @@
         <v>19.4</v>
       </c>
       <c r="AH91" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="AR91">
         <v>53.24</v>
@@ -12540,7 +12537,7 @@
         <v>22.9</v>
       </c>
       <c r="AH92" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AR92">
         <v>75.93000000000001</v>
@@ -12659,7 +12656,7 @@
         <v>24.8</v>
       </c>
       <c r="AH93" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AR93">
         <v>68.52</v>
@@ -12956,7 +12953,7 @@
         <v>15.5</v>
       </c>
       <c r="AH96" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AI96">
         <v>35000</v>
@@ -13253,22 +13250,22 @@
         <v>1.05</v>
       </c>
       <c r="T99">
-        <v>1109</v>
+        <v>1061</v>
       </c>
       <c r="U99">
-        <v>587.954</v>
+        <v>562.506</v>
       </c>
       <c r="V99">
-        <v>158.169</v>
+        <v>160.133</v>
       </c>
       <c r="W99">
-        <v>83.85599999999999</v>
+        <v>84.89700000000001</v>
       </c>
       <c r="X99">
-        <v>734.845</v>
+        <v>695.549</v>
       </c>
       <c r="Y99">
-        <v>389.59</v>
+        <v>368.756</v>
       </c>
       <c r="Z99">
         <v>12317</v>
@@ -13295,7 +13292,7 @@
         <v>12.2</v>
       </c>
       <c r="AH99" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AI99">
         <v>29844</v>
@@ -13708,7 +13705,7 @@
         <v>0.624</v>
       </c>
       <c r="AH103" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="AR103">
         <v>76.84999999999999</v>
@@ -13871,22 +13868,22 @@
         <v>0.93</v>
       </c>
       <c r="T105">
-        <v>1432</v>
+        <v>1346</v>
       </c>
       <c r="U105">
-        <v>526.028</v>
+        <v>494.436</v>
       </c>
       <c r="V105">
-        <v>104.247</v>
+        <v>91.581</v>
       </c>
       <c r="W105">
-        <v>38.294</v>
+        <v>33.641</v>
       </c>
       <c r="X105">
-        <v>510.518</v>
+        <v>445.242</v>
       </c>
       <c r="Y105">
-        <v>187.532</v>
+        <v>163.554</v>
       </c>
       <c r="Z105">
         <v>8028</v>
@@ -13913,7 +13910,7 @@
         <v>10</v>
       </c>
       <c r="AH105" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AI105">
         <v>114590</v>
@@ -14041,16 +14038,16 @@
         <v>0.92</v>
       </c>
       <c r="R106">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="S106">
-        <v>22.365</v>
+        <v>17.573</v>
       </c>
       <c r="T106">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="U106">
-        <v>113.423</v>
+        <v>105.435</v>
       </c>
       <c r="Z106">
         <v>10577</v>
@@ -14077,7 +14074,7 @@
         <v>50.3</v>
       </c>
       <c r="AH106" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AI106">
         <v>15407</v>
@@ -14223,7 +14220,7 @@
         <v>7.6</v>
       </c>
       <c r="AH107" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AR107">
         <v>37.04</v>
@@ -14339,7 +14336,7 @@
         <v>3.5</v>
       </c>
       <c r="AH108" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="AR108">
         <v>51.85</v>
@@ -14467,7 +14464,7 @@
         <v>11.7</v>
       </c>
       <c r="AH109" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="AR109">
         <v>77.31</v>
@@ -14592,7 +14589,7 @@
         <v>26</v>
       </c>
       <c r="AH110" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="AI110">
         <v>3204</v>
@@ -14800,10 +14797,10 @@
         <v>1</v>
       </c>
       <c r="X112">
-        <v>18.787</v>
+        <v>23.26</v>
       </c>
       <c r="Y112">
-        <v>42.548</v>
+        <v>52.679</v>
       </c>
       <c r="AI112">
         <v>31633</v>
@@ -15014,7 +15011,7 @@
         <v>23.4</v>
       </c>
       <c r="AH114" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AR114">
         <v>50.93</v>
@@ -15231,7 +15228,7 @@
         <v>2.8</v>
       </c>
       <c r="AH116" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="AI116">
         <v>695088</v>
@@ -15629,7 +15626,7 @@
         <v>423.6</v>
       </c>
       <c r="AH120" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="AR120">
         <v>73.61</v>
@@ -15852,7 +15849,7 @@
         <v>16.8</v>
       </c>
       <c r="AH122" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="AI122">
         <v>351723</v>
@@ -15992,7 +15989,7 @@
         <v>3.5</v>
       </c>
       <c r="AH123" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="AR123">
         <v>64.81</v>
@@ -16120,7 +16117,7 @@
         <v>58.6</v>
       </c>
       <c r="AH124" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="AI124">
         <v>3800</v>
@@ -16263,7 +16260,7 @@
         <v>7.6</v>
       </c>
       <c r="AH125" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="AR125">
         <v>38.89</v>
@@ -16388,7 +16385,7 @@
         <v>21.2</v>
       </c>
       <c r="AH126" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AI126">
         <v>113175</v>
@@ -16501,28 +16498,28 @@
         <v>0.88</v>
       </c>
       <c r="R127">
-        <v>680</v>
+        <v>646</v>
       </c>
       <c r="S127">
-        <v>39.685</v>
+        <v>37.701</v>
       </c>
       <c r="T127">
-        <v>1667</v>
+        <v>1573</v>
       </c>
       <c r="U127">
-        <v>97.28700000000001</v>
+        <v>91.801</v>
       </c>
       <c r="V127">
-        <v>233.989</v>
+        <v>245.886</v>
       </c>
       <c r="W127">
-        <v>13.656</v>
+        <v>14.35</v>
       </c>
       <c r="X127">
-        <v>1253.227</v>
+        <v>1205.636</v>
       </c>
       <c r="Y127">
-        <v>73.139</v>
+        <v>70.36199999999999</v>
       </c>
       <c r="AA127">
         <v>5934044</v>
@@ -16543,7 +16540,7 @@
         <v>9.699999999999999</v>
       </c>
       <c r="AH127" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="AI127">
         <v>330494</v>
@@ -16680,7 +16677,7 @@
         <v>3392.6</v>
       </c>
       <c r="AH128" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AR128">
         <v>22.22</v>
@@ -16995,7 +16992,7 @@
         <v>4.5</v>
       </c>
       <c r="AH131" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="AR131">
         <v>58.33</v>
@@ -17143,7 +17140,7 @@
         <v>6.9</v>
       </c>
       <c r="AH133" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AS133">
         <v>2083380</v>
@@ -17235,10 +17232,10 @@
         <v>0.84</v>
       </c>
       <c r="T134">
-        <v>135</v>
+        <v>90</v>
       </c>
       <c r="U134">
-        <v>24.902</v>
+        <v>16.601</v>
       </c>
       <c r="V134">
         <v>10.175</v>
@@ -17247,10 +17244,10 @@
         <v>1.877</v>
       </c>
       <c r="X134">
-        <v>87.502</v>
+        <v>42.733</v>
       </c>
       <c r="Y134">
-        <v>16.14</v>
+        <v>7.883</v>
       </c>
       <c r="Z134">
         <v>21297</v>
@@ -17277,7 +17274,7 @@
         <v>59.6</v>
       </c>
       <c r="AH134" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="AI134">
         <v>165515</v>
@@ -17580,7 +17577,7 @@
         <v>24.5</v>
       </c>
       <c r="AH137" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AR137">
         <v>50.46</v>
@@ -17702,7 +17699,7 @@
         <v>8.199999999999999</v>
       </c>
       <c r="AH138" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AR138">
         <v>78.7</v>
@@ -17818,7 +17815,7 @@
         <v>7.5</v>
       </c>
       <c r="AH139" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AI139">
         <v>6420</v>
@@ -18050,7 +18047,7 @@
         <v>4.5</v>
       </c>
       <c r="AH141" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AR141">
         <v>55.56</v>
@@ -18273,7 +18270,7 @@
         <v>18.8</v>
       </c>
       <c r="AH143" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="AR143">
         <v>63.43</v>
@@ -18374,16 +18371,16 @@
         <v>0.88</v>
       </c>
       <c r="T144">
-        <v>14377</v>
+        <v>13339</v>
       </c>
       <c r="U144">
-        <v>379.876</v>
+        <v>352.449</v>
       </c>
       <c r="X144">
-        <v>66.777</v>
+        <v>81.727</v>
       </c>
       <c r="Y144">
-        <v>1.764</v>
+        <v>2.159</v>
       </c>
       <c r="Z144">
         <v>41614</v>
@@ -18410,7 +18407,7 @@
         <v>7.4</v>
       </c>
       <c r="AH144" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="AI144">
         <v>1566604</v>
@@ -18535,22 +18532,22 @@
         <v>1.33</v>
       </c>
       <c r="R145">
-        <v>742</v>
+        <v>858</v>
       </c>
       <c r="S145">
-        <v>72.76900000000001</v>
+        <v>84.145</v>
       </c>
       <c r="T145">
-        <v>6117</v>
+        <v>6694</v>
       </c>
       <c r="U145">
-        <v>599.9</v>
+        <v>656.486</v>
       </c>
       <c r="X145">
-        <v>606.249</v>
+        <v>627.086</v>
       </c>
       <c r="Y145">
-        <v>59.455</v>
+        <v>61.499</v>
       </c>
       <c r="Z145">
         <v>45261</v>
@@ -18577,7 +18574,7 @@
         <v>4.9</v>
       </c>
       <c r="AH145" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AI145">
         <v>364211</v>
@@ -18729,7 +18726,7 @@
         <v>14.7</v>
       </c>
       <c r="AH146" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="AR146">
         <v>56.48</v>
@@ -18827,16 +18824,16 @@
         <v>0.86</v>
       </c>
       <c r="R147">
-        <v>1020</v>
+        <v>996</v>
       </c>
       <c r="S147">
-        <v>53.021</v>
+        <v>51.773</v>
       </c>
       <c r="X147">
-        <v>4713.686</v>
+        <v>8450.349</v>
       </c>
       <c r="Y147">
-        <v>245.024</v>
+        <v>439.26</v>
       </c>
       <c r="Z147">
         <v>25550</v>
@@ -18863,7 +18860,7 @@
         <v>8.300000000000001</v>
       </c>
       <c r="AH147" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AI147">
         <v>794795</v>
@@ -19015,7 +19012,7 @@
         <v>19.6</v>
       </c>
       <c r="AH148" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AR148">
         <v>50.46</v>
@@ -19140,7 +19137,7 @@
         <v>29</v>
       </c>
       <c r="AH149" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="AR149">
         <v>74.06999999999999</v>
@@ -19739,7 +19736,7 @@
         <v>185.5</v>
       </c>
       <c r="AH156" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AI156">
         <v>440618</v>
@@ -19873,7 +19870,7 @@
         <v>7.3</v>
       </c>
       <c r="AH157" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AR157">
         <v>50.46</v>
@@ -19998,7 +19995,7 @@
         <v>6.3</v>
       </c>
       <c r="AH158" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="AI158">
         <v>526930</v>
@@ -20352,7 +20349,7 @@
         <v>1135.1</v>
       </c>
       <c r="AH161" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="AI161">
         <v>181000</v>
@@ -20473,6 +20470,12 @@
       <c r="Q162">
         <v>0.95</v>
       </c>
+      <c r="T162">
+        <v>3335</v>
+      </c>
+      <c r="U162">
+        <v>610.846</v>
+      </c>
       <c r="Z162">
         <v>12313</v>
       </c>
@@ -20498,7 +20501,7 @@
         <v>4.8</v>
       </c>
       <c r="AH162" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AI162">
         <v>191327</v>
@@ -20626,28 +20629,28 @@
         <v>0.97</v>
       </c>
       <c r="R163">
-        <v>190</v>
+        <v>167</v>
       </c>
       <c r="S163">
-        <v>91.393</v>
+        <v>80.33</v>
       </c>
       <c r="T163">
-        <v>1149</v>
+        <v>1053</v>
       </c>
       <c r="U163">
-        <v>552.688</v>
+        <v>506.51</v>
       </c>
       <c r="V163">
-        <v>102.902</v>
+        <v>85.91800000000001</v>
       </c>
       <c r="W163">
-        <v>49.498</v>
+        <v>41.328</v>
       </c>
       <c r="X163">
-        <v>695.3390000000001</v>
+        <v>578.45</v>
       </c>
       <c r="Y163">
-        <v>334.469</v>
+        <v>278.244</v>
       </c>
       <c r="Z163">
         <v>37299</v>
@@ -20674,7 +20677,7 @@
         <v>11.8</v>
       </c>
       <c r="AH163" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AI163">
         <v>83335</v>
@@ -20989,7 +20992,7 @@
         <v>7.7</v>
       </c>
       <c r="AH166" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="AR166">
         <v>72.22</v>
@@ -21143,7 +21146,7 @@
         <v>94.7</v>
       </c>
       <c r="AH168" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="AR168">
         <v>63.89</v>
@@ -21262,7 +21265,7 @@
         <v>225.4</v>
       </c>
       <c r="AH169" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AR169">
         <v>43.52</v>
@@ -21347,17 +21350,29 @@
       <c r="Q170">
         <v>1.46</v>
       </c>
+      <c r="R170">
+        <v>4515</v>
+      </c>
+      <c r="S170">
+        <v>96.568</v>
+      </c>
+      <c r="T170">
+        <v>30789</v>
+      </c>
+      <c r="U170">
+        <v>658.521</v>
+      </c>
       <c r="V170">
-        <v>115.55</v>
+        <v>128.499</v>
       </c>
       <c r="W170">
-        <v>2.471</v>
+        <v>2.748</v>
       </c>
       <c r="X170">
-        <v>3480.431</v>
+        <v>2756.255</v>
       </c>
       <c r="Y170">
-        <v>74.44</v>
+        <v>58.951</v>
       </c>
       <c r="AA170">
         <v>28228026</v>
@@ -21378,7 +21393,7 @@
         <v>7.1</v>
       </c>
       <c r="AH170" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AI170">
         <v>1865342</v>
@@ -21530,7 +21545,7 @@
         <v>18.6</v>
       </c>
       <c r="AH171" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AI171">
         <v>139914</v>
@@ -21836,22 +21851,22 @@
         <v>1.25</v>
       </c>
       <c r="R174">
-        <v>303</v>
+        <v>260</v>
       </c>
       <c r="S174">
-        <v>30.002</v>
+        <v>25.744</v>
       </c>
       <c r="T174">
-        <v>2127</v>
+        <v>1830</v>
       </c>
       <c r="U174">
-        <v>210.609</v>
+        <v>181.201</v>
       </c>
       <c r="V174">
-        <v>110.567</v>
+        <v>91.81</v>
       </c>
       <c r="W174">
-        <v>10.948</v>
+        <v>9.090999999999999</v>
       </c>
       <c r="Z174">
         <v>26885</v>
@@ -21872,7 +21887,7 @@
         <v>9.1</v>
       </c>
       <c r="AH174" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AI174">
         <v>320378</v>
@@ -22024,7 +22039,7 @@
         <v>11.8</v>
       </c>
       <c r="AH175" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AI175">
         <v>315033</v>
@@ -22238,7 +22253,7 @@
         <v>473.5</v>
       </c>
       <c r="AH177" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="AR177">
         <v>19.44</v>
@@ -22719,7 +22734,7 @@
         <v>16.5</v>
       </c>
       <c r="AH182" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AR182">
         <v>37.5</v>
@@ -22847,7 +22862,7 @@
         <v>60.5</v>
       </c>
       <c r="AH183" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="AR183">
         <v>68.52</v>
@@ -23067,7 +23082,7 @@
         <v>21.4</v>
       </c>
       <c r="AH185" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AI185">
         <v>2500806</v>
@@ -23207,7 +23222,7 @@
         <v>32</v>
       </c>
       <c r="AH186" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="AR186">
         <v>49.07</v>
@@ -23335,7 +23350,7 @@
         <v>5.2</v>
       </c>
       <c r="AH187" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AR187">
         <v>54.63</v>
@@ -23460,7 +23475,7 @@
         <v>49</v>
       </c>
       <c r="AH188" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AI188">
         <v>3849374</v>
@@ -23585,22 +23600,22 @@
         <v>0.91</v>
       </c>
       <c r="R189">
-        <v>3937</v>
+        <v>3625</v>
       </c>
       <c r="S189">
-        <v>57.994</v>
+        <v>53.398</v>
       </c>
       <c r="T189">
-        <v>36931</v>
+        <v>31670</v>
       </c>
       <c r="U189">
-        <v>544.015</v>
+        <v>466.517</v>
       </c>
       <c r="X189">
-        <v>25365</v>
+        <v>19585</v>
       </c>
       <c r="Y189">
-        <v>373.641</v>
+        <v>288.498</v>
       </c>
       <c r="Z189">
         <v>606382</v>
@@ -23627,7 +23642,7 @@
         <v>28.1</v>
       </c>
       <c r="AH189" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AI189">
         <v>10992444</v>
@@ -23755,28 +23770,28 @@
         <v>0.9</v>
       </c>
       <c r="R190">
-        <v>20113</v>
+        <v>17918</v>
       </c>
       <c r="S190">
-        <v>60.764</v>
+        <v>54.132</v>
       </c>
       <c r="T190">
-        <v>104303</v>
+        <v>88668</v>
       </c>
       <c r="U190">
-        <v>315.112</v>
+        <v>267.877</v>
       </c>
       <c r="V190">
-        <v>1067</v>
+        <v>1003</v>
       </c>
       <c r="W190">
-        <v>3.224</v>
+        <v>3.03</v>
       </c>
       <c r="X190">
-        <v>28089</v>
+        <v>22007</v>
       </c>
       <c r="Y190">
-        <v>84.86</v>
+        <v>66.486</v>
       </c>
       <c r="Z190">
         <v>939538</v>
@@ -23797,7 +23812,7 @@
         <v>3.809</v>
       </c>
       <c r="AH190" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AI190">
         <v>35203710</v>
@@ -23943,7 +23958,7 @@
         <v>11.5</v>
       </c>
       <c r="AH191" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AR191">
         <v>64.81</v>
@@ -24700,7 +24715,7 @@
         <v>8.1</v>
       </c>
       <c r="AH199" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AR199">
         <v>49.07</v>
@@ -24828,7 +24843,7 @@
         <v>12.4</v>
       </c>
       <c r="AH200" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AR200">
         <v>84.26000000000001</v>

</xml_diff>

<commit_message>
Update complete dataset with hospital & ICU data
</commit_message>
<xml_diff>
--- a/public/data/latest/owid-covid-latest.xlsx
+++ b/public/data/latest/owid-covid-latest.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="945" uniqueCount="454">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="945" uniqueCount="455">
   <si>
     <t>iso_code</t>
   </si>
@@ -1364,6 +1364,9 @@
   </si>
   <si>
     <t>2021-02-04</t>
+  </si>
+  <si>
+    <t>2021-02-05</t>
   </si>
   <si>
     <t>tests performed</t>
@@ -2113,7 +2116,7 @@
         <v>4</v>
       </c>
       <c r="AH4" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AR4">
         <v>60.19</v>
@@ -2348,7 +2351,7 @@
         <v>11.3</v>
       </c>
       <c r="AH6" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="AI6">
         <v>1036</v>
@@ -2648,7 +2651,7 @@
         <v>3.8</v>
       </c>
       <c r="AH9" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="AI9">
         <v>444018</v>
@@ -2924,7 +2927,7 @@
         <v>5588.5</v>
       </c>
       <c r="AH12" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AR12">
         <v>75.45999999999999</v>
@@ -3025,16 +3028,16 @@
         <v>0.96</v>
       </c>
       <c r="R13">
-        <v>323</v>
+        <v>297</v>
       </c>
       <c r="S13">
-        <v>35.863</v>
+        <v>32.977</v>
       </c>
       <c r="T13">
-        <v>1518</v>
+        <v>1387</v>
       </c>
       <c r="U13">
-        <v>168.547</v>
+        <v>154.002</v>
       </c>
       <c r="Z13">
         <v>81397</v>
@@ -3055,7 +3058,7 @@
         <v>10.423</v>
       </c>
       <c r="AH13" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AI13">
         <v>238241</v>
@@ -3400,7 +3403,7 @@
         <v>24.7</v>
       </c>
       <c r="AH16" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="AI16">
         <v>177233</v>
@@ -3543,7 +3546,7 @@
         <v>29.4</v>
       </c>
       <c r="AH17" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AI17">
         <v>567</v>
@@ -3784,7 +3787,7 @@
         <v>9.6</v>
       </c>
       <c r="AH19" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AR19">
         <v>27.78</v>
@@ -3882,28 +3885,22 @@
         <v>1.08</v>
       </c>
       <c r="R20">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="S20">
-        <v>27.783</v>
+        <v>27.18</v>
       </c>
       <c r="T20">
-        <v>1923</v>
+        <v>1788</v>
       </c>
       <c r="U20">
-        <v>165.924</v>
-      </c>
-      <c r="V20">
-        <v>2420</v>
-      </c>
-      <c r="W20">
-        <v>208.808</v>
+        <v>154.276</v>
       </c>
       <c r="X20">
-        <v>967.191</v>
+        <v>812.4</v>
       </c>
       <c r="Y20">
-        <v>83.453</v>
+        <v>70.09699999999999</v>
       </c>
       <c r="Z20">
         <v>43266</v>
@@ -3930,7 +3927,7 @@
         <v>18.2</v>
       </c>
       <c r="AH20" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AI20">
         <v>351513</v>
@@ -4272,7 +4269,7 @@
         <v>13988.3</v>
       </c>
       <c r="AH23" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="AR23">
         <v>69.91</v>
@@ -4394,7 +4391,7 @@
         <v>3.1</v>
       </c>
       <c r="AH24" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AI24">
         <v>3560</v>
@@ -4531,7 +4528,7 @@
         <v>8.300000000000001</v>
       </c>
       <c r="AH25" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AR25">
         <v>42.59</v>
@@ -4944,16 +4941,16 @@
         <v>0.83</v>
       </c>
       <c r="R29">
-        <v>281</v>
+        <v>263</v>
       </c>
       <c r="S29">
-        <v>40.441</v>
+        <v>37.85</v>
       </c>
       <c r="T29">
-        <v>2857</v>
+        <v>2866</v>
       </c>
       <c r="U29">
-        <v>411.171</v>
+        <v>412.466</v>
       </c>
       <c r="Z29">
         <v>11452</v>
@@ -4980,7 +4977,7 @@
         <v>17.6</v>
       </c>
       <c r="AH29" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AI29">
         <v>54025</v>
@@ -5485,16 +5482,16 @@
         <v>0.92</v>
       </c>
       <c r="R34">
-        <v>834</v>
+        <v>737</v>
       </c>
       <c r="S34">
-        <v>22.097</v>
+        <v>19.527</v>
       </c>
       <c r="T34">
-        <v>3975</v>
+        <v>3432</v>
       </c>
       <c r="U34">
-        <v>105.32</v>
+        <v>90.93300000000001</v>
       </c>
       <c r="Z34">
         <v>50138</v>
@@ -5521,7 +5518,7 @@
         <v>14.2</v>
       </c>
       <c r="AH34" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="AI34">
         <v>1015083</v>
@@ -5655,7 +5652,7 @@
         <v>0.849</v>
       </c>
       <c r="AH35" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AR35">
         <v>64.81</v>
@@ -5961,7 +5958,7 @@
         <v>12.7</v>
       </c>
       <c r="AH38" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AI38">
         <v>291937</v>
@@ -6226,7 +6223,7 @@
         <v>6</v>
       </c>
       <c r="AH40" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AR40">
         <v>81.02</v>
@@ -6675,7 +6672,7 @@
         <v>16.3</v>
       </c>
       <c r="AH44" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="AR44">
         <v>23.15</v>
@@ -6770,16 +6767,16 @@
         <v>0.86</v>
       </c>
       <c r="T45">
-        <v>1474</v>
+        <v>1249</v>
       </c>
       <c r="U45">
-        <v>359.051</v>
+        <v>304.243</v>
       </c>
       <c r="X45">
-        <v>825.838</v>
+        <v>627.436</v>
       </c>
       <c r="Y45">
-        <v>201.165</v>
+        <v>152.837</v>
       </c>
       <c r="Z45">
         <v>7023</v>
@@ -6806,7 +6803,7 @@
         <v>10.8</v>
       </c>
       <c r="AH45" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="AI45">
         <v>87929</v>
@@ -6955,7 +6952,7 @@
         <v>19.8</v>
       </c>
       <c r="AH46" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AR46">
         <v>83.33</v>
@@ -7053,28 +7050,28 @@
         <v>0.7</v>
       </c>
       <c r="R47">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="S47">
-        <v>39.959</v>
+        <v>36.534</v>
       </c>
       <c r="T47">
-        <v>173</v>
+        <v>140</v>
       </c>
       <c r="U47">
-        <v>197.511</v>
+        <v>159.836</v>
       </c>
       <c r="V47">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="W47">
-        <v>17.125</v>
+        <v>19.409</v>
       </c>
       <c r="X47">
-        <v>86</v>
+        <v>62</v>
       </c>
       <c r="Y47">
-        <v>98.185</v>
+        <v>70.78400000000001</v>
       </c>
       <c r="Z47">
         <v>27085</v>
@@ -7101,7 +7098,7 @@
         <v>172.1</v>
       </c>
       <c r="AH47" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AI47">
         <v>25168</v>
@@ -7223,28 +7220,28 @@
         <v>0.9</v>
       </c>
       <c r="R48">
-        <v>1047</v>
+        <v>954</v>
       </c>
       <c r="S48">
-        <v>97.768</v>
+        <v>89.084</v>
       </c>
       <c r="T48">
-        <v>5798</v>
+        <v>5482</v>
       </c>
       <c r="U48">
-        <v>541.415</v>
+        <v>511.907</v>
       </c>
       <c r="V48">
-        <v>1845.197</v>
+        <v>1771.792</v>
       </c>
       <c r="W48">
-        <v>172.304</v>
+        <v>165.449</v>
       </c>
       <c r="X48">
-        <v>10376.344</v>
+        <v>9654.353999999999</v>
       </c>
       <c r="Y48">
-        <v>968.938</v>
+        <v>901.519</v>
       </c>
       <c r="Z48">
         <v>56043</v>
@@ -7265,7 +7262,7 @@
         <v>7.2</v>
       </c>
       <c r="AH48" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AI48">
         <v>327759</v>
@@ -7408,7 +7405,7 @@
         <v>5</v>
       </c>
       <c r="AH49" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="AR49">
         <v>32.41</v>
@@ -7503,22 +7500,22 @@
         <v>0.76</v>
       </c>
       <c r="R50">
-        <v>124</v>
+        <v>97</v>
       </c>
       <c r="S50">
-        <v>21.408</v>
+        <v>16.747</v>
       </c>
       <c r="T50">
-        <v>725</v>
+        <v>529</v>
       </c>
       <c r="U50">
-        <v>125.168</v>
+        <v>91.33</v>
       </c>
       <c r="X50">
-        <v>607.544</v>
+        <v>380.089</v>
       </c>
       <c r="Y50">
-        <v>104.89</v>
+        <v>65.621</v>
       </c>
       <c r="Z50">
         <v>15960</v>
@@ -7545,7 +7542,7 @@
         <v>193.3</v>
       </c>
       <c r="AH50" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AI50">
         <v>298112</v>
@@ -7860,7 +7857,7 @@
         <v>4.8</v>
       </c>
       <c r="AH53" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="AR53">
         <v>70.37</v>
@@ -7982,7 +7979,7 @@
         <v>0.283</v>
       </c>
       <c r="AH54" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="AI54">
         <v>6228</v>
@@ -8226,7 +8223,7 @@
         <v>105.205</v>
       </c>
       <c r="AH56" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AR56">
         <v>47.22</v>
@@ -8514,28 +8511,28 @@
         <v>1.01</v>
       </c>
       <c r="R59">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="S59">
-        <v>33.923</v>
+        <v>28.646</v>
       </c>
       <c r="T59">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="U59">
-        <v>320.383</v>
+        <v>319.629</v>
       </c>
       <c r="V59">
-        <v>32.042</v>
+        <v>26.034</v>
       </c>
       <c r="W59">
-        <v>24.154</v>
+        <v>19.625</v>
       </c>
       <c r="X59">
-        <v>295.383</v>
+        <v>298.387</v>
       </c>
       <c r="Y59">
-        <v>222.672</v>
+        <v>224.936</v>
       </c>
       <c r="Z59">
         <v>5920</v>
@@ -8562,7 +8559,7 @@
         <v>9</v>
       </c>
       <c r="AH59" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AI59">
         <v>46194</v>
@@ -8812,7 +8809,7 @@
         <v>11</v>
       </c>
       <c r="AH61" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AR61">
         <v>46.3</v>
@@ -9016,7 +9013,7 @@
         <v>528</v>
       </c>
       <c r="AH64" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AR64">
         <v>41.67</v>
@@ -9117,16 +9114,16 @@
         <v>1.07</v>
       </c>
       <c r="R65">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="S65">
-        <v>4.332</v>
+        <v>3.61</v>
       </c>
       <c r="T65">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="U65">
-        <v>24.546</v>
+        <v>22.741</v>
       </c>
       <c r="Z65">
         <v>6767</v>
@@ -9153,7 +9150,7 @@
         <v>37.3</v>
       </c>
       <c r="AH65" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AI65">
         <v>193917</v>
@@ -9278,28 +9275,28 @@
         <v>1.17</v>
       </c>
       <c r="R66">
-        <v>2955</v>
+        <v>3148</v>
       </c>
       <c r="S66">
-        <v>45.271</v>
+        <v>48.228</v>
       </c>
       <c r="T66">
-        <v>26357</v>
+        <v>27573</v>
       </c>
       <c r="U66">
-        <v>403.793</v>
+        <v>422.422</v>
       </c>
       <c r="V66">
-        <v>1656.849</v>
+        <v>1732.825</v>
       </c>
       <c r="W66">
-        <v>25.383</v>
+        <v>26.547</v>
       </c>
       <c r="X66">
-        <v>10483.638</v>
+        <v>10425.195</v>
       </c>
       <c r="Y66">
-        <v>160.611</v>
+        <v>159.716</v>
       </c>
       <c r="Z66">
         <v>214907</v>
@@ -9320,7 +9317,7 @@
         <v>14.9</v>
       </c>
       <c r="AH66" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="AI66">
         <v>1825982</v>
@@ -9736,16 +9733,16 @@
         <v>0.92</v>
       </c>
       <c r="R70">
-        <v>4607</v>
+        <v>4337</v>
       </c>
       <c r="S70">
-        <v>54.987</v>
+        <v>51.764</v>
       </c>
       <c r="X70">
-        <v>2510.918</v>
+        <v>2044.663</v>
       </c>
       <c r="Y70">
-        <v>29.969</v>
+        <v>24.404</v>
       </c>
       <c r="AA70">
         <v>38471483</v>
@@ -9766,7 +9763,7 @@
         <v>10</v>
       </c>
       <c r="AH70" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AI70">
         <v>2987398</v>
@@ -9915,7 +9912,7 @@
         <v>6.4</v>
       </c>
       <c r="AH71" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="AR71">
         <v>38.89</v>
@@ -10019,10 +10016,10 @@
         <v>0.89</v>
       </c>
       <c r="V72">
-        <v>87.46899999999999</v>
+        <v>65.116</v>
       </c>
       <c r="W72">
-        <v>8.391999999999999</v>
+        <v>6.247</v>
       </c>
       <c r="Z72">
         <v>37591</v>
@@ -10049,7 +10046,7 @@
         <v>38.5</v>
       </c>
       <c r="AH72" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="AI72">
         <v>359723</v>
@@ -10287,7 +10284,7 @@
         <v>9.5</v>
       </c>
       <c r="AH74" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="AR74">
         <v>51.39</v>
@@ -10860,10 +10857,10 @@
         <v>0.82</v>
       </c>
       <c r="T80">
-        <v>3793</v>
+        <v>3562</v>
       </c>
       <c r="U80">
-        <v>392.636</v>
+        <v>368.724</v>
       </c>
       <c r="Z80">
         <v>15434</v>
@@ -10890,7 +10887,7 @@
         <v>13</v>
       </c>
       <c r="AH80" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AI80">
         <v>357303</v>
@@ -11018,16 +11015,16 @@
         <v>0.67</v>
       </c>
       <c r="T81">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="U81">
-        <v>49.817</v>
+        <v>46.886</v>
       </c>
       <c r="X81">
-        <v>3.824</v>
+        <v>0.956</v>
       </c>
       <c r="Y81">
-        <v>11.205</v>
+        <v>2.801</v>
       </c>
       <c r="Z81">
         <v>716</v>
@@ -11054,7 +11051,7 @@
         <v>285.2</v>
       </c>
       <c r="AH81" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AI81">
         <v>16951</v>
@@ -11203,7 +11200,7 @@
         <v>53.4</v>
       </c>
       <c r="AH82" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="AI82">
         <v>4959445</v>
@@ -11346,7 +11343,7 @@
         <v>3.5</v>
       </c>
       <c r="AH83" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="AI83">
         <v>796819</v>
@@ -11527,7 +11524,7 @@
         <v>8.300000000000001</v>
       </c>
       <c r="AH85" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AR85">
         <v>72.69</v>
@@ -11652,7 +11649,7 @@
         <v>46.9</v>
       </c>
       <c r="AH86" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="AR86">
         <v>44.44</v>
@@ -11750,28 +11747,28 @@
         <v>0.83</v>
       </c>
       <c r="R87">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="S87">
-        <v>44.757</v>
+        <v>42.732</v>
       </c>
       <c r="T87">
-        <v>1914</v>
+        <v>1515</v>
       </c>
       <c r="U87">
-        <v>387.622</v>
+        <v>306.817</v>
       </c>
       <c r="V87">
-        <v>66.452</v>
+        <v>67.458</v>
       </c>
       <c r="W87">
-        <v>13.458</v>
+        <v>13.662</v>
       </c>
       <c r="X87">
-        <v>840.713</v>
+        <v>618.201</v>
       </c>
       <c r="Y87">
-        <v>170.261</v>
+        <v>125.198</v>
       </c>
       <c r="Z87">
         <v>18190</v>
@@ -11798,7 +11795,7 @@
         <v>15.9</v>
       </c>
       <c r="AH87" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AI87">
         <v>219200</v>
@@ -11881,7 +11878,7 @@
         <v>339</v>
       </c>
       <c r="D88" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="E88">
         <v>675618</v>
@@ -11923,28 +11920,28 @@
         <v>1.04</v>
       </c>
       <c r="R88">
-        <v>420</v>
+        <v>395</v>
       </c>
       <c r="S88">
-        <v>48.524</v>
+        <v>45.636</v>
       </c>
       <c r="T88">
-        <v>1772</v>
+        <v>1668</v>
       </c>
       <c r="U88">
-        <v>204.724</v>
+        <v>192.709</v>
       </c>
       <c r="V88">
-        <v>1115</v>
+        <v>1004</v>
       </c>
       <c r="W88">
-        <v>128.819</v>
+        <v>115.995</v>
       </c>
       <c r="X88">
-        <v>1817</v>
+        <v>1594</v>
       </c>
       <c r="Y88">
-        <v>209.923</v>
+        <v>184.159</v>
       </c>
       <c r="Z88">
         <v>54737</v>
@@ -11971,7 +11968,7 @@
         <v>10.8</v>
       </c>
       <c r="AH88" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AI88">
         <v>5336910</v>
@@ -12099,22 +12096,22 @@
         <v>0.91</v>
       </c>
       <c r="R89">
-        <v>2400</v>
+        <v>2215</v>
       </c>
       <c r="S89">
-        <v>39.694</v>
+        <v>36.635</v>
       </c>
       <c r="T89">
-        <v>23709</v>
+        <v>22311</v>
       </c>
       <c r="U89">
-        <v>392.132</v>
+        <v>369.01</v>
       </c>
       <c r="X89">
-        <v>3663.197</v>
+        <v>3208.428</v>
       </c>
       <c r="Y89">
-        <v>60.587</v>
+        <v>53.065</v>
       </c>
       <c r="Z89">
         <v>244429</v>
@@ -12141,7 +12138,7 @@
         <v>20.5</v>
       </c>
       <c r="AH89" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AI89">
         <v>2335997</v>
@@ -12293,7 +12290,7 @@
         <v>8.6</v>
       </c>
       <c r="AH90" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="AR90">
         <v>71.3</v>
@@ -12418,7 +12415,7 @@
         <v>19.4</v>
       </c>
       <c r="AH91" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="AR91">
         <v>53.24</v>
@@ -12540,7 +12537,7 @@
         <v>22.9</v>
       </c>
       <c r="AH92" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AR92">
         <v>75.93000000000001</v>
@@ -12659,7 +12656,7 @@
         <v>24.8</v>
       </c>
       <c r="AH93" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AR93">
         <v>68.52</v>
@@ -12956,7 +12953,7 @@
         <v>15.5</v>
       </c>
       <c r="AH96" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AI96">
         <v>35000</v>
@@ -13253,22 +13250,22 @@
         <v>1.05</v>
       </c>
       <c r="T99">
-        <v>1109</v>
+        <v>1061</v>
       </c>
       <c r="U99">
-        <v>587.954</v>
+        <v>562.506</v>
       </c>
       <c r="V99">
-        <v>158.169</v>
+        <v>160.133</v>
       </c>
       <c r="W99">
-        <v>83.85599999999999</v>
+        <v>84.89700000000001</v>
       </c>
       <c r="X99">
-        <v>734.845</v>
+        <v>695.549</v>
       </c>
       <c r="Y99">
-        <v>389.59</v>
+        <v>368.756</v>
       </c>
       <c r="Z99">
         <v>12317</v>
@@ -13295,7 +13292,7 @@
         <v>12.2</v>
       </c>
       <c r="AH99" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AI99">
         <v>29844</v>
@@ -13708,7 +13705,7 @@
         <v>0.624</v>
       </c>
       <c r="AH103" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="AR103">
         <v>76.84999999999999</v>
@@ -13871,22 +13868,22 @@
         <v>0.93</v>
       </c>
       <c r="T105">
-        <v>1432</v>
+        <v>1346</v>
       </c>
       <c r="U105">
-        <v>526.028</v>
+        <v>494.436</v>
       </c>
       <c r="V105">
-        <v>104.247</v>
+        <v>91.581</v>
       </c>
       <c r="W105">
-        <v>38.294</v>
+        <v>33.641</v>
       </c>
       <c r="X105">
-        <v>510.518</v>
+        <v>445.242</v>
       </c>
       <c r="Y105">
-        <v>187.532</v>
+        <v>163.554</v>
       </c>
       <c r="Z105">
         <v>8028</v>
@@ -13913,7 +13910,7 @@
         <v>10</v>
       </c>
       <c r="AH105" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AI105">
         <v>114590</v>
@@ -14041,16 +14038,16 @@
         <v>0.92</v>
       </c>
       <c r="R106">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="S106">
-        <v>22.365</v>
+        <v>17.573</v>
       </c>
       <c r="T106">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="U106">
-        <v>113.423</v>
+        <v>105.435</v>
       </c>
       <c r="Z106">
         <v>10577</v>
@@ -14077,7 +14074,7 @@
         <v>50.3</v>
       </c>
       <c r="AH106" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AI106">
         <v>15407</v>
@@ -14223,7 +14220,7 @@
         <v>7.6</v>
       </c>
       <c r="AH107" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AR107">
         <v>37.04</v>
@@ -14339,7 +14336,7 @@
         <v>3.5</v>
       </c>
       <c r="AH108" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="AR108">
         <v>51.85</v>
@@ -14467,7 +14464,7 @@
         <v>11.7</v>
       </c>
       <c r="AH109" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="AR109">
         <v>77.31</v>
@@ -14592,7 +14589,7 @@
         <v>26</v>
       </c>
       <c r="AH110" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="AI110">
         <v>3204</v>
@@ -14800,10 +14797,10 @@
         <v>1</v>
       </c>
       <c r="X112">
-        <v>18.787</v>
+        <v>23.26</v>
       </c>
       <c r="Y112">
-        <v>42.548</v>
+        <v>52.679</v>
       </c>
       <c r="AI112">
         <v>31633</v>
@@ -15014,7 +15011,7 @@
         <v>23.4</v>
       </c>
       <c r="AH114" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AR114">
         <v>50.93</v>
@@ -15231,7 +15228,7 @@
         <v>2.8</v>
       </c>
       <c r="AH116" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="AI116">
         <v>695088</v>
@@ -15629,7 +15626,7 @@
         <v>423.6</v>
       </c>
       <c r="AH120" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="AR120">
         <v>73.61</v>
@@ -15852,7 +15849,7 @@
         <v>16.8</v>
       </c>
       <c r="AH122" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="AI122">
         <v>351723</v>
@@ -15992,7 +15989,7 @@
         <v>3.5</v>
       </c>
       <c r="AH123" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="AR123">
         <v>64.81</v>
@@ -16120,7 +16117,7 @@
         <v>58.6</v>
       </c>
       <c r="AH124" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="AI124">
         <v>3800</v>
@@ -16263,7 +16260,7 @@
         <v>7.6</v>
       </c>
       <c r="AH125" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="AR125">
         <v>38.89</v>
@@ -16388,7 +16385,7 @@
         <v>21.2</v>
       </c>
       <c r="AH126" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AI126">
         <v>113175</v>
@@ -16501,28 +16498,28 @@
         <v>0.88</v>
       </c>
       <c r="R127">
-        <v>680</v>
+        <v>646</v>
       </c>
       <c r="S127">
-        <v>39.685</v>
+        <v>37.701</v>
       </c>
       <c r="T127">
-        <v>1667</v>
+        <v>1573</v>
       </c>
       <c r="U127">
-        <v>97.28700000000001</v>
+        <v>91.801</v>
       </c>
       <c r="V127">
-        <v>233.989</v>
+        <v>245.886</v>
       </c>
       <c r="W127">
-        <v>13.656</v>
+        <v>14.35</v>
       </c>
       <c r="X127">
-        <v>1253.227</v>
+        <v>1205.636</v>
       </c>
       <c r="Y127">
-        <v>73.139</v>
+        <v>70.36199999999999</v>
       </c>
       <c r="AA127">
         <v>5934044</v>
@@ -16543,7 +16540,7 @@
         <v>9.699999999999999</v>
       </c>
       <c r="AH127" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="AI127">
         <v>330494</v>
@@ -16680,7 +16677,7 @@
         <v>3392.6</v>
       </c>
       <c r="AH128" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AR128">
         <v>22.22</v>
@@ -16995,7 +16992,7 @@
         <v>4.5</v>
       </c>
       <c r="AH131" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="AR131">
         <v>58.33</v>
@@ -17143,7 +17140,7 @@
         <v>6.9</v>
       </c>
       <c r="AH133" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AS133">
         <v>2083380</v>
@@ -17235,10 +17232,10 @@
         <v>0.84</v>
       </c>
       <c r="T134">
-        <v>135</v>
+        <v>90</v>
       </c>
       <c r="U134">
-        <v>24.902</v>
+        <v>16.601</v>
       </c>
       <c r="V134">
         <v>10.175</v>
@@ -17247,10 +17244,10 @@
         <v>1.877</v>
       </c>
       <c r="X134">
-        <v>87.502</v>
+        <v>42.733</v>
       </c>
       <c r="Y134">
-        <v>16.14</v>
+        <v>7.883</v>
       </c>
       <c r="Z134">
         <v>21297</v>
@@ -17277,7 +17274,7 @@
         <v>59.6</v>
       </c>
       <c r="AH134" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="AI134">
         <v>165515</v>
@@ -17580,7 +17577,7 @@
         <v>24.5</v>
       </c>
       <c r="AH137" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AR137">
         <v>50.46</v>
@@ -17702,7 +17699,7 @@
         <v>8.199999999999999</v>
       </c>
       <c r="AH138" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AR138">
         <v>78.7</v>
@@ -17818,7 +17815,7 @@
         <v>7.5</v>
       </c>
       <c r="AH139" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AI139">
         <v>6420</v>
@@ -18050,7 +18047,7 @@
         <v>4.5</v>
       </c>
       <c r="AH141" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AR141">
         <v>55.56</v>
@@ -18273,7 +18270,7 @@
         <v>18.8</v>
       </c>
       <c r="AH143" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="AR143">
         <v>63.43</v>
@@ -18374,16 +18371,16 @@
         <v>0.88</v>
       </c>
       <c r="T144">
-        <v>14377</v>
+        <v>13339</v>
       </c>
       <c r="U144">
-        <v>379.876</v>
+        <v>352.449</v>
       </c>
       <c r="X144">
-        <v>66.777</v>
+        <v>81.727</v>
       </c>
       <c r="Y144">
-        <v>1.764</v>
+        <v>2.159</v>
       </c>
       <c r="Z144">
         <v>41614</v>
@@ -18410,7 +18407,7 @@
         <v>7.4</v>
       </c>
       <c r="AH144" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="AI144">
         <v>1566604</v>
@@ -18535,22 +18532,22 @@
         <v>1.33</v>
       </c>
       <c r="R145">
-        <v>742</v>
+        <v>858</v>
       </c>
       <c r="S145">
-        <v>72.76900000000001</v>
+        <v>84.145</v>
       </c>
       <c r="T145">
-        <v>6117</v>
+        <v>6694</v>
       </c>
       <c r="U145">
-        <v>599.9</v>
+        <v>656.486</v>
       </c>
       <c r="X145">
-        <v>606.249</v>
+        <v>627.086</v>
       </c>
       <c r="Y145">
-        <v>59.455</v>
+        <v>61.499</v>
       </c>
       <c r="Z145">
         <v>45261</v>
@@ -18577,7 +18574,7 @@
         <v>4.9</v>
       </c>
       <c r="AH145" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AI145">
         <v>364211</v>
@@ -18729,7 +18726,7 @@
         <v>14.7</v>
       </c>
       <c r="AH146" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="AR146">
         <v>56.48</v>
@@ -18827,16 +18824,16 @@
         <v>0.86</v>
       </c>
       <c r="R147">
-        <v>1020</v>
+        <v>996</v>
       </c>
       <c r="S147">
-        <v>53.021</v>
+        <v>51.773</v>
       </c>
       <c r="X147">
-        <v>4713.686</v>
+        <v>8450.349</v>
       </c>
       <c r="Y147">
-        <v>245.024</v>
+        <v>439.26</v>
       </c>
       <c r="Z147">
         <v>25550</v>
@@ -18863,7 +18860,7 @@
         <v>8.300000000000001</v>
       </c>
       <c r="AH147" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AI147">
         <v>794795</v>
@@ -19015,7 +19012,7 @@
         <v>19.6</v>
       </c>
       <c r="AH148" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AR148">
         <v>50.46</v>
@@ -19140,7 +19137,7 @@
         <v>29</v>
       </c>
       <c r="AH149" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="AR149">
         <v>74.06999999999999</v>
@@ -19739,7 +19736,7 @@
         <v>185.5</v>
       </c>
       <c r="AH156" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AI156">
         <v>440618</v>
@@ -19873,7 +19870,7 @@
         <v>7.3</v>
       </c>
       <c r="AH157" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AR157">
         <v>50.46</v>
@@ -19998,7 +19995,7 @@
         <v>6.3</v>
       </c>
       <c r="AH158" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="AI158">
         <v>526930</v>
@@ -20352,7 +20349,7 @@
         <v>1135.1</v>
       </c>
       <c r="AH161" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="AI161">
         <v>181000</v>
@@ -20473,6 +20470,12 @@
       <c r="Q162">
         <v>0.95</v>
       </c>
+      <c r="T162">
+        <v>3335</v>
+      </c>
+      <c r="U162">
+        <v>610.846</v>
+      </c>
       <c r="Z162">
         <v>12313</v>
       </c>
@@ -20498,7 +20501,7 @@
         <v>4.8</v>
       </c>
       <c r="AH162" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AI162">
         <v>191327</v>
@@ -20626,28 +20629,28 @@
         <v>0.97</v>
       </c>
       <c r="R163">
-        <v>190</v>
+        <v>167</v>
       </c>
       <c r="S163">
-        <v>91.393</v>
+        <v>80.33</v>
       </c>
       <c r="T163">
-        <v>1149</v>
+        <v>1053</v>
       </c>
       <c r="U163">
-        <v>552.688</v>
+        <v>506.51</v>
       </c>
       <c r="V163">
-        <v>102.902</v>
+        <v>85.91800000000001</v>
       </c>
       <c r="W163">
-        <v>49.498</v>
+        <v>41.328</v>
       </c>
       <c r="X163">
-        <v>695.3390000000001</v>
+        <v>578.45</v>
       </c>
       <c r="Y163">
-        <v>334.469</v>
+        <v>278.244</v>
       </c>
       <c r="Z163">
         <v>37299</v>
@@ -20674,7 +20677,7 @@
         <v>11.8</v>
       </c>
       <c r="AH163" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AI163">
         <v>83335</v>
@@ -20989,7 +20992,7 @@
         <v>7.7</v>
       </c>
       <c r="AH166" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="AR166">
         <v>72.22</v>
@@ -21143,7 +21146,7 @@
         <v>94.7</v>
       </c>
       <c r="AH168" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="AR168">
         <v>63.89</v>
@@ -21262,7 +21265,7 @@
         <v>225.4</v>
       </c>
       <c r="AH169" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AR169">
         <v>43.52</v>
@@ -21347,17 +21350,29 @@
       <c r="Q170">
         <v>1.46</v>
       </c>
+      <c r="R170">
+        <v>4515</v>
+      </c>
+      <c r="S170">
+        <v>96.568</v>
+      </c>
+      <c r="T170">
+        <v>30789</v>
+      </c>
+      <c r="U170">
+        <v>658.521</v>
+      </c>
       <c r="V170">
-        <v>115.55</v>
+        <v>128.499</v>
       </c>
       <c r="W170">
-        <v>2.471</v>
+        <v>2.748</v>
       </c>
       <c r="X170">
-        <v>3480.431</v>
+        <v>2756.255</v>
       </c>
       <c r="Y170">
-        <v>74.44</v>
+        <v>58.951</v>
       </c>
       <c r="AA170">
         <v>28228026</v>
@@ -21378,7 +21393,7 @@
         <v>7.1</v>
       </c>
       <c r="AH170" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AI170">
         <v>1865342</v>
@@ -21530,7 +21545,7 @@
         <v>18.6</v>
       </c>
       <c r="AH171" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AI171">
         <v>139914</v>
@@ -21836,22 +21851,22 @@
         <v>1.25</v>
       </c>
       <c r="R174">
-        <v>303</v>
+        <v>260</v>
       </c>
       <c r="S174">
-        <v>30.002</v>
+        <v>25.744</v>
       </c>
       <c r="T174">
-        <v>2127</v>
+        <v>1830</v>
       </c>
       <c r="U174">
-        <v>210.609</v>
+        <v>181.201</v>
       </c>
       <c r="V174">
-        <v>110.567</v>
+        <v>91.81</v>
       </c>
       <c r="W174">
-        <v>10.948</v>
+        <v>9.090999999999999</v>
       </c>
       <c r="Z174">
         <v>26885</v>
@@ -21872,7 +21887,7 @@
         <v>9.1</v>
       </c>
       <c r="AH174" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AI174">
         <v>320378</v>
@@ -22024,7 +22039,7 @@
         <v>11.8</v>
       </c>
       <c r="AH175" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AI175">
         <v>315033</v>
@@ -22238,7 +22253,7 @@
         <v>473.5</v>
       </c>
       <c r="AH177" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="AR177">
         <v>19.44</v>
@@ -22719,7 +22734,7 @@
         <v>16.5</v>
       </c>
       <c r="AH182" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AR182">
         <v>37.5</v>
@@ -22847,7 +22862,7 @@
         <v>60.5</v>
       </c>
       <c r="AH183" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="AR183">
         <v>68.52</v>
@@ -23067,7 +23082,7 @@
         <v>21.4</v>
       </c>
       <c r="AH185" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AI185">
         <v>2500806</v>
@@ -23207,7 +23222,7 @@
         <v>32</v>
       </c>
       <c r="AH186" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="AR186">
         <v>49.07</v>
@@ -23335,7 +23350,7 @@
         <v>5.2</v>
       </c>
       <c r="AH187" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AR187">
         <v>54.63</v>
@@ -23460,7 +23475,7 @@
         <v>49</v>
       </c>
       <c r="AH188" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AI188">
         <v>3849374</v>
@@ -23585,22 +23600,22 @@
         <v>0.91</v>
       </c>
       <c r="R189">
-        <v>3937</v>
+        <v>3625</v>
       </c>
       <c r="S189">
-        <v>57.994</v>
+        <v>53.398</v>
       </c>
       <c r="T189">
-        <v>36931</v>
+        <v>31670</v>
       </c>
       <c r="U189">
-        <v>544.015</v>
+        <v>466.517</v>
       </c>
       <c r="X189">
-        <v>25365</v>
+        <v>19585</v>
       </c>
       <c r="Y189">
-        <v>373.641</v>
+        <v>288.498</v>
       </c>
       <c r="Z189">
         <v>606382</v>
@@ -23627,7 +23642,7 @@
         <v>28.1</v>
       </c>
       <c r="AH189" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AI189">
         <v>10992444</v>
@@ -23755,28 +23770,28 @@
         <v>0.9</v>
       </c>
       <c r="R190">
-        <v>20113</v>
+        <v>17918</v>
       </c>
       <c r="S190">
-        <v>60.764</v>
+        <v>54.132</v>
       </c>
       <c r="T190">
-        <v>104303</v>
+        <v>88668</v>
       </c>
       <c r="U190">
-        <v>315.112</v>
+        <v>267.877</v>
       </c>
       <c r="V190">
-        <v>1067</v>
+        <v>1003</v>
       </c>
       <c r="W190">
-        <v>3.224</v>
+        <v>3.03</v>
       </c>
       <c r="X190">
-        <v>28089</v>
+        <v>22007</v>
       </c>
       <c r="Y190">
-        <v>84.86</v>
+        <v>66.486</v>
       </c>
       <c r="Z190">
         <v>939538</v>
@@ -23797,7 +23812,7 @@
         <v>3.809</v>
       </c>
       <c r="AH190" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AI190">
         <v>35203710</v>
@@ -23943,7 +23958,7 @@
         <v>11.5</v>
       </c>
       <c r="AH191" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AR191">
         <v>64.81</v>
@@ -24700,7 +24715,7 @@
         <v>8.1</v>
       </c>
       <c r="AH199" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AR199">
         <v>49.07</v>
@@ -24828,7 +24843,7 @@
         <v>12.4</v>
       </c>
       <c r="AH200" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AR200">
         <v>84.26000000000001</v>

</xml_diff>

<commit_message>
Manual JHU update with per capita values for continents
</commit_message>
<xml_diff>
--- a/public/data/latest/owid-covid-latest.xlsx
+++ b/public/data/latest/owid-covid-latest.xlsx
@@ -2041,6 +2041,24 @@
       <c r="J3">
         <v>552.857</v>
       </c>
+      <c r="K3">
+        <v>2754.759</v>
+      </c>
+      <c r="L3">
+        <v>8.467000000000001</v>
+      </c>
+      <c r="M3">
+        <v>10.217</v>
+      </c>
+      <c r="N3">
+        <v>71.78400000000001</v>
+      </c>
+      <c r="O3">
+        <v>0.521</v>
+      </c>
+      <c r="P3">
+        <v>0.412</v>
+      </c>
     </row>
     <row r="4" spans="1:59">
       <c r="A4" t="s">
@@ -2831,6 +2849,24 @@
       <c r="J11">
         <v>932.7140000000001</v>
       </c>
+      <c r="K11">
+        <v>5114.304</v>
+      </c>
+      <c r="L11">
+        <v>14.657</v>
+      </c>
+      <c r="M11">
+        <v>14.814</v>
+      </c>
+      <c r="N11">
+        <v>82.304</v>
+      </c>
+      <c r="O11">
+        <v>0.203</v>
+      </c>
+      <c r="P11">
+        <v>0.201</v>
+      </c>
     </row>
     <row r="12" spans="1:59">
       <c r="A12" t="s">
@@ -8702,6 +8738,24 @@
       <c r="J62">
         <v>4677.714</v>
       </c>
+      <c r="K62">
+        <v>42373.851</v>
+      </c>
+      <c r="L62">
+        <v>172.557</v>
+      </c>
+      <c r="M62">
+        <v>197.949</v>
+      </c>
+      <c r="N62">
+        <v>999.057</v>
+      </c>
+      <c r="O62">
+        <v>8.006</v>
+      </c>
+      <c r="P62">
+        <v>6.248</v>
+      </c>
     </row>
     <row r="63" spans="1:59">
       <c r="C63" t="s">
@@ -16734,6 +16788,24 @@
       <c r="J133">
         <v>4360</v>
       </c>
+      <c r="K133">
+        <v>52673.584</v>
+      </c>
+      <c r="L133">
+        <v>191.33</v>
+      </c>
+      <c r="M133">
+        <v>215.531</v>
+      </c>
+      <c r="N133">
+        <v>1151.517</v>
+      </c>
+      <c r="O133">
+        <v>8.563000000000001</v>
+      </c>
+      <c r="P133">
+        <v>7.364</v>
+      </c>
     </row>
     <row r="134" spans="1:59">
       <c r="A134" t="s">
@@ -17040,6 +17112,24 @@
       <c r="J136">
         <v>0</v>
       </c>
+      <c r="K136">
+        <v>753.928</v>
+      </c>
+      <c r="L136">
+        <v>0.305</v>
+      </c>
+      <c r="M136">
+        <v>0.308</v>
+      </c>
+      <c r="N136">
+        <v>22.143</v>
+      </c>
+      <c r="O136">
+        <v>0</v>
+      </c>
+      <c r="P136">
+        <v>0</v>
+      </c>
     </row>
     <row r="137" spans="1:59">
       <c r="A137" t="s">
@@ -20631,6 +20721,24 @@
       </c>
       <c r="J168">
         <v>1865.714</v>
+      </c>
+      <c r="K168">
+        <v>38395.099</v>
+      </c>
+      <c r="L168">
+        <v>245.415</v>
+      </c>
+      <c r="M168">
+        <v>175.096</v>
+      </c>
+      <c r="N168">
+        <v>1003.522</v>
+      </c>
+      <c r="O168">
+        <v>6.704</v>
+      </c>
+      <c r="P168">
+        <v>4.331</v>
       </c>
     </row>
     <row r="169" spans="1:59">

</xml_diff>

<commit_message>
Manual complete dataset update (new HDI values)
</commit_message>
<xml_diff>
--- a/public/data/latest/owid-covid-latest.xlsx
+++ b/public/data/latest/owid-covid-latest.xlsx
@@ -2013,7 +2013,7 @@
         <v>64.83</v>
       </c>
       <c r="BG2">
-        <v>0.498</v>
+        <v>0.511</v>
       </c>
     </row>
     <row r="3" spans="1:59">
@@ -2179,7 +2179,7 @@
         <v>78.56999999999999</v>
       </c>
       <c r="BG4">
-        <v>0.785</v>
+        <v>0.795</v>
       </c>
     </row>
     <row r="5" spans="1:59">
@@ -2292,7 +2292,7 @@
         <v>76.88</v>
       </c>
       <c r="BG5">
-        <v>0.754</v>
+        <v>0.748</v>
       </c>
     </row>
     <row r="6" spans="1:59">
@@ -2408,7 +2408,7 @@
         <v>83.73</v>
       </c>
       <c r="BG6">
-        <v>0.858</v>
+        <v>0.868</v>
       </c>
     </row>
     <row r="7" spans="1:59">
@@ -2577,7 +2577,7 @@
         <v>77.02</v>
       </c>
       <c r="BG8">
-        <v>0.78</v>
+        <v>0.778</v>
       </c>
     </row>
     <row r="9" spans="1:59">
@@ -2726,7 +2726,7 @@
         <v>76.67</v>
       </c>
       <c r="BG9">
-        <v>0.825</v>
+        <v>0.845</v>
       </c>
     </row>
     <row r="10" spans="1:59">
@@ -2821,7 +2821,7 @@
         <v>75.09</v>
       </c>
       <c r="BG10">
-        <v>0.755</v>
+        <v>0.776</v>
       </c>
     </row>
     <row r="11" spans="1:59">
@@ -2987,7 +2987,7 @@
         <v>83.44</v>
       </c>
       <c r="BG12">
-        <v>0.9389999999999999</v>
+        <v>0.944</v>
       </c>
     </row>
     <row r="13" spans="1:59">
@@ -3142,7 +3142,7 @@
         <v>81.54000000000001</v>
       </c>
       <c r="BG13">
-        <v>0.908</v>
+        <v>0.922</v>
       </c>
     </row>
     <row r="14" spans="1:59">
@@ -3237,7 +3237,7 @@
         <v>73</v>
       </c>
       <c r="BG14">
-        <v>0.757</v>
+        <v>0.756</v>
       </c>
     </row>
     <row r="15" spans="1:59">
@@ -3329,7 +3329,7 @@
         <v>73.92</v>
       </c>
       <c r="BG15">
-        <v>0.8070000000000001</v>
+        <v>0.8139999999999999</v>
       </c>
     </row>
     <row r="16" spans="1:59">
@@ -3469,7 +3469,7 @@
         <v>77.29000000000001</v>
       </c>
       <c r="BG16">
-        <v>0.846</v>
+        <v>0.852</v>
       </c>
     </row>
     <row r="17" spans="1:59">
@@ -3612,7 +3612,7 @@
         <v>72.59</v>
       </c>
       <c r="BG17">
-        <v>0.608</v>
+        <v>0.632</v>
       </c>
     </row>
     <row r="18" spans="1:59">
@@ -3707,7 +3707,7 @@
         <v>79.19</v>
       </c>
       <c r="BG18">
-        <v>0.8</v>
+        <v>0.8139999999999999</v>
       </c>
     </row>
     <row r="19" spans="1:59">
@@ -3820,7 +3820,7 @@
         <v>74.79000000000001</v>
       </c>
       <c r="BG19">
-        <v>0.8080000000000001</v>
+        <v>0.823</v>
       </c>
     </row>
     <row r="20" spans="1:59">
@@ -3987,7 +3987,7 @@
         <v>81.63</v>
       </c>
       <c r="BG20">
-        <v>0.916</v>
+        <v>0.931</v>
       </c>
     </row>
     <row r="21" spans="1:59">
@@ -4076,7 +4076,7 @@
         <v>74.62</v>
       </c>
       <c r="BG21">
-        <v>0.708</v>
+        <v>0.716</v>
       </c>
     </row>
     <row r="22" spans="1:59">
@@ -4174,7 +4174,7 @@
         <v>61.77</v>
       </c>
       <c r="BG22">
-        <v>0.515</v>
+        <v>0.545</v>
       </c>
     </row>
     <row r="23" spans="1:59">
@@ -4293,7 +4293,7 @@
         <v>71.78</v>
       </c>
       <c r="BG23">
-        <v>0.612</v>
+        <v>0.654</v>
       </c>
     </row>
     <row r="24" spans="1:59">
@@ -4427,7 +4427,7 @@
         <v>71.51000000000001</v>
       </c>
       <c r="BG24">
-        <v>0.6929999999999999</v>
+        <v>0.718</v>
       </c>
     </row>
     <row r="25" spans="1:59">
@@ -4552,7 +4552,7 @@
         <v>77.40000000000001</v>
       </c>
       <c r="BG25">
-        <v>0.768</v>
+        <v>0.78</v>
       </c>
     </row>
     <row r="26" spans="1:59">
@@ -4644,7 +4644,7 @@
         <v>69.59</v>
       </c>
       <c r="BG26">
-        <v>0.717</v>
+        <v>0.735</v>
       </c>
     </row>
     <row r="27" spans="1:59">
@@ -4763,7 +4763,7 @@
         <v>75.88</v>
       </c>
       <c r="BG27">
-        <v>0.759</v>
+        <v>0.765</v>
       </c>
     </row>
     <row r="28" spans="1:59">
@@ -4855,7 +4855,7 @@
         <v>75.86</v>
       </c>
       <c r="BG28">
-        <v>0.853</v>
+        <v>0.838</v>
       </c>
     </row>
     <row r="29" spans="1:59">
@@ -5016,7 +5016,7 @@
         <v>75.05</v>
       </c>
       <c r="BG29">
-        <v>0.8129999999999999</v>
+        <v>0.8159999999999999</v>
       </c>
     </row>
     <row r="30" spans="1:59">
@@ -5114,7 +5114,7 @@
         <v>61.58</v>
       </c>
       <c r="BG30">
-        <v>0.423</v>
+        <v>0.452</v>
       </c>
     </row>
     <row r="31" spans="1:59">
@@ -5206,7 +5206,7 @@
         <v>61.58</v>
       </c>
       <c r="BG31">
-        <v>0.417</v>
+        <v>0.433</v>
       </c>
     </row>
     <row r="32" spans="1:59">
@@ -5289,7 +5289,7 @@
         <v>69.81999999999999</v>
       </c>
       <c r="BG32">
-        <v>0.582</v>
+        <v>0.594</v>
       </c>
     </row>
     <row r="33" spans="1:59">
@@ -5381,7 +5381,7 @@
         <v>59.29</v>
       </c>
       <c r="BG33">
-        <v>0.556</v>
+        <v>0.5629999999999999</v>
       </c>
     </row>
     <row r="34" spans="1:59">
@@ -5542,7 +5542,7 @@
         <v>82.43000000000001</v>
       </c>
       <c r="BG34">
-        <v>0.926</v>
+        <v>0.929</v>
       </c>
     </row>
     <row r="35" spans="1:59">
@@ -5643,7 +5643,7 @@
         <v>72.98</v>
       </c>
       <c r="BG35">
-        <v>0.654</v>
+        <v>0.665</v>
       </c>
     </row>
     <row r="36" spans="1:59">
@@ -5729,7 +5729,7 @@
         <v>53.28</v>
       </c>
       <c r="BG36">
-        <v>0.367</v>
+        <v>0.397</v>
       </c>
     </row>
     <row r="37" spans="1:59">
@@ -5818,7 +5818,7 @@
         <v>54.24</v>
       </c>
       <c r="BG37">
-        <v>0.404</v>
+        <v>0.398</v>
       </c>
     </row>
     <row r="38" spans="1:59">
@@ -5967,7 +5967,7 @@
         <v>80.18000000000001</v>
       </c>
       <c r="BG38">
-        <v>0.843</v>
+        <v>0.851</v>
       </c>
     </row>
     <row r="39" spans="1:59">
@@ -6071,7 +6071,7 @@
         <v>76.91</v>
       </c>
       <c r="BG39">
-        <v>0.752</v>
+        <v>0.761</v>
       </c>
     </row>
     <row r="40" spans="1:59">
@@ -6196,7 +6196,7 @@
         <v>77.29000000000001</v>
       </c>
       <c r="BG40">
-        <v>0.747</v>
+        <v>0.767</v>
       </c>
     </row>
     <row r="41" spans="1:59">
@@ -6291,7 +6291,7 @@
         <v>64.31999999999999</v>
       </c>
       <c r="BG41">
-        <v>0.503</v>
+        <v>0.554</v>
       </c>
     </row>
     <row r="42" spans="1:59">
@@ -6386,7 +6386,7 @@
         <v>64.56999999999999</v>
       </c>
       <c r="BG42">
-        <v>0.606</v>
+        <v>0.574</v>
       </c>
     </row>
     <row r="43" spans="1:59">
@@ -6508,7 +6508,7 @@
         <v>80.28</v>
       </c>
       <c r="BG43">
-        <v>0.794</v>
+        <v>0.8100000000000001</v>
       </c>
     </row>
     <row r="44" spans="1:59">
@@ -6624,7 +6624,7 @@
         <v>57.78</v>
       </c>
       <c r="BG44">
-        <v>0.492</v>
+        <v>0.538</v>
       </c>
     </row>
     <row r="45" spans="1:59">
@@ -6785,7 +6785,7 @@
         <v>78.48999999999999</v>
       </c>
       <c r="BG45">
-        <v>0.831</v>
+        <v>0.851</v>
       </c>
     </row>
     <row r="46" spans="1:59">
@@ -6904,7 +6904,7 @@
         <v>78.8</v>
       </c>
       <c r="BG46">
-        <v>0.777</v>
+        <v>0.783</v>
       </c>
     </row>
     <row r="47" spans="1:59">
@@ -7065,7 +7065,7 @@
         <v>80.98</v>
       </c>
       <c r="BG47">
-        <v>0.869</v>
+        <v>0.887</v>
       </c>
     </row>
     <row r="48" spans="1:59">
@@ -7229,7 +7229,7 @@
         <v>79.38</v>
       </c>
       <c r="BG48">
-        <v>0.888</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="49" spans="1:59">
@@ -7339,7 +7339,7 @@
         <v>60.68</v>
       </c>
       <c r="BG49">
-        <v>0.457</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="50" spans="1:59">
@@ -7506,7 +7506,7 @@
         <v>80.90000000000001</v>
       </c>
       <c r="BG50">
-        <v>0.929</v>
+        <v>0.9399999999999999</v>
       </c>
     </row>
     <row r="51" spans="1:59">
@@ -7601,7 +7601,7 @@
         <v>67.11</v>
       </c>
       <c r="BG51">
-        <v>0.476</v>
+        <v>0.524</v>
       </c>
     </row>
     <row r="52" spans="1:59">
@@ -7666,7 +7666,7 @@
         <v>75</v>
       </c>
       <c r="BG52">
-        <v>0.715</v>
+        <v>0.742</v>
       </c>
     </row>
     <row r="53" spans="1:59">
@@ -7791,7 +7791,7 @@
         <v>74.08</v>
       </c>
       <c r="BG53">
-        <v>0.736</v>
+        <v>0.756</v>
       </c>
     </row>
     <row r="54" spans="1:59">
@@ -7931,7 +7931,7 @@
         <v>77.01000000000001</v>
       </c>
       <c r="BG54">
-        <v>0.752</v>
+        <v>0.759</v>
       </c>
     </row>
     <row r="55" spans="1:59">
@@ -8041,7 +8041,7 @@
         <v>71.98999999999999</v>
       </c>
       <c r="BG55">
-        <v>0.696</v>
+        <v>0.707</v>
       </c>
     </row>
     <row r="56" spans="1:59">
@@ -8139,7 +8139,7 @@
         <v>73.31999999999999</v>
       </c>
       <c r="BG56">
-        <v>0.674</v>
+        <v>0.673</v>
       </c>
     </row>
     <row r="57" spans="1:59">
@@ -8225,7 +8225,7 @@
         <v>58.74</v>
       </c>
       <c r="BG57">
-        <v>0.591</v>
+        <v>0.592</v>
       </c>
     </row>
     <row r="58" spans="1:59">
@@ -8317,7 +8317,7 @@
         <v>66.31999999999999</v>
       </c>
       <c r="BG58">
-        <v>0.44</v>
+        <v>0.459</v>
       </c>
     </row>
     <row r="59" spans="1:59">
@@ -8490,7 +8490,7 @@
         <v>78.73999999999999</v>
       </c>
       <c r="BG59">
-        <v>0.871</v>
+        <v>0.892</v>
       </c>
     </row>
     <row r="60" spans="1:59">
@@ -8585,7 +8585,7 @@
         <v>60.19</v>
       </c>
       <c r="BG60">
-        <v>0.588</v>
+        <v>0.611</v>
       </c>
     </row>
     <row r="61" spans="1:59">
@@ -8710,7 +8710,7 @@
         <v>66.59999999999999</v>
       </c>
       <c r="BG61">
-        <v>0.463</v>
+        <v>0.485</v>
       </c>
     </row>
     <row r="62" spans="1:59">
@@ -8929,7 +8929,7 @@
         <v>67.44</v>
       </c>
       <c r="BG64">
-        <v>0.741</v>
+        <v>0.743</v>
       </c>
     </row>
     <row r="65" spans="1:59">
@@ -9087,7 +9087,7 @@
         <v>81.91</v>
       </c>
       <c r="BG65">
-        <v>0.92</v>
+        <v>0.9379999999999999</v>
       </c>
     </row>
     <row r="66" spans="1:59">
@@ -9340,7 +9340,7 @@
         <v>66.47</v>
       </c>
       <c r="BG67">
-        <v>0.702</v>
+        <v>0.703</v>
       </c>
     </row>
     <row r="68" spans="1:59">
@@ -9438,7 +9438,7 @@
         <v>62.05</v>
       </c>
       <c r="BG68">
-        <v>0.46</v>
+        <v>0.496</v>
       </c>
     </row>
     <row r="69" spans="1:59">
@@ -9533,7 +9533,7 @@
         <v>73.77</v>
       </c>
       <c r="BG69">
-        <v>0.78</v>
+        <v>0.8120000000000001</v>
       </c>
     </row>
     <row r="70" spans="1:59">
@@ -9685,7 +9685,7 @@
         <v>81.33</v>
       </c>
       <c r="BG70">
-        <v>0.9360000000000001</v>
+        <v>0.947</v>
       </c>
     </row>
     <row r="71" spans="1:59">
@@ -9810,7 +9810,7 @@
         <v>64.06999999999999</v>
       </c>
       <c r="BG71">
-        <v>0.592</v>
+        <v>0.611</v>
       </c>
     </row>
     <row r="72" spans="1:59">
@@ -9965,7 +9965,7 @@
         <v>82.23999999999999</v>
       </c>
       <c r="BG72">
-        <v>0.87</v>
+        <v>0.888</v>
       </c>
     </row>
     <row r="73" spans="1:59">
@@ -10048,7 +10048,7 @@
         <v>72.40000000000001</v>
       </c>
       <c r="BG73">
-        <v>0.772</v>
+        <v>0.779</v>
       </c>
     </row>
     <row r="74" spans="1:59">
@@ -10167,7 +10167,7 @@
         <v>74.3</v>
       </c>
       <c r="BG74">
-        <v>0.65</v>
+        <v>0.663</v>
       </c>
     </row>
     <row r="75" spans="1:59">
@@ -10259,7 +10259,7 @@
         <v>61.6</v>
       </c>
       <c r="BG75">
-        <v>0.459</v>
+        <v>0.477</v>
       </c>
     </row>
     <row r="76" spans="1:59">
@@ -10345,7 +10345,7 @@
         <v>58.32</v>
       </c>
       <c r="BG76">
-        <v>0.455</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="77" spans="1:59">
@@ -10434,7 +10434,7 @@
         <v>69.91</v>
       </c>
       <c r="BG77">
-        <v>0.654</v>
+        <v>0.6820000000000001</v>
       </c>
     </row>
     <row r="78" spans="1:59">
@@ -10532,7 +10532,7 @@
         <v>64</v>
       </c>
       <c r="BG78">
-        <v>0.498</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="79" spans="1:59">
@@ -10627,7 +10627,7 @@
         <v>75.27</v>
       </c>
       <c r="BG79">
-        <v>0.617</v>
+        <v>0.634</v>
       </c>
     </row>
     <row r="80" spans="1:59">
@@ -10680,7 +10680,7 @@
         <v>84.86</v>
       </c>
       <c r="BG80">
-        <v>0.9330000000000001</v>
+        <v>0.949</v>
       </c>
     </row>
     <row r="81" spans="1:59">
@@ -10835,7 +10835,7 @@
         <v>76.88</v>
       </c>
       <c r="BG81">
-        <v>0.838</v>
+        <v>0.854</v>
       </c>
     </row>
     <row r="82" spans="1:59">
@@ -10987,7 +10987,7 @@
         <v>82.98999999999999</v>
       </c>
       <c r="BG82">
-        <v>0.9350000000000001</v>
+        <v>0.949</v>
       </c>
     </row>
     <row r="83" spans="1:59">
@@ -11124,7 +11124,7 @@
         <v>69.66</v>
       </c>
       <c r="BG83">
-        <v>0.64</v>
+        <v>0.645</v>
       </c>
     </row>
     <row r="84" spans="1:59">
@@ -11276,7 +11276,7 @@
         <v>71.72</v>
       </c>
       <c r="BG84">
-        <v>0.694</v>
+        <v>0.718</v>
       </c>
     </row>
     <row r="85" spans="1:59">
@@ -11424,7 +11424,7 @@
         <v>76.68000000000001</v>
       </c>
       <c r="BG86">
-        <v>0.798</v>
+        <v>0.783</v>
       </c>
     </row>
     <row r="87" spans="1:59">
@@ -11543,7 +11543,7 @@
         <v>70.59999999999999</v>
       </c>
       <c r="BG87">
-        <v>0.6850000000000001</v>
+        <v>0.674</v>
       </c>
     </row>
     <row r="88" spans="1:59">
@@ -11713,7 +11713,7 @@
         <v>82.3</v>
       </c>
       <c r="BG88">
-        <v>0.9379999999999999</v>
+        <v>0.955</v>
       </c>
     </row>
     <row r="89" spans="1:59">
@@ -11886,7 +11886,7 @@
         <v>82.97</v>
       </c>
       <c r="BG89">
-        <v>0.903</v>
+        <v>0.919</v>
       </c>
     </row>
     <row r="90" spans="1:59">
@@ -12053,7 +12053,7 @@
         <v>83.51000000000001</v>
       </c>
       <c r="BG90">
-        <v>0.88</v>
+        <v>0.892</v>
       </c>
     </row>
     <row r="91" spans="1:59">
@@ -12175,7 +12175,7 @@
         <v>74.47</v>
       </c>
       <c r="BG91">
-        <v>0.732</v>
+        <v>0.734</v>
       </c>
     </row>
     <row r="92" spans="1:59">
@@ -12294,7 +12294,7 @@
         <v>84.63</v>
       </c>
       <c r="BG92">
-        <v>0.909</v>
+        <v>0.919</v>
       </c>
     </row>
     <row r="93" spans="1:59">
@@ -12410,7 +12410,7 @@
         <v>74.53</v>
       </c>
       <c r="BG93">
-        <v>0.735</v>
+        <v>0.729</v>
       </c>
     </row>
     <row r="94" spans="1:59">
@@ -12508,7 +12508,7 @@
         <v>73.59999999999999</v>
       </c>
       <c r="BG94">
-        <v>0.8</v>
+        <v>0.825</v>
       </c>
     </row>
     <row r="95" spans="1:59">
@@ -12627,7 +12627,7 @@
         <v>66.7</v>
       </c>
       <c r="BG95">
-        <v>0.59</v>
+        <v>0.601</v>
       </c>
     </row>
     <row r="96" spans="1:59">
@@ -12811,7 +12811,7 @@
         <v>75.48999999999999</v>
       </c>
       <c r="BG97">
-        <v>0.803</v>
+        <v>0.806</v>
       </c>
     </row>
     <row r="98" spans="1:59">
@@ -12909,7 +12909,7 @@
         <v>71.45</v>
       </c>
       <c r="BG98">
-        <v>0.672</v>
+        <v>0.697</v>
       </c>
     </row>
     <row r="99" spans="1:59">
@@ -12995,7 +12995,7 @@
         <v>67.92</v>
       </c>
       <c r="BG99">
-        <v>0.601</v>
+        <v>0.613</v>
       </c>
     </row>
     <row r="100" spans="1:59">
@@ -13162,7 +13162,7 @@
         <v>75.29000000000001</v>
       </c>
       <c r="BG100">
-        <v>0.847</v>
+        <v>0.866</v>
       </c>
     </row>
     <row r="101" spans="1:59">
@@ -13254,7 +13254,7 @@
         <v>78.93000000000001</v>
       </c>
       <c r="BG101">
-        <v>0.757</v>
+        <v>0.744</v>
       </c>
     </row>
     <row r="102" spans="1:59">
@@ -13349,7 +13349,7 @@
         <v>54.33</v>
       </c>
       <c r="BG102">
-        <v>0.52</v>
+        <v>0.527</v>
       </c>
     </row>
     <row r="103" spans="1:59">
@@ -13447,7 +13447,7 @@
         <v>64.09999999999999</v>
       </c>
       <c r="BG103">
-        <v>0.435</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="104" spans="1:59">
@@ -13542,7 +13542,7 @@
         <v>72.91</v>
       </c>
       <c r="BG104">
-        <v>0.706</v>
+        <v>0.724</v>
       </c>
     </row>
     <row r="105" spans="1:59">
@@ -13616,7 +13616,7 @@
         <v>82.48999999999999</v>
       </c>
       <c r="BG105">
-        <v>0.916</v>
+        <v>0.919</v>
       </c>
     </row>
     <row r="106" spans="1:59">
@@ -13783,7 +13783,7 @@
         <v>75.93000000000001</v>
       </c>
       <c r="BG106">
-        <v>0.858</v>
+        <v>0.882</v>
       </c>
     </row>
     <row r="107" spans="1:59">
@@ -13944,7 +13944,7 @@
         <v>82.25</v>
       </c>
       <c r="BG107">
-        <v>0.904</v>
+        <v>0.916</v>
       </c>
     </row>
     <row r="108" spans="1:59">
@@ -14057,7 +14057,7 @@
         <v>67.04000000000001</v>
       </c>
       <c r="BG108">
-        <v>0.519</v>
+        <v>0.528</v>
       </c>
     </row>
     <row r="109" spans="1:59">
@@ -14176,7 +14176,7 @@
         <v>64.26000000000001</v>
       </c>
       <c r="BG109">
-        <v>0.477</v>
+        <v>0.483</v>
       </c>
     </row>
     <row r="110" spans="1:59">
@@ -14298,7 +14298,7 @@
         <v>76.16</v>
       </c>
       <c r="BG110">
-        <v>0.802</v>
+        <v>0.8100000000000001</v>
       </c>
     </row>
     <row r="111" spans="1:59">
@@ -14429,7 +14429,7 @@
         <v>78.92</v>
       </c>
       <c r="BG111">
-        <v>0.717</v>
+        <v>0.74</v>
       </c>
     </row>
     <row r="112" spans="1:59">
@@ -14524,7 +14524,7 @@
         <v>59.31</v>
       </c>
       <c r="BG112">
-        <v>0.427</v>
+        <v>0.434</v>
       </c>
     </row>
     <row r="113" spans="1:59">
@@ -14652,7 +14652,7 @@
         <v>82.53</v>
       </c>
       <c r="BG113">
-        <v>0.878</v>
+        <v>0.895</v>
       </c>
     </row>
     <row r="114" spans="1:59">
@@ -14717,7 +14717,7 @@
         <v>73.7</v>
       </c>
       <c r="BG114">
-        <v>0.708</v>
+        <v>0.704</v>
       </c>
     </row>
     <row r="115" spans="1:59">
@@ -14827,7 +14827,7 @@
         <v>64.92</v>
       </c>
       <c r="BG115">
-        <v>0.52</v>
+        <v>0.546</v>
       </c>
     </row>
     <row r="116" spans="1:59">
@@ -14922,7 +14922,7 @@
         <v>74.98999999999999</v>
       </c>
       <c r="BG116">
-        <v>0.79</v>
+        <v>0.804</v>
       </c>
     </row>
     <row r="117" spans="1:59">
@@ -15074,7 +15074,7 @@
         <v>75.05</v>
       </c>
       <c r="BG117">
-        <v>0.774</v>
+        <v>0.779</v>
       </c>
     </row>
     <row r="118" spans="1:59">
@@ -15145,7 +15145,7 @@
         <v>67.88</v>
       </c>
       <c r="BG118">
-        <v>0.627</v>
+        <v>0.62</v>
       </c>
     </row>
     <row r="119" spans="1:59">
@@ -15243,7 +15243,7 @@
         <v>71.90000000000001</v>
       </c>
       <c r="BG119">
-        <v>0.7</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="120" spans="1:59">
@@ -15436,7 +15436,7 @@
         <v>69.87</v>
       </c>
       <c r="BG121">
-        <v>0.741</v>
+        <v>0.737</v>
       </c>
     </row>
     <row r="122" spans="1:59">
@@ -15528,7 +15528,7 @@
         <v>76.88</v>
       </c>
       <c r="BG122">
-        <v>0.8139999999999999</v>
+        <v>0.829</v>
       </c>
     </row>
     <row r="123" spans="1:59">
@@ -15665,7 +15665,7 @@
         <v>76.68000000000001</v>
       </c>
       <c r="BG123">
-        <v>0.667</v>
+        <v>0.6860000000000001</v>
       </c>
     </row>
     <row r="124" spans="1:59">
@@ -15790,7 +15790,7 @@
         <v>60.85</v>
       </c>
       <c r="BG124">
-        <v>0.437</v>
+        <v>0.456</v>
       </c>
     </row>
     <row r="125" spans="1:59">
@@ -15930,7 +15930,7 @@
         <v>67.13</v>
       </c>
       <c r="BG125">
-        <v>0.578</v>
+        <v>0.583</v>
       </c>
     </row>
     <row r="126" spans="1:59">
@@ -16052,7 +16052,7 @@
         <v>63.71</v>
       </c>
       <c r="BG126">
-        <v>0.647</v>
+        <v>0.646</v>
       </c>
     </row>
     <row r="127" spans="1:59">
@@ -16189,7 +16189,7 @@
         <v>70.78</v>
       </c>
       <c r="BG127">
-        <v>0.574</v>
+        <v>0.602</v>
       </c>
     </row>
     <row r="128" spans="1:59">
@@ -16341,7 +16341,7 @@
         <v>82.28</v>
       </c>
       <c r="BG128">
-        <v>0.931</v>
+        <v>0.944</v>
       </c>
     </row>
     <row r="129" spans="1:59">
@@ -16460,7 +16460,7 @@
         <v>82.29000000000001</v>
       </c>
       <c r="BG129">
-        <v>0.917</v>
+        <v>0.931</v>
       </c>
     </row>
     <row r="130" spans="1:59">
@@ -16549,7 +16549,7 @@
         <v>74.48</v>
       </c>
       <c r="BG130">
-        <v>0.658</v>
+        <v>0.66</v>
       </c>
     </row>
     <row r="131" spans="1:59">
@@ -16647,7 +16647,7 @@
         <v>62.42</v>
       </c>
       <c r="BG131">
-        <v>0.354</v>
+        <v>0.394</v>
       </c>
     </row>
     <row r="132" spans="1:59">
@@ -16760,7 +16760,7 @@
         <v>54.69</v>
       </c>
       <c r="BG132">
-        <v>0.532</v>
+        <v>0.539</v>
       </c>
     </row>
     <row r="133" spans="1:59">
@@ -16917,7 +16917,7 @@
         <v>75.8</v>
       </c>
       <c r="BG134">
-        <v>0.757</v>
+        <v>0.774</v>
       </c>
     </row>
     <row r="135" spans="1:59">
@@ -17084,7 +17084,7 @@
         <v>82.40000000000001</v>
       </c>
       <c r="BG135">
-        <v>0.953</v>
+        <v>0.957</v>
       </c>
     </row>
     <row r="136" spans="1:59">
@@ -17247,7 +17247,7 @@
         <v>77.86</v>
       </c>
       <c r="BG137">
-        <v>0.821</v>
+        <v>0.8129999999999999</v>
       </c>
     </row>
     <row r="138" spans="1:59">
@@ -17372,7 +17372,7 @@
         <v>67.27</v>
       </c>
       <c r="BG138">
-        <v>0.5620000000000001</v>
+        <v>0.5570000000000001</v>
       </c>
     </row>
     <row r="139" spans="1:59">
@@ -17479,7 +17479,7 @@
         <v>74.05</v>
       </c>
       <c r="BG139">
-        <v>0.6860000000000001</v>
+        <v>0.708</v>
       </c>
     </row>
     <row r="140" spans="1:59">
@@ -17601,7 +17601,7 @@
         <v>78.51000000000001</v>
       </c>
       <c r="BG140">
-        <v>0.789</v>
+        <v>0.8149999999999999</v>
       </c>
     </row>
     <row r="141" spans="1:59">
@@ -17690,7 +17690,7 @@
         <v>64.5</v>
       </c>
       <c r="BG141">
-        <v>0.544</v>
+        <v>0.555</v>
       </c>
     </row>
     <row r="142" spans="1:59">
@@ -17815,7 +17815,7 @@
         <v>74.25</v>
       </c>
       <c r="BG142">
-        <v>0.702</v>
+        <v>0.728</v>
       </c>
     </row>
     <row r="143" spans="1:59">
@@ -17907,7 +17907,7 @@
         <v>76.73999999999999</v>
       </c>
       <c r="BG143">
-        <v>0.75</v>
+        <v>0.777</v>
       </c>
     </row>
     <row r="144" spans="1:59">
@@ -18029,7 +18029,7 @@
         <v>71.23</v>
       </c>
       <c r="BG144">
-        <v>0.699</v>
+        <v>0.718</v>
       </c>
     </row>
     <row r="145" spans="1:59">
@@ -18187,7 +18187,7 @@
         <v>78.73</v>
       </c>
       <c r="BG145">
-        <v>0.865</v>
+        <v>0.88</v>
       </c>
     </row>
     <row r="146" spans="1:59">
@@ -18354,7 +18354,7 @@
         <v>82.05</v>
       </c>
       <c r="BG146">
-        <v>0.847</v>
+        <v>0.864</v>
       </c>
     </row>
     <row r="147" spans="1:59">
@@ -18473,7 +18473,7 @@
         <v>80.23</v>
       </c>
       <c r="BG147">
-        <v>0.856</v>
+        <v>0.848</v>
       </c>
     </row>
     <row r="148" spans="1:59">
@@ -18634,7 +18634,7 @@
         <v>76.05</v>
       </c>
       <c r="BG148">
-        <v>0.8110000000000001</v>
+        <v>0.828</v>
       </c>
     </row>
     <row r="149" spans="1:59">
@@ -18756,7 +18756,7 @@
         <v>72.58</v>
       </c>
       <c r="BG149">
-        <v>0.8159999999999999</v>
+        <v>0.824</v>
       </c>
     </row>
     <row r="150" spans="1:59">
@@ -18878,7 +18878,7 @@
         <v>69.02</v>
       </c>
       <c r="BG150">
-        <v>0.524</v>
+        <v>0.543</v>
       </c>
     </row>
     <row r="151" spans="1:59">
@@ -18937,7 +18937,7 @@
         <v>76.23</v>
       </c>
       <c r="BG151">
-        <v>0.778</v>
+        <v>0.779</v>
       </c>
     </row>
     <row r="152" spans="1:59">
@@ -19023,7 +19023,7 @@
         <v>76.2</v>
       </c>
       <c r="BG152">
-        <v>0.747</v>
+        <v>0.759</v>
       </c>
     </row>
     <row r="153" spans="1:59">
@@ -19106,7 +19106,7 @@
         <v>72.53</v>
       </c>
       <c r="BG153">
-        <v>0.723</v>
+        <v>0.738</v>
       </c>
     </row>
     <row r="154" spans="1:59">
@@ -19180,7 +19180,7 @@
         <v>73.31999999999999</v>
       </c>
       <c r="BG154">
-        <v>0.713</v>
+        <v>0.715</v>
       </c>
     </row>
     <row r="155" spans="1:59">
@@ -19340,7 +19340,7 @@
         <v>70.39</v>
       </c>
       <c r="BG156">
-        <v>0.589</v>
+        <v>0.625</v>
       </c>
     </row>
     <row r="157" spans="1:59">
@@ -19471,7 +19471,7 @@
         <v>75.13</v>
       </c>
       <c r="BG157">
-        <v>0.853</v>
+        <v>0.854</v>
       </c>
     </row>
     <row r="158" spans="1:59">
@@ -19593,7 +19593,7 @@
         <v>67.94</v>
       </c>
       <c r="BG158">
-        <v>0.505</v>
+        <v>0.512</v>
       </c>
     </row>
     <row r="159" spans="1:59">
@@ -19727,7 +19727,7 @@
         <v>76</v>
       </c>
       <c r="BG159">
-        <v>0.787</v>
+        <v>0.806</v>
       </c>
     </row>
     <row r="160" spans="1:59">
@@ -19849,7 +19849,7 @@
         <v>73.40000000000001</v>
       </c>
       <c r="BG160">
-        <v>0.797</v>
+        <v>0.796</v>
       </c>
     </row>
     <row r="161" spans="1:59">
@@ -19944,7 +19944,7 @@
         <v>54.7</v>
       </c>
       <c r="BG161">
-        <v>0.419</v>
+        <v>0.452</v>
       </c>
     </row>
     <row r="162" spans="1:59">
@@ -20081,7 +20081,7 @@
         <v>83.62</v>
       </c>
       <c r="BG162">
-        <v>0.9320000000000001</v>
+        <v>0.9379999999999999</v>
       </c>
     </row>
     <row r="163" spans="1:59">
@@ -20236,7 +20236,7 @@
         <v>77.54000000000001</v>
       </c>
       <c r="BG163">
-        <v>0.855</v>
+        <v>0.86</v>
       </c>
     </row>
     <row r="164" spans="1:59">
@@ -20406,7 +20406,7 @@
         <v>81.31999999999999</v>
       </c>
       <c r="BG164">
-        <v>0.896</v>
+        <v>0.917</v>
       </c>
     </row>
     <row r="165" spans="1:59">
@@ -20486,7 +20486,7 @@
         <v>73</v>
       </c>
       <c r="BG165">
-        <v>0.546</v>
+        <v>0.5669999999999999</v>
       </c>
     </row>
     <row r="166" spans="1:59">
@@ -20694,7 +20694,7 @@
         <v>64.13</v>
       </c>
       <c r="BG167">
-        <v>0.699</v>
+        <v>0.709</v>
       </c>
     </row>
     <row r="168" spans="1:59">
@@ -20860,7 +20860,7 @@
         <v>83.03</v>
       </c>
       <c r="BG169">
-        <v>0.903</v>
+        <v>0.916</v>
       </c>
     </row>
     <row r="170" spans="1:59">
@@ -20961,7 +20961,7 @@
         <v>57.85</v>
       </c>
       <c r="BG170">
-        <v>0.388</v>
+        <v>0.433</v>
       </c>
     </row>
     <row r="171" spans="1:59">
@@ -21128,7 +21128,7 @@
         <v>83.56</v>
       </c>
       <c r="BG171">
-        <v>0.891</v>
+        <v>0.904</v>
       </c>
     </row>
     <row r="172" spans="1:59">
@@ -21265,7 +21265,7 @@
         <v>76.98</v>
       </c>
       <c r="BG172">
-        <v>0.77</v>
+        <v>0.782</v>
       </c>
     </row>
     <row r="173" spans="1:59">
@@ -21354,7 +21354,7 @@
         <v>65.31</v>
       </c>
       <c r="BG173">
-        <v>0.502</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="174" spans="1:59">
@@ -21449,7 +21449,7 @@
         <v>71.68000000000001</v>
       </c>
       <c r="BG174">
-        <v>0.72</v>
+        <v>0.738</v>
       </c>
     </row>
     <row r="175" spans="1:59">
@@ -21610,7 +21610,7 @@
         <v>82.8</v>
       </c>
       <c r="BG175">
-        <v>0.9330000000000001</v>
+        <v>0.945</v>
       </c>
     </row>
     <row r="176" spans="1:59">
@@ -21741,7 +21741,7 @@
         <v>83.78</v>
       </c>
       <c r="BG176">
-        <v>0.944</v>
+        <v>0.955</v>
       </c>
     </row>
     <row r="177" spans="1:59">
@@ -21818,7 +21818,7 @@
         <v>72.7</v>
       </c>
       <c r="BG177">
-        <v>0.536</v>
+        <v>0.5669999999999999</v>
       </c>
     </row>
     <row r="178" spans="1:59">
@@ -22005,7 +22005,7 @@
         <v>71.09999999999999</v>
       </c>
       <c r="BG179">
-        <v>0.65</v>
+        <v>0.668</v>
       </c>
     </row>
     <row r="180" spans="1:59">
@@ -22103,7 +22103,7 @@
         <v>65.45999999999999</v>
       </c>
       <c r="BG180">
-        <v>0.538</v>
+        <v>0.529</v>
       </c>
     </row>
     <row r="181" spans="1:59">
@@ -22228,7 +22228,7 @@
         <v>77.15000000000001</v>
       </c>
       <c r="BG181">
-        <v>0.755</v>
+        <v>0.777</v>
       </c>
     </row>
     <row r="182" spans="1:59">
@@ -22314,7 +22314,7 @@
         <v>69.5</v>
       </c>
       <c r="BG182">
-        <v>0.625</v>
+        <v>0.606</v>
       </c>
     </row>
     <row r="183" spans="1:59">
@@ -22439,7 +22439,7 @@
         <v>61.04</v>
       </c>
       <c r="BG183">
-        <v>0.503</v>
+        <v>0.515</v>
       </c>
     </row>
     <row r="184" spans="1:59">
@@ -22555,7 +22555,7 @@
         <v>73.51000000000001</v>
       </c>
       <c r="BG184">
-        <v>0.784</v>
+        <v>0.796</v>
       </c>
     </row>
     <row r="185" spans="1:59">
@@ -22650,7 +22650,7 @@
         <v>76.7</v>
       </c>
       <c r="BG185">
-        <v>0.735</v>
+        <v>0.74</v>
       </c>
     </row>
     <row r="186" spans="1:59">
@@ -22787,7 +22787,7 @@
         <v>77.69</v>
       </c>
       <c r="BG186">
-        <v>0.791</v>
+        <v>0.82</v>
       </c>
     </row>
     <row r="187" spans="1:59">
@@ -22912,7 +22912,7 @@
         <v>63.37</v>
       </c>
       <c r="BG187">
-        <v>0.516</v>
+        <v>0.544</v>
       </c>
     </row>
     <row r="188" spans="1:59">
@@ -23034,7 +23034,7 @@
         <v>72.06</v>
       </c>
       <c r="BG188">
-        <v>0.751</v>
+        <v>0.779</v>
       </c>
     </row>
     <row r="189" spans="1:59">
@@ -23168,7 +23168,7 @@
         <v>77.97</v>
       </c>
       <c r="BG189">
-        <v>0.863</v>
+        <v>0.89</v>
       </c>
     </row>
     <row r="190" spans="1:59">
@@ -23335,7 +23335,7 @@
         <v>81.31999999999999</v>
       </c>
       <c r="BG190">
-        <v>0.922</v>
+        <v>0.9320000000000001</v>
       </c>
     </row>
     <row r="191" spans="1:59">
@@ -23502,7 +23502,7 @@
         <v>78.86</v>
       </c>
       <c r="BG191">
-        <v>0.924</v>
+        <v>0.926</v>
       </c>
     </row>
     <row r="192" spans="1:59">
@@ -23624,7 +23624,7 @@
         <v>77.91</v>
       </c>
       <c r="BG192">
-        <v>0.804</v>
+        <v>0.8169999999999999</v>
       </c>
     </row>
     <row r="193" spans="1:59">
@@ -23716,7 +23716,7 @@
         <v>71.72</v>
       </c>
       <c r="BG193">
-        <v>0.71</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="194" spans="1:59">
@@ -23799,7 +23799,7 @@
         <v>70.47</v>
       </c>
       <c r="BG194">
-        <v>0.603</v>
+        <v>0.609</v>
       </c>
     </row>
     <row r="195" spans="1:59">
@@ -23929,7 +23929,7 @@
         <v>72.06</v>
       </c>
       <c r="BG196">
-        <v>0.761</v>
+        <v>0.711</v>
       </c>
     </row>
     <row r="197" spans="1:59">
@@ -24027,7 +24027,7 @@
         <v>75.40000000000001</v>
       </c>
       <c r="BG197">
-        <v>0.694</v>
+        <v>0.704</v>
       </c>
     </row>
     <row r="198" spans="1:59">
@@ -24145,6 +24145,9 @@
       <c r="BF198">
         <v>72.58</v>
       </c>
+      <c r="BG198">
+        <v>0.737</v>
+      </c>
     </row>
     <row r="199" spans="1:59">
       <c r="A199" t="s">
@@ -24241,7 +24244,7 @@
         <v>66.12</v>
       </c>
       <c r="BG199">
-        <v>0.452</v>
+        <v>0.47</v>
       </c>
     </row>
     <row r="200" spans="1:59">
@@ -24366,7 +24369,7 @@
         <v>63.89</v>
       </c>
       <c r="BG200">
-        <v>0.588</v>
+        <v>0.584</v>
       </c>
     </row>
     <row r="201" spans="1:59">
@@ -24491,7 +24494,7 @@
         <v>61.49</v>
       </c>
       <c r="BG201">
-        <v>0.535</v>
+        <v>0.571</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refresh vaccination data with continents
</commit_message>
<xml_diff>
--- a/public/data/latest/owid-covid-latest.xlsx
+++ b/public/data/latest/owid-covid-latest.xlsx
@@ -2155,6 +2155,33 @@
       <c r="P3">
         <v>0.215</v>
       </c>
+      <c r="AI3">
+        <v>7296864</v>
+      </c>
+      <c r="AJ3">
+        <v>5232410</v>
+      </c>
+      <c r="AK3">
+        <v>2145318</v>
+      </c>
+      <c r="AL3">
+        <v>218289</v>
+      </c>
+      <c r="AM3">
+        <v>259345</v>
+      </c>
+      <c r="AN3">
+        <v>0.54</v>
+      </c>
+      <c r="AO3">
+        <v>0.39</v>
+      </c>
+      <c r="AP3">
+        <v>0.16</v>
+      </c>
+      <c r="AQ3">
+        <v>193</v>
+      </c>
       <c r="AS3">
         <v>1340598113</v>
       </c>
@@ -3085,6 +3112,33 @@
       <c r="P12">
         <v>0.181</v>
       </c>
+      <c r="AI12">
+        <v>148060742</v>
+      </c>
+      <c r="AJ12">
+        <v>58806626</v>
+      </c>
+      <c r="AK12">
+        <v>18842574</v>
+      </c>
+      <c r="AL12">
+        <v>3752559</v>
+      </c>
+      <c r="AM12">
+        <v>4410146</v>
+      </c>
+      <c r="AN12">
+        <v>3.19</v>
+      </c>
+      <c r="AO12">
+        <v>1.27</v>
+      </c>
+      <c r="AP12">
+        <v>0.41</v>
+      </c>
+      <c r="AQ12">
+        <v>950</v>
+      </c>
       <c r="AS12">
         <v>4639847425</v>
       </c>
@@ -9485,6 +9539,33 @@
       <c r="P65">
         <v>4.135</v>
       </c>
+      <c r="AI65">
+        <v>90952985</v>
+      </c>
+      <c r="AJ65">
+        <v>69886655</v>
+      </c>
+      <c r="AK65">
+        <v>21045647</v>
+      </c>
+      <c r="AL65">
+        <v>702510</v>
+      </c>
+      <c r="AM65">
+        <v>1739799</v>
+      </c>
+      <c r="AN65">
+        <v>12.15</v>
+      </c>
+      <c r="AO65">
+        <v>9.33</v>
+      </c>
+      <c r="AP65">
+        <v>2.81</v>
+      </c>
+      <c r="AQ65">
+        <v>2324</v>
+      </c>
       <c r="AS65">
         <v>748680069</v>
       </c>
@@ -18434,6 +18515,33 @@
       <c r="P143">
         <v>3.13</v>
       </c>
+      <c r="AI143">
+        <v>119995334</v>
+      </c>
+      <c r="AJ143">
+        <v>79685572</v>
+      </c>
+      <c r="AK143">
+        <v>40339714</v>
+      </c>
+      <c r="AL143">
+        <v>1910596</v>
+      </c>
+      <c r="AM143">
+        <v>2801081</v>
+      </c>
+      <c r="AN143">
+        <v>20.27</v>
+      </c>
+      <c r="AO143">
+        <v>13.46</v>
+      </c>
+      <c r="AP143">
+        <v>6.81</v>
+      </c>
+      <c r="AQ143">
+        <v>4731</v>
+      </c>
       <c r="AS143">
         <v>592072204</v>
       </c>
@@ -18770,6 +18878,27 @@
       <c r="P146">
         <v>0.033</v>
       </c>
+      <c r="AI146">
+        <v>200437</v>
+      </c>
+      <c r="AJ146">
+        <v>177294</v>
+      </c>
+      <c r="AL146">
+        <v>17656</v>
+      </c>
+      <c r="AM146">
+        <v>13728</v>
+      </c>
+      <c r="AN146">
+        <v>0.47</v>
+      </c>
+      <c r="AO146">
+        <v>0.42</v>
+      </c>
+      <c r="AQ146">
+        <v>322</v>
+      </c>
       <c r="AS146">
         <v>42677809</v>
       </c>
@@ -22712,6 +22841,33 @@
       </c>
       <c r="P178">
         <v>5.801</v>
+      </c>
+      <c r="AI178">
+        <v>23808009</v>
+      </c>
+      <c r="AJ178">
+        <v>17854028</v>
+      </c>
+      <c r="AK178">
+        <v>5953981</v>
+      </c>
+      <c r="AL178">
+        <v>519506</v>
+      </c>
+      <c r="AM178">
+        <v>783970</v>
+      </c>
+      <c r="AN178">
+        <v>5.53</v>
+      </c>
+      <c r="AO178">
+        <v>4.14</v>
+      </c>
+      <c r="AP178">
+        <v>1.38</v>
+      </c>
+      <c r="AQ178">
+        <v>1820</v>
       </c>
       <c r="AS178">
         <v>430759772</v>

</xml_diff>